<commit_message>
Android Security Requiments V1 - col H translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Информация" sheetId="1" state="visible" r:id="rId2"/>
@@ -1915,7 +1915,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="158">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2200,256 +2200,260 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="18" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="21" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="25" fillId="8" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="8" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="8" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="22" fillId="9" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="8" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="21" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="22" fillId="7" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="22" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="22" fillId="7" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="8" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="5" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="18" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="21" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="25" fillId="8" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="8" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="8" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="22" fillId="9" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="8" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="21" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="22" fillId="7" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="22" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="22" fillId="7" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="8" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="5" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -2721,7 +2725,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2761,8 +2765,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.717177360436632"/>
-          <c:y val="0.0138929943836831"/>
+          <c:x val="0.717146540610228"/>
+          <c:y val="0.0138940211366492"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2780,10 +2784,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.221453435901844"/>
-          <c:y val="0.112621933195389"/>
-          <c:w val="0.502471098886931"/>
-          <c:h val="0.840821755838014"/>
+          <c:x val="0.221443919209282"/>
+          <c:y val="0.112630256448156"/>
+          <c:w val="0.502449505801461"/>
+          <c:h val="0.840736087502771"/>
         </c:manualLayout>
       </c:layout>
       <c:radarChart>
@@ -2901,13 +2905,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="68782684"/>
-        <c:axId val="15130499"/>
+        <c:axId val="52591096"/>
+        <c:axId val="82544757"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="68782684"/>
+        <c:axId val="52591096"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2945,7 +2949,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15130499"/>
+        <c:crossAx val="82544757"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2953,7 +2957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15130499"/>
+        <c:axId val="82544757"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2996,7 +3000,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68782684"/>
+        <c:crossAx val="52591096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3056,7 +3060,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3096,8 +3100,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.648894274462284"/>
-          <c:y val="0.0247331615752668"/>
+          <c:x val="0.648866193526052"/>
+          <c:y val="0.0247349823321555"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3115,10 +3119,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.221448046046652"/>
-          <c:y val="0.112624217887376"/>
-          <c:w val="0.502445146492405"/>
-          <c:h val="0.840853882959146"/>
+          <c:x val="0.221438462870002"/>
+          <c:y val="0.112632508833922"/>
+          <c:w val="0.502423403150424"/>
+          <c:h val="0.840768551236749"/>
         </c:manualLayout>
       </c:layout>
       <c:radarChart>
@@ -3236,13 +3240,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50635670"/>
-        <c:axId val="53673754"/>
+        <c:axId val="15287082"/>
+        <c:axId val="46074959"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="50635670"/>
+        <c:axId val="15287082"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3280,7 +3284,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53673754"/>
+        <c:crossAx val="46074959"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3288,7 +3292,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53673754"/>
+        <c:axId val="46074959"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3331,7 +3335,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50635670"/>
+        <c:crossAx val="15287082"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3402,9 +3406,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>6612840</xdr:colOff>
+      <xdr:colOff>6612480</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>41400</xdr:rowOff>
+      <xdr:rowOff>41040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3417,8 +3421,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8134200" y="221040"/>
-          <a:ext cx="669240" cy="713520"/>
+          <a:off x="8133480" y="221040"/>
+          <a:ext cx="668880" cy="713160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3444,9 +3448,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>77040</xdr:colOff>
+      <xdr:colOff>76680</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>66600</xdr:rowOff>
+      <xdr:rowOff>66240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3455,7 +3459,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="413280" y="3249720"/>
-        <a:ext cx="8376480" cy="4871160"/>
+        <a:ext cx="8376840" cy="4870800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3474,9 +3478,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>149400</xdr:colOff>
+      <xdr:colOff>149040</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>96120</xdr:rowOff>
+      <xdr:rowOff>95760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3484,8 +3488,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10932480" y="3260160"/>
-        <a:ext cx="8318160" cy="4890240"/>
+        <a:off x="10933200" y="3260160"/>
+        <a:ext cx="8318520" cy="4889880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3509,7 +3513,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.2"/>
@@ -3581,8 +3585,8 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="9" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( "https://github.com/OWASP/owasp-masvs/blob/", MASVS_VERSION, "/Document-ru/"))</f>
-        <v>https://github.com/OWASP/owasp-masvs/blob/1.1.4/Document-ru/</v>
+        <f aca="false">HYPERLINK(CONCATENATE( "https://github.com/OWASP/owasp-masvs/blob/", MASVS_VERSION, "/Document/"))</f>
+        <v>https://github.com/OWASP/owasp-masvs/blob/1.1.4/Document/</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3600,8 +3604,8 @@
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="12" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( "https://github.com/OWASP/owasp-mstg/blob/", MSTG_VERSION, "/Document-ru/"))</f>
-        <v>https://github.com/OWASP/owasp-mstg/blob/1.1.3/Document-ru/</v>
+        <f aca="false">HYPERLINK(CONCATENATE( "https://github.com/OWASP/owasp-mstg/blob/", MSTG_VERSION, "/Document/"))</f>
+        <v>https://github.com/OWASP/owasp-mstg/blob/1.1.3/Document/</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="31.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3908,7 +3912,7 @@
   </sheetPr>
   <dimension ref="B1:X50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -3922,9 +3926,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="25" width="5.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="25" width="10.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="25" width="8.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="25" width="10.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="25" width="10.99"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="10" style="25" width="8.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="25" width="10.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="25" width="10.99"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="25" style="25" width="8.8"/>
   </cols>
   <sheetData>
@@ -4520,8 +4524,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B64" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B77" activeCellId="0" sqref="B77"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4630,8 +4634,8 @@
       </c>
       <c r="G5" s="70"/>
       <c r="H5" s="71" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#architectural-information"), "Architectural Information")</f>
-        <v>Architectural Information</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#architectural-information"), "Информация об архитектуре")</f>
+        <v>Информация об архитектуре</v>
       </c>
       <c r="I5" s="71" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x05h-Testing-Platform-Interaction.md#testing-for-insecure-configuration-of-instant-apps-mstg-arch-1-mstg-arch-7"), "Testing for insecure Configuration of Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)")</f>
@@ -4658,8 +4662,8 @@
       </c>
       <c r="G6" s="70"/>
       <c r="H6" s="74" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"), "Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
-        <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"), "Ошибка инъекции (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
+        <v>Ошибка инъекции (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
       <c r="I6" s="75" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
@@ -4686,8 +4690,8 @@
       </c>
       <c r="G7" s="70"/>
       <c r="H7" s="71" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#architectural-information"), "Architectural Information")</f>
-        <v>Architectural Information</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#architectural-information"), "Информация об архитектуре")</f>
+        <v>Информация об архитектуре</v>
       </c>
       <c r="I7" s="76"/>
       <c r="J7" s="76"/>
@@ -4711,8 +4715,8 @@
       </c>
       <c r="G8" s="70"/>
       <c r="H8" s="71" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#identifying-sensitive-data"), "Identifying Sensitive Data")</f>
-        <v>Identifying Sensitive Data</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#identifying-sensitive-data"), "Выявление конфиденциальных данных")</f>
+        <v>Выявление конфиденциальных данных</v>
       </c>
       <c r="I8" s="76"/>
       <c r="J8" s="76"/>
@@ -4736,8 +4740,8 @@
         <v>77</v>
       </c>
       <c r="H9" s="71" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#environmental-information"), "Environmental Information")</f>
-        <v>Environmental Information</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#environmental-information"), "Информация об окружении")</f>
+        <v>Информация об окружении</v>
       </c>
       <c r="I9" s="76"/>
       <c r="J9" s="76"/>
@@ -4761,8 +4765,8 @@
         <v>77</v>
       </c>
       <c r="H10" s="71" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#mapping-the-application"), "Mapping the Application")</f>
-        <v>Mapping the Application</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#mapping-the-application"), "Составление карты приложения")</f>
+        <v>Составление карты приложения</v>
       </c>
       <c r="I10" s="76"/>
       <c r="J10" s="76"/>
@@ -4786,8 +4790,8 @@
         <v>77</v>
       </c>
       <c r="H11" s="71" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-for-insecure-configuration-of-instant-apps-mstg-arch-1-mstg-arch-7"),"Testing for insecure Configuration of Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)")</f>
-        <v>Testing for insecure Configuration of Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-for-insecure-configuration-of-instant-apps-mstg-arch-1-mstg-arch-7"),"Тестирование на небезопасную конфигурацию Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)")</f>
+        <v>Тестирование на небезопасную конфигурацию Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)</v>
       </c>
       <c r="I11" s="75" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#principles-of-testing"), "Principles of Testing")</f>
@@ -4817,8 +4821,8 @@
         <v>77</v>
       </c>
       <c r="H12" s="71" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04g-Testing-Cryptography.md#cryptographic-policy"), "Cryptographic policy")</f>
-        <v>Cryptographic policy</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04g-Testing-Cryptography.md#cryptographic-policy"), "Криптографическая политика")</f>
+        <v>Криптографическая политика</v>
       </c>
       <c r="I12" s="76"/>
       <c r="J12" s="76"/>
@@ -4842,8 +4846,8 @@
         <v>77</v>
       </c>
       <c r="H13" s="71" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x05h-Testing-Platform-Interaction.md#testing-enforced-updating-mstg-arch-9"), "Testing enforced updating (MSTG-ARCH-9)")</f>
-        <v>Testing enforced updating (MSTG-ARCH-9)</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x05h-Testing-Platform-Interaction.md#testing-enforced-updating-mstg-arch-9"), "Тест принудительного обновления (MSTG-ARCH-9)")</f>
+        <v>Тест принудительного обновления (MSTG-ARCH-9)</v>
       </c>
       <c r="I13" s="76"/>
       <c r="J13" s="76"/>
@@ -4867,8 +4871,8 @@
         <v>77</v>
       </c>
       <c r="H14" s="71" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#security-testing-and-the-sdlc"), "Security Testing and the SDLC")</f>
-        <v>Security Testing and the SDLC</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#security-testing-and-the-sdlc"), "Тестирование безопасности и SDLC (жизненного цикла разработки ПО)")</f>
+        <v>Тестирование безопасности и SDLC (жизненного цикла разработки ПО)</v>
       </c>
       <c r="I14" s="76"/>
       <c r="J14" s="76"/>
@@ -7006,7 +7010,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="129" width="8"/>
@@ -7107,7 +7111,7 @@
         <v>64</v>
       </c>
       <c r="G5" s="70"/>
-      <c r="H5" s="71" t="str">
+      <c r="H5" s="134" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#architectural-information"), "Architectural Information")</f>
         <v>Architectural Information</v>
       </c>
@@ -7132,7 +7136,7 @@
         <v>64</v>
       </c>
       <c r="G6" s="70"/>
-      <c r="H6" s="71" t="str">
+      <c r="H6" s="134" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"), "Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
         <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
@@ -7140,7 +7144,7 @@
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
         <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
-      <c r="J6" s="134"/>
+      <c r="J6" s="135"/>
       <c r="K6" s="73"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7160,7 +7164,7 @@
         <v>64</v>
       </c>
       <c r="G7" s="70"/>
-      <c r="H7" s="71" t="str">
+      <c r="H7" s="134" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#architectural-information"), "Architectural Information")</f>
         <v>Architectural Information</v>
       </c>
@@ -7185,7 +7189,7 @@
         <v>64</v>
       </c>
       <c r="G8" s="70"/>
-      <c r="H8" s="71" t="str">
+      <c r="H8" s="134" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#identifying-sensitive-data"), "Identifying Sensitive Data")</f>
         <v>Identifying Sensitive Data</v>
       </c>
@@ -7210,7 +7214,7 @@
       <c r="G9" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="71" t="str">
+      <c r="H9" s="134" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#environmental-information"), "Environmental Information")</f>
         <v>Environmental Information</v>
       </c>
@@ -7235,7 +7239,7 @@
       <c r="G10" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="71" t="str">
+      <c r="H10" s="134" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#mapping-the-application"), "Mapping the Application")</f>
         <v>Mapping the Application</v>
       </c>
@@ -7260,7 +7264,7 @@
       <c r="G11" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H11" s="71" t="str">
+      <c r="H11" s="134" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#principles-of-testing"), "Principles of Testing")</f>
         <v>Principles of Testing</v>
       </c>
@@ -7288,7 +7292,7 @@
       <c r="G12" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H12" s="71" t="str">
+      <c r="H12" s="134" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04g-Testing-Cryptography.md#cryptographic-policy"), "Cryptographic policy")</f>
         <v>Cryptographic policy</v>
       </c>
@@ -7313,7 +7317,7 @@
       <c r="G13" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H13" s="71" t="str">
+      <c r="H13" s="134" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x06h-Testing-Platform-Interaction.md#testing-enforced-updating-mstg-arch-9"), "Testing enforced updating (MSTG-ARCH-9)")</f>
         <v>Testing enforced updating (MSTG-ARCH-9)</v>
       </c>
@@ -7338,7 +7342,7 @@
       <c r="G14" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H14" s="71" t="str">
+      <c r="H14" s="134" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#security-testing-and-the-sdlc"), "Security Testing and the SDLC")</f>
         <v>Security Testing and the SDLC</v>
       </c>
@@ -7632,7 +7636,7 @@
       <c r="I26" s="76"/>
       <c r="J26" s="76"/>
       <c r="K26" s="73"/>
-      <c r="L26" s="135"/>
+      <c r="L26" s="136"/>
     </row>
     <row r="27" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="87" t="s">
@@ -7867,7 +7871,7 @@
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
-      <c r="J36" s="136"/>
+      <c r="J36" s="137"/>
       <c r="K36" s="125"/>
     </row>
     <row r="37" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7920,7 +7924,7 @@
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
-      <c r="J38" s="136"/>
+      <c r="J38" s="137"/>
       <c r="K38" s="125"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7996,7 +8000,7 @@
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#dynamic-testing-mstg-auth-6"),"Dynamic Testing (MSTG-AUTH-6)")</f>
         <v>Dynamic Testing (MSTG-AUTH-6)</v>
       </c>
-      <c r="J41" s="136"/>
+      <c r="J41" s="137"/>
       <c r="K41" s="125"/>
     </row>
     <row r="42" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8021,7 +8025,7 @@
         <v>Testing Session Timeout (MSTG-AUTH-7)</v>
       </c>
       <c r="I42" s="97"/>
-      <c r="J42" s="137"/>
+      <c r="J42" s="138"/>
       <c r="K42" s="99"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8046,7 +8050,7 @@
         <v>Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)</v>
       </c>
       <c r="I43" s="90"/>
-      <c r="J43" s="136"/>
+      <c r="J43" s="137"/>
       <c r="K43" s="125"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8401,7 +8405,7 @@
         <v>64</v>
       </c>
       <c r="G58" s="70"/>
-      <c r="H58" s="71" t="str">
+      <c r="H58" s="134" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x06h-Testing-Platform-Interaction.md#testing-for-sensitive-functionality-exposure-through-ipc-mstg-platform-4"), "Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)")</f>
         <v>Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)</v>
       </c>
@@ -8759,12 +8763,12 @@
       <c r="G73" s="108"/>
       <c r="H73" s="108"/>
       <c r="I73" s="109"/>
-      <c r="J73" s="138"/>
-      <c r="K73" s="139"/>
+      <c r="J73" s="139"/>
+      <c r="K73" s="140"/>
     </row>
     <row r="74" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="140"/>
-      <c r="C74" s="140"/>
+      <c r="B74" s="141"/>
+      <c r="C74" s="141"/>
       <c r="D74" s="92"/>
       <c r="E74" s="114"/>
       <c r="F74" s="114"/>
@@ -8775,8 +8779,8 @@
       <c r="K74" s="92"/>
     </row>
     <row r="75" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="140"/>
-      <c r="C75" s="140"/>
+      <c r="B75" s="141"/>
+      <c r="C75" s="141"/>
       <c r="D75" s="92"/>
       <c r="E75" s="114"/>
       <c r="F75" s="114"/>
@@ -8787,8 +8791,8 @@
       <c r="K75" s="92"/>
     </row>
     <row r="76" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="140"/>
-      <c r="C76" s="140"/>
+      <c r="B76" s="141"/>
+      <c r="C76" s="141"/>
       <c r="D76" s="92"/>
       <c r="E76" s="114"/>
       <c r="F76" s="114"/>
@@ -8877,8 +8881,8 @@
       <c r="K81" s="92"/>
     </row>
     <row r="82" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="140"/>
-      <c r="C82" s="140"/>
+      <c r="B82" s="141"/>
+      <c r="C82" s="141"/>
       <c r="D82" s="92"/>
       <c r="E82" s="114"/>
       <c r="F82" s="114"/>
@@ -8889,8 +8893,8 @@
       <c r="K82" s="92"/>
     </row>
     <row r="83" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="140"/>
-      <c r="C83" s="140"/>
+      <c r="B83" s="141"/>
+      <c r="C83" s="141"/>
       <c r="D83" s="92"/>
       <c r="E83" s="114"/>
       <c r="F83" s="114"/>
@@ -8901,8 +8905,8 @@
       <c r="K83" s="92"/>
     </row>
     <row r="84" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="140"/>
-      <c r="C84" s="140"/>
+      <c r="B84" s="141"/>
+      <c r="C84" s="141"/>
       <c r="D84" s="92"/>
       <c r="E84" s="114"/>
       <c r="F84" s="114"/>
@@ -8913,8 +8917,8 @@
       <c r="K84" s="92"/>
     </row>
     <row r="85" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="140"/>
-      <c r="C85" s="140"/>
+      <c r="B85" s="141"/>
+      <c r="C85" s="141"/>
       <c r="D85" s="92"/>
       <c r="E85" s="114"/>
       <c r="F85" s="114"/>
@@ -8979,7 +8983,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="129" width="7.3"/>
@@ -9123,7 +9127,7 @@
       <c r="F8" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="141" t="s">
+      <c r="G8" s="142" t="s">
         <v>301</v>
       </c>
       <c r="H8" s="125"/>
@@ -9144,7 +9148,7 @@
       <c r="F9" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G9" s="141" t="s">
+      <c r="G9" s="142" t="s">
         <v>301</v>
       </c>
       <c r="H9" s="125"/>
@@ -9165,7 +9169,7 @@
       <c r="F10" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="141" t="s">
+      <c r="G10" s="142" t="s">
         <v>301</v>
       </c>
       <c r="H10" s="125"/>
@@ -9228,7 +9232,7 @@
       <c r="F13" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="141" t="s">
+      <c r="G13" s="142" t="s">
         <v>301</v>
       </c>
       <c r="H13" s="125"/>
@@ -9293,7 +9297,7 @@
       <c r="F17" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="142" t="str">
+      <c r="G17" s="143" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks-mstg-resilience-3-and-mstg-resilience-11"),"File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)")</f>
         <v>File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)</v>
       </c>
@@ -9330,8 +9334,8 @@
       <c r="H19" s="110"/>
     </row>
     <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="140"/>
-      <c r="C20" s="140"/>
+      <c r="B20" s="141"/>
+      <c r="C20" s="141"/>
       <c r="D20" s="92"/>
       <c r="E20" s="114"/>
       <c r="F20" s="114"/>
@@ -9339,8 +9343,8 @@
       <c r="H20" s="92"/>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="140"/>
-      <c r="C21" s="140"/>
+      <c r="B21" s="141"/>
+      <c r="C21" s="141"/>
       <c r="D21" s="92"/>
       <c r="E21" s="114"/>
       <c r="F21" s="114"/>
@@ -9411,8 +9415,8 @@
       <c r="H26" s="92"/>
     </row>
     <row r="27" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="140"/>
-      <c r="C27" s="140"/>
+      <c r="B27" s="141"/>
+      <c r="C27" s="141"/>
       <c r="D27" s="92"/>
       <c r="E27" s="114"/>
       <c r="F27" s="114"/>
@@ -9420,8 +9424,8 @@
       <c r="H27" s="92"/>
     </row>
     <row r="28" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="140"/>
-      <c r="C28" s="140"/>
+      <c r="B28" s="141"/>
+      <c r="C28" s="141"/>
       <c r="D28" s="92"/>
       <c r="E28" s="114"/>
       <c r="F28" s="114"/>
@@ -9429,8 +9433,8 @@
       <c r="H28" s="92"/>
     </row>
     <row r="29" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="140"/>
-      <c r="C29" s="140"/>
+      <c r="B29" s="141"/>
+      <c r="C29" s="141"/>
       <c r="D29" s="92"/>
       <c r="E29" s="114"/>
       <c r="F29" s="114"/>
@@ -9438,22 +9442,22 @@
       <c r="H29" s="92"/>
     </row>
     <row r="30" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="140"/>
-      <c r="C30" s="140"/>
+      <c r="B30" s="141"/>
+      <c r="C30" s="141"/>
       <c r="D30" s="92"/>
       <c r="E30" s="114"/>
       <c r="F30" s="114"/>
     </row>
     <row r="31" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="140"/>
-      <c r="C31" s="140"/>
+      <c r="B31" s="141"/>
+      <c r="C31" s="141"/>
       <c r="D31" s="92"/>
       <c r="E31" s="114"/>
       <c r="F31" s="114"/>
     </row>
     <row r="32" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="140"/>
-      <c r="C32" s="140"/>
+      <c r="B32" s="141"/>
+      <c r="C32" s="141"/>
       <c r="D32" s="92"/>
       <c r="E32" s="114"/>
       <c r="F32" s="114"/>
@@ -9526,7 +9530,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.7"/>
@@ -9534,412 +9538,412 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="144" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="144"/>
+      <c r="B1" s="144"/>
+      <c r="C1" s="145"/>
       <c r="D1" s="52"/>
       <c r="E1" s="52"/>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="145" t="s">
+      <c r="A2" s="146" t="s">
         <v>319</v>
       </c>
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="146" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="145" t="s">
+      <c r="C2" s="146" t="s">
         <v>321</v>
       </c>
-      <c r="D2" s="145" t="s">
+      <c r="D2" s="146" t="s">
         <v>322</v>
       </c>
-      <c r="E2" s="145" t="s">
+      <c r="E2" s="146" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="146" t="s">
+      <c r="A3" s="147" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="147" t="n">
+      <c r="B3" s="148" t="n">
         <v>0.1</v>
       </c>
-      <c r="C3" s="147"/>
-      <c r="D3" s="148" t="n">
+      <c r="C3" s="148"/>
+      <c r="D3" s="149" t="n">
         <v>42765</v>
       </c>
-      <c r="E3" s="149" t="s">
+      <c r="E3" s="150" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="149" t="s">
+      <c r="A4" s="150" t="s">
         <v>325</v>
       </c>
-      <c r="B4" s="147" t="n">
+      <c r="B4" s="148" t="n">
         <v>0.2</v>
       </c>
-      <c r="C4" s="147"/>
-      <c r="D4" s="148" t="n">
+      <c r="C4" s="148"/>
+      <c r="D4" s="149" t="n">
         <v>42766</v>
       </c>
-      <c r="E4" s="149" t="s">
+      <c r="E4" s="150" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="149" t="s">
+      <c r="A5" s="150" t="s">
         <v>327</v>
       </c>
-      <c r="B5" s="147" t="n">
+      <c r="B5" s="148" t="n">
         <v>0.3</v>
       </c>
-      <c r="C5" s="147"/>
-      <c r="D5" s="148" t="n">
+      <c r="C5" s="148"/>
+      <c r="D5" s="149" t="n">
         <v>42778</v>
       </c>
-      <c r="E5" s="149" t="s">
+      <c r="E5" s="150" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="149" t="s">
+      <c r="A6" s="150" t="s">
         <v>329</v>
       </c>
-      <c r="B6" s="147" t="s">
+      <c r="B6" s="148" t="s">
         <v>330</v>
       </c>
-      <c r="C6" s="147"/>
-      <c r="D6" s="148" t="n">
+      <c r="C6" s="148"/>
+      <c r="D6" s="149" t="n">
         <v>42780</v>
       </c>
-      <c r="E6" s="149" t="s">
+      <c r="E6" s="150" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="149" t="s">
+      <c r="A7" s="150" t="s">
         <v>325</v>
       </c>
-      <c r="B7" s="150" t="s">
+      <c r="B7" s="151" t="s">
         <v>332</v>
       </c>
-      <c r="C7" s="150"/>
-      <c r="D7" s="148" t="n">
+      <c r="C7" s="151"/>
+      <c r="D7" s="149" t="n">
         <v>42781</v>
       </c>
-      <c r="E7" s="149" t="s">
+      <c r="E7" s="150" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="149" t="s">
+      <c r="A8" s="150" t="s">
         <v>329</v>
       </c>
-      <c r="B8" s="150" t="s">
+      <c r="B8" s="151" t="s">
         <v>334</v>
       </c>
-      <c r="C8" s="150"/>
-      <c r="D8" s="148" t="n">
+      <c r="C8" s="151"/>
+      <c r="D8" s="149" t="n">
         <v>42829</v>
       </c>
-      <c r="E8" s="149" t="s">
+      <c r="E8" s="150" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="149" t="s">
+      <c r="A9" s="150" t="s">
         <v>325</v>
       </c>
-      <c r="B9" s="150" t="s">
+      <c r="B9" s="151" t="s">
         <v>334</v>
       </c>
-      <c r="C9" s="150"/>
-      <c r="D9" s="148" t="n">
+      <c r="C9" s="151"/>
+      <c r="D9" s="149" t="n">
         <v>42919</v>
       </c>
-      <c r="E9" s="149" t="s">
+      <c r="E9" s="150" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="149" t="s">
+      <c r="A10" s="150" t="s">
         <v>325</v>
       </c>
-      <c r="B10" s="150" t="s">
+      <c r="B10" s="151" t="s">
         <v>337</v>
       </c>
-      <c r="C10" s="150"/>
-      <c r="D10" s="148" t="n">
+      <c r="C10" s="151"/>
+      <c r="D10" s="149" t="n">
         <v>42963</v>
       </c>
-      <c r="E10" s="149" t="s">
+      <c r="E10" s="150" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="149" t="s">
+      <c r="A11" s="150" t="s">
         <v>325</v>
       </c>
-      <c r="B11" s="150" t="s">
+      <c r="B11" s="151" t="s">
         <v>339</v>
       </c>
-      <c r="C11" s="150"/>
-      <c r="D11" s="148" t="n">
+      <c r="C11" s="151"/>
+      <c r="D11" s="149" t="n">
         <v>43113</v>
       </c>
-      <c r="E11" s="149" t="s">
+      <c r="E11" s="150" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="149" t="s">
+      <c r="A12" s="150" t="s">
         <v>325</v>
       </c>
-      <c r="B12" s="150" t="n">
+      <c r="B12" s="151" t="n">
         <v>1.1</v>
       </c>
-      <c r="C12" s="150"/>
-      <c r="D12" s="148" t="n">
+      <c r="C12" s="151"/>
+      <c r="D12" s="149" t="n">
         <v>43289</v>
       </c>
-      <c r="E12" s="149" t="s">
+      <c r="E12" s="150" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="149" t="s">
+      <c r="A13" s="150" t="s">
         <v>342</v>
       </c>
-      <c r="B13" s="151" t="s">
+      <c r="B13" s="152" t="s">
         <v>343</v>
       </c>
-      <c r="C13" s="152"/>
-      <c r="D13" s="148" t="n">
+      <c r="C13" s="153"/>
+      <c r="D13" s="149" t="n">
         <v>43464</v>
       </c>
-      <c r="E13" s="153" t="s">
+      <c r="E13" s="154" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="149" t="s">
+      <c r="A14" s="150" t="s">
         <v>345</v>
       </c>
-      <c r="B14" s="151" t="s">
+      <c r="B14" s="152" t="s">
         <v>346</v>
       </c>
-      <c r="C14" s="152"/>
-      <c r="D14" s="148" t="n">
+      <c r="C14" s="153"/>
+      <c r="D14" s="149" t="n">
         <v>43469</v>
       </c>
-      <c r="E14" s="153" t="s">
+      <c r="E14" s="154" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="409.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="154" t="s">
+      <c r="A15" s="155" t="s">
         <v>347</v>
       </c>
-      <c r="B15" s="150" t="s">
+      <c r="B15" s="151" t="s">
         <v>348</v>
       </c>
-      <c r="C15" s="150" t="s">
+      <c r="C15" s="151" t="s">
         <v>349</v>
       </c>
-      <c r="D15" s="148" t="n">
+      <c r="D15" s="149" t="n">
         <v>43471</v>
       </c>
-      <c r="E15" s="155" t="s">
+      <c r="E15" s="156" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="149" t="s">
+      <c r="A16" s="150" t="s">
         <v>342</v>
       </c>
-      <c r="B16" s="151" t="s">
+      <c r="B16" s="152" t="s">
         <v>351</v>
       </c>
-      <c r="C16" s="150" t="s">
+      <c r="C16" s="151" t="s">
         <v>349</v>
       </c>
-      <c r="D16" s="156" t="n">
+      <c r="D16" s="157" t="n">
         <v>43475</v>
       </c>
-      <c r="E16" s="153" t="s">
+      <c r="E16" s="154" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="78" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="154" t="s">
+      <c r="A17" s="155" t="s">
         <v>347</v>
       </c>
-      <c r="B17" s="151" t="s">
+      <c r="B17" s="152" t="s">
         <v>353</v>
       </c>
-      <c r="C17" s="150" t="s">
+      <c r="C17" s="151" t="s">
         <v>349</v>
       </c>
-      <c r="D17" s="148" t="n">
+      <c r="D17" s="149" t="n">
         <v>43476</v>
       </c>
-      <c r="E17" s="154" t="s">
+      <c r="E17" s="155" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="154" t="s">
+      <c r="A18" s="155" t="s">
         <v>347</v>
       </c>
-      <c r="B18" s="151" t="s">
+      <c r="B18" s="152" t="s">
         <v>355</v>
       </c>
-      <c r="C18" s="150" t="s">
+      <c r="C18" s="151" t="s">
         <v>349</v>
       </c>
-      <c r="D18" s="148" t="n">
+      <c r="D18" s="149" t="n">
         <v>43478</v>
       </c>
-      <c r="E18" s="154" t="s">
+      <c r="E18" s="155" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="154" t="s">
+      <c r="A19" s="155" t="s">
         <v>347</v>
       </c>
-      <c r="B19" s="151" t="s">
+      <c r="B19" s="152" t="s">
         <v>357</v>
       </c>
-      <c r="C19" s="150" t="s">
+      <c r="C19" s="151" t="s">
         <v>349</v>
       </c>
-      <c r="D19" s="148" t="n">
+      <c r="D19" s="149" t="n">
         <v>43478</v>
       </c>
-      <c r="E19" s="154" t="s">
+      <c r="E19" s="155" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="109.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="154" t="s">
+      <c r="A20" s="155" t="s">
         <v>342</v>
       </c>
-      <c r="B20" s="151" t="s">
+      <c r="B20" s="152" t="s">
         <v>359</v>
       </c>
-      <c r="C20" s="150" t="s">
+      <c r="C20" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="148" t="n">
+      <c r="D20" s="149" t="n">
         <v>43641</v>
       </c>
-      <c r="E20" s="155" t="s">
+      <c r="E20" s="156" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="154" t="s">
+      <c r="A21" s="155" t="s">
         <v>342</v>
       </c>
-      <c r="B21" s="151" t="s">
+      <c r="B21" s="152" t="s">
         <v>361</v>
       </c>
-      <c r="C21" s="150" t="s">
+      <c r="C21" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="148" t="n">
+      <c r="D21" s="149" t="n">
         <v>43642</v>
       </c>
-      <c r="E21" s="154" t="s">
+      <c r="E21" s="155" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="154" t="s">
+      <c r="A22" s="155" t="s">
         <v>342</v>
       </c>
-      <c r="B22" s="151" t="s">
+      <c r="B22" s="152" t="s">
         <v>363</v>
       </c>
-      <c r="C22" s="150" t="s">
+      <c r="C22" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="148" t="n">
+      <c r="D22" s="149" t="n">
         <v>43649</v>
       </c>
-      <c r="E22" s="154" t="s">
+      <c r="E22" s="155" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="154" t="s">
+      <c r="A23" s="155" t="s">
         <v>342</v>
       </c>
-      <c r="B23" s="151" t="s">
+      <c r="B23" s="152" t="s">
         <v>363</v>
       </c>
-      <c r="C23" s="150" t="s">
+      <c r="C23" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="148" t="n">
+      <c r="D23" s="149" t="n">
         <v>43672</v>
       </c>
-      <c r="E23" s="154" t="s">
+      <c r="E23" s="155" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="154" t="s">
+      <c r="A24" s="155" t="s">
         <v>342</v>
       </c>
-      <c r="B24" s="151" t="s">
+      <c r="B24" s="152" t="s">
         <v>363</v>
       </c>
-      <c r="C24" s="150" t="s">
+      <c r="C24" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="148" t="n">
+      <c r="D24" s="149" t="n">
         <v>43674</v>
       </c>
-      <c r="E24" s="154" t="s">
+      <c r="E24" s="155" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="154" t="s">
+      <c r="A25" s="155" t="s">
         <v>342</v>
       </c>
-      <c r="B25" s="151" t="s">
+      <c r="B25" s="152" t="s">
         <v>367</v>
       </c>
-      <c r="C25" s="150" t="s">
+      <c r="C25" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="148" t="n">
+      <c r="D25" s="149" t="n">
         <v>43685</v>
       </c>
-      <c r="E25" s="154" t="s">
+      <c r="E25" s="155" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="154" t="s">
+      <c r="A26" s="155" t="s">
         <v>369</v>
       </c>
-      <c r="B26" s="151" t="s">
+      <c r="B26" s="152" t="s">
         <v>367</v>
       </c>
-      <c r="C26" s="150" t="s">
+      <c r="C26" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="148" t="n">
+      <c r="D26" s="149" t="n">
         <v>43719</v>
       </c>
-      <c r="E26" s="154" t="s">
+      <c r="E26" s="155" t="s">
         <v>370</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Android Security Requiments V1 translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -2216,7 +2216,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="21" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="21" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2228,7 +2228,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2725,7 +2725,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2905,11 +2905,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="52591096"/>
-        <c:axId val="82544757"/>
+        <c:axId val="32912189"/>
+        <c:axId val="78507761"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="52591096"/>
+        <c:axId val="32912189"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2949,7 +2949,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82544757"/>
+        <c:crossAx val="78507761"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2957,7 +2957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82544757"/>
+        <c:axId val="78507761"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3000,7 +3000,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52591096"/>
+        <c:crossAx val="32912189"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3060,7 +3060,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3240,11 +3240,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="15287082"/>
-        <c:axId val="46074959"/>
+        <c:axId val="73179645"/>
+        <c:axId val="17863334"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="15287082"/>
+        <c:axId val="73179645"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3284,7 +3284,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46074959"/>
+        <c:crossAx val="17863334"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3292,7 +3292,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46074959"/>
+        <c:axId val="17863334"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3335,7 +3335,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15287082"/>
+        <c:crossAx val="73179645"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4524,8 +4524,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4638,8 +4638,8 @@
         <v>Информация об архитектуре</v>
       </c>
       <c r="I5" s="71" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x05h-Testing-Platform-Interaction.md#testing-for-insecure-configuration-of-instant-apps-mstg-arch-1-mstg-arch-7"), "Testing for insecure Configuration of Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)")</f>
-        <v>Testing for insecure Configuration of Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x05h-Testing-Platform-Interaction.md#testing-for-insecure-configuration-of-instant-apps-mstg-arch-1-mstg-arch-7"), "Тестирование на небезопасную конфигурацию Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)")</f>
+        <v>Тестирование на небезопасную конфигурацию Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)</v>
       </c>
       <c r="J5" s="72"/>
       <c r="K5" s="73"/>
@@ -4666,8 +4666,8 @@
         <v>Ошибка инъекции (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
       <c r="I6" s="75" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
-        <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Проверка наличия соответствующей авторизации (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
+        <v>Проверка наличия соответствующей авторизации (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
       <c r="J6" s="75"/>
       <c r="K6" s="73"/>
@@ -4794,12 +4794,12 @@
         <v>Тестирование на небезопасную конфигурацию Instant Apps (MSTG-ARCH-1, MSTG-ARCH-7)</v>
       </c>
       <c r="I11" s="75" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#principles-of-testing"), "Principles of Testing")</f>
-        <v>Principles of Testing</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#principles-of-testing"), "Принципы тестирования")</f>
+        <v>Принципы тестирования</v>
       </c>
       <c r="J11" s="78" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#penetration-testing-aka-pentesting"), "Penetration Testing (a.k.a. Pentesting)")</f>
-        <v>Penetration Testing (a.k.a. Pentesting)</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#penetration-testing-aka-pentesting"), "Тестирование на проникновение (a.k.a. Pentesting)")</f>
+        <v>Тестирование на проникновение (a.k.a. Pentesting)</v>
       </c>
       <c r="K11" s="73"/>
     </row>

</xml_diff>

<commit_message>
Android Security Requiments V2 translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -1915,7 +1915,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="160">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2272,192 +2272,200 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="8" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="21" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="22" fillId="7" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="22" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="22" fillId="7" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="8" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="5" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="8" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="21" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="22" fillId="7" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="22" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="22" fillId="7" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="8" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="5" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2725,7 +2733,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2905,11 +2913,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="32912189"/>
-        <c:axId val="78507761"/>
+        <c:axId val="35326757"/>
+        <c:axId val="31600279"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="32912189"/>
+        <c:axId val="35326757"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2949,7 +2957,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78507761"/>
+        <c:crossAx val="31600279"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2957,7 +2965,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78507761"/>
+        <c:axId val="31600279"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3000,7 +3008,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32912189"/>
+        <c:crossAx val="35326757"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3060,7 +3068,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3240,11 +3248,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="73179645"/>
-        <c:axId val="17863334"/>
+        <c:axId val="78372543"/>
+        <c:axId val="50379015"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="73179645"/>
+        <c:axId val="78372543"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3284,7 +3292,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17863334"/>
+        <c:crossAx val="50379015"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3292,7 +3300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="17863334"/>
+        <c:axId val="50379015"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3335,7 +3343,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73179645"/>
+        <c:crossAx val="78372543"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4524,8 +4532,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4912,12 +4920,12 @@
       </c>
       <c r="G16" s="70"/>
       <c r="H16" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-local-storage-for-sensitive-data-mstg-storage-1-and-mstg-storage-2"),"Testing Local Storage for Sensitive Data (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
-        <v>Testing Local Storage for Sensitive Data (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-local-storage-for-sensitive-data-mstg-storage-1-and-mstg-storage-2"),"Проверка наличия конфиденциальных даннх на локальном хранилище (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
+        <v>Проверка наличия конфиденциальных даннх на локальном хранилище (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
       <c r="I16" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-key-management-mstg-storage-1-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
-        <v>Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-key-management-mstg-storage-1-mstg-crypto-1-and-mstg-crypto-5"),"Проверка системы управления ключами (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
+        <v>Проверка системы управления ключами (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
       <c r="J16" s="72"/>
       <c r="K16" s="73"/>
@@ -4936,8 +4944,8 @@
       <c r="F17" s="69"/>
       <c r="G17" s="70"/>
       <c r="H17" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-local-storage-for-sensitive-data-mstg-storage-1-and-mstg-storage-2"),"Testing Local Storage for Sensitive Data (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
-        <v>Testing Local Storage for Sensitive Data (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-local-storage-for-sensitive-data-mstg-storage-1-and-mstg-storage-2"),"Проверка наличия конфиденциальных данных на локальном хранилище (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
+        <v>Проверка наличия конфиденциальных данных на локальном хранилище (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
       <c r="I17" s="76"/>
       <c r="J17" s="76"/>
@@ -4961,8 +4969,8 @@
       </c>
       <c r="G18" s="70"/>
       <c r="H18" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-logs-for-sensitive-data-mstg-storage-3"),"Testing Logs for Sensitive Data (MSTG-STORAGE-3)")</f>
-        <v>Testing Logs for Sensitive Data (MSTG-STORAGE-3)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-logs-for-sensitive-data-mstg-storage-3"),"Проверка наличия конфиденциальных данных в записях лога (MSTG-STORAGE-3)")</f>
+        <v>Проверка наличия конфиденциальных данных в записях лога (MSTG-STORAGE-3)</v>
       </c>
       <c r="I18" s="76"/>
       <c r="J18" s="76"/>
@@ -4986,8 +4994,8 @@
       </c>
       <c r="G19" s="70"/>
       <c r="H19" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-sent-to-third-parties-mstg-storage-4"),"Determining Whether Sensitive Data is Sent to Third Parties (MSTG-STORAGE-4)")</f>
-        <v>Determining Whether Sensitive Data is Sent to Third Parties (MSTG-STORAGE-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-sent-to-third-parties-mstg-storage-4"),"Проверка передачи конфиденциальных данных третим сторонам (MSTG-STORAGE-4)")</f>
+        <v>Проверка передачи конфиденциальных данных третим сторонам (MSTG-STORAGE-4)</v>
       </c>
       <c r="I19" s="76"/>
       <c r="J19" s="76"/>
@@ -5011,8 +5019,8 @@
       </c>
       <c r="G20" s="70"/>
       <c r="H20" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#determining-whether-the-keyboard-cache-is-disabled-for-text-input-fields-mstg-storage-5"),"Determining Whether the Keyboard Cache Is Disabled for Text Input Fields (MSTG-STORAGE-5)")</f>
-        <v>Determining Whether the Keyboard Cache Is Disabled for Text Input Fields (MSTG-STORAGE-5)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#determining-whether-the-keyboard-cache-is-disabled-for-text-input-fields-mstg-storage-5"),"Проверка отключения кэша клавиатуры для полей ввода текста (MSTG-STORAGE-5)")</f>
+        <v>Проверка отключения кэша клавиатуры для полей ввода текста (MSTG-STORAGE-5)</v>
       </c>
       <c r="I20" s="76"/>
       <c r="J20" s="76"/>
@@ -5036,8 +5044,8 @@
       </c>
       <c r="G21" s="70"/>
       <c r="H21" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#determining-whether-sensitive-stored-data-has-been-exposed-via-ipc-mechanisms-mstg-storage-6"),"Determining Whether Sensitive Stored Data Has Been Exposed via IPC Mechanisms (MSTG-STORAGE-6)")</f>
-        <v>Determining Whether Sensitive Stored Data Has Been Exposed via IPC Mechanisms (MSTG-STORAGE-6)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#determining-whether-sensitive-stored-data-has-been-exposed-via-ipc-mechanisms-mstg-storage-6"),"Проверка передачи конфиденциальных данных при обмене данными между потоками (IPC) (MSTG-STORAGE-6)")</f>
+        <v>Проверка передачи конфиденциальных данных при обмене данными между потоками (IPC) (MSTG-STORAGE-6)</v>
       </c>
       <c r="I21" s="76"/>
       <c r="J21" s="76"/>
@@ -5061,8 +5069,8 @@
       </c>
       <c r="G22" s="70"/>
       <c r="H22" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#checking-for-sensitive-data-disclosure-through-the-user-interface-mstg-storage-7"),"Checking for Sensitive Data Disclosure Through the User Interface (MSTG-STORAGE-7)")</f>
-        <v>Checking for Sensitive Data Disclosure Through the User Interface (MSTG-STORAGE-7)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#checking-for-sensitive-data-disclosure-through-the-user-interface-mstg-storage-7"),"Проверка раскрытия конфиденциальных данных через пользовательский интерфейс (MSTG-STORAGE-7)")</f>
+        <v>Проверка раскрытия конфиденциальных данных через пользовательский интерфейс (MSTG-STORAGE-7)</v>
       </c>
       <c r="I22" s="76"/>
       <c r="J22" s="76"/>
@@ -5086,8 +5094,8 @@
         <v>77</v>
       </c>
       <c r="H23" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-backups-for-sensitive-data-mstg-storage-8"),"Testing Backups for Sensitive Data (MSTG-STORAGE-8)")</f>
-        <v>Testing Backups for Sensitive Data (MSTG-STORAGE-8)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-backups-for-sensitive-data-mstg-storage-8"),"Тестирование бэкапов на наличие конфиденциальных данных (MSTG-STORAGE-8)")</f>
+        <v>Тестирование бэкапов на наличие конфиденциальных данных (MSTG-STORAGE-8)</v>
       </c>
       <c r="I23" s="76"/>
       <c r="J23" s="76"/>
@@ -5111,8 +5119,8 @@
         <v>77</v>
       </c>
       <c r="H24" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#finding-sensitive-information-in-auto-generated-screenshots-mstg-storage-9"),"Finding Sensitive Information in Auto-Generated Screenshots (MSTG-STORAGE-9)")</f>
-        <v>Finding Sensitive Information in Auto-Generated Screenshots (MSTG-STORAGE-9)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#finding-sensitive-information-in-auto-generated-screenshots-mstg-storage-9"),"Поиск конфиденциальных данных в автоматически генерируемых снимках экрана (MSTG-STORAGE-9)")</f>
+        <v>Поиск конфиденциальных данных в автоматически генерируемых снимках экрана (MSTG-STORAGE-9)</v>
       </c>
       <c r="I24" s="76"/>
       <c r="J24" s="76"/>
@@ -5136,8 +5144,8 @@
         <v>77</v>
       </c>
       <c r="H25" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#checking-memory-for-sensitive-data-mstg-storage-10"),"Checking Memory for Sensitive Data (MSTG-STORAGE-10)")</f>
-        <v>Checking Memory for Sensitive Data (MSTG-STORAGE-10)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#checking-memory-for-sensitive-data-mstg-storage-10"),"Проверка памяти на конфиденциальные данные (MSTG-STORAGE-10)")</f>
+        <v>Проверка памяти на конфиденциальные данные (MSTG-STORAGE-10)</v>
       </c>
       <c r="I25" s="76"/>
       <c r="J25" s="76"/>
@@ -5161,12 +5169,12 @@
         <v>77</v>
       </c>
       <c r="H26" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-the-device-access-security-policy-mstg-storage-11"),"Testing the Device-Access-Security Policy (MSTG-STORAGE-11)")</f>
-        <v>Testing the Device-Access-Security Policy (MSTG-STORAGE-11)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-the-device-access-security-policy-mstg-storage-11"),"Проверка политики безопасности доступа к устройству (MSTG-STORAGE-11)")</f>
+        <v>Проверка политики безопасности доступа к устройству (MSTG-STORAGE-11)</v>
       </c>
       <c r="I26" s="75" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05f-Testing-Local-Authentication.md#testing-confirm-credentials-mstg-auth-1-and-mstg-storage-11"),"Testing Confirm Credentials (MSTG-AUTH-1 and MSTG-STORAGE-11)")</f>
-        <v>Testing Confirm Credentials (MSTG-AUTH-1 and MSTG-STORAGE-11)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05f-Testing-Local-Authentication.md#testing-confirm-credentials-mstg-auth-1-and-mstg-storage-11"),"Проверка учетных данных (MSTG-AUTH-1 and MSTG-STORAGE-11)")</f>
+        <v>Проверка учетных данных (MSTG-AUTH-1 and MSTG-STORAGE-11)</v>
       </c>
       <c r="J26" s="76"/>
       <c r="K26" s="73"/>
@@ -5189,8 +5197,8 @@
         <v>77</v>
       </c>
       <c r="H27" s="94" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04i-Testing-user-interaction.md#testing-user-education-mstg-storage-12"),"Testing User Education (MSTG-STORAGE-12)")</f>
-        <v>Testing User Education (MSTG-STORAGE-12)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04i-Testing-user-interaction.md#testing-user-education-mstg-storage-12"),"Проверка знаний пользователей (MSTG-STORAGE-12)")</f>
+        <v>Проверка знаний пользователей (MSTG-STORAGE-12)</v>
       </c>
       <c r="I27" s="76"/>
       <c r="J27" s="76"/>
@@ -7140,11 +7148,11 @@
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"), "Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
         <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
-      <c r="I6" s="90" t="str">
+      <c r="I6" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
         <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
-      <c r="J6" s="135"/>
+      <c r="J6" s="136"/>
       <c r="K6" s="73"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7383,7 +7391,7 @@
         <v>64</v>
       </c>
       <c r="G16" s="70"/>
-      <c r="H16" s="90" t="str">
+      <c r="H16" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-local-data-storage-mstg-storage-1-and-mstg-storage-2"),"Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
         <v>Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
@@ -7404,7 +7412,7 @@
       <c r="E17" s="68"/>
       <c r="F17" s="69"/>
       <c r="G17" s="70"/>
-      <c r="H17" s="90" t="str">
+      <c r="H17" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-local-data-storage-mstg-storage-1-and-mstg-storage-2"),"Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
         <v>Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
@@ -7429,7 +7437,7 @@
         <v>64</v>
       </c>
       <c r="G18" s="70"/>
-      <c r="H18" s="90" t="str">
+      <c r="H18" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#checking-logs-for-sensitive-data-mstg-storage-3"),"Checking Logs for Sensitive Data (MSTG-STORAGE-3)")</f>
         <v>Checking Logs for Sensitive Data (MSTG-STORAGE-3)</v>
       </c>
@@ -7454,7 +7462,7 @@
         <v>64</v>
       </c>
       <c r="G19" s="70"/>
-      <c r="H19" s="90" t="str">
+      <c r="H19" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-sent-to-third-parties-mstg-storage-4"),"Determining Whether Sensitive Data Is Sent to Third Parties (MSTG-STORAGE-4)")</f>
         <v>Determining Whether Sensitive Data Is Sent to Third Parties (MSTG-STORAGE-4)</v>
       </c>
@@ -7479,7 +7487,7 @@
         <v>64</v>
       </c>
       <c r="G20" s="70"/>
-      <c r="H20" s="90" t="str">
+      <c r="H20" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#finding-sensitive-data-in-the-keyboard-cache-mstg-storage-5"),"Finding Sensitive Data in the Keyboard Cache (MSTG-STORAGE-5)")</f>
         <v>Finding Sensitive Data in the Keyboard Cache (MSTG-STORAGE-5)</v>
       </c>
@@ -7504,7 +7512,7 @@
         <v>64</v>
       </c>
       <c r="G21" s="70"/>
-      <c r="H21" s="89" t="str">
+      <c r="H21" s="137" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-exposed-via-ipc-mechanisms-mstg-storage-6"),"Determining Whether Sensitive Data Is Exposed via IPC Mechanisms (MSTG-STORAGE-6)")</f>
         <v>Determining Whether Sensitive Data Is Exposed via IPC Mechanisms (MSTG-STORAGE-6)</v>
       </c>
@@ -7529,7 +7537,7 @@
         <v>64</v>
       </c>
       <c r="G22" s="70"/>
-      <c r="H22" s="90" t="str">
+      <c r="H22" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#checking-for-sensitive-data-disclosed-through-the-user-interface-mstg-storage-7"),"Checking for Sensitive Data Disclosed Through the User Interface (MSTG-STORAGE-7)")</f>
         <v>Checking for Sensitive Data Disclosed Through the User Interface (MSTG-STORAGE-7)</v>
       </c>
@@ -7554,7 +7562,7 @@
       <c r="G23" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H23" s="90" t="str">
+      <c r="H23" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-backups-for-sensitive-data-mstg-storage-8"),"Testing Backups for Sensitive Data (MSTG-STORAGE-8)")</f>
         <v>Testing Backups for Sensitive Data (MSTG-STORAGE-8)</v>
       </c>
@@ -7579,7 +7587,7 @@
       <c r="G24" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H24" s="90" t="str">
+      <c r="H24" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-auto-generated-screenshots-for-sensitive-information-mstg-storage-9"),"Testing Auto-Generated Screenshots for Sensitive Information (MSTG-STORAGE-9)")</f>
         <v>Testing Auto-Generated Screenshots for Sensitive Information (MSTG-STORAGE-9)</v>
       </c>
@@ -7604,7 +7612,7 @@
       <c r="G25" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H25" s="90" t="str">
+      <c r="H25" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-memory-for-sensitive-data-mstg-storage-10"),"Testing Memory for Sensitive Data (MSTG-STORAGE-10)")</f>
         <v>Testing Memory for Sensitive Data (MSTG-STORAGE-10)</v>
       </c>
@@ -7629,14 +7637,14 @@
       <c r="G26" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H26" s="90" t="str">
+      <c r="H26" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06f-Testing-Local-Authentication.md#testing-local-authentication-mstg-auth-8-and-mstg-storage-11"),"Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)")</f>
         <v>Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)</v>
       </c>
       <c r="I26" s="76"/>
       <c r="J26" s="76"/>
       <c r="K26" s="73"/>
-      <c r="L26" s="136"/>
+      <c r="L26" s="138"/>
     </row>
     <row r="27" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="87" t="s">
@@ -7697,7 +7705,7 @@
         <v>64</v>
       </c>
       <c r="G29" s="70"/>
-      <c r="H29" s="90" t="str">
+      <c r="H29" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
@@ -7722,7 +7730,7 @@
         <v>64</v>
       </c>
       <c r="G30" s="70"/>
-      <c r="H30" s="89" t="str">
+      <c r="H30" s="137" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#verifying-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-and-mstg-crypto-3"),"Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
@@ -7747,7 +7755,7 @@
         <v>64</v>
       </c>
       <c r="G31" s="70"/>
-      <c r="H31" s="89" t="str">
+      <c r="H31" s="137" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#verifying-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-and-mstg-crypto-3"),"Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
@@ -7772,7 +7780,7 @@
         <v>64</v>
       </c>
       <c r="G32" s="70"/>
-      <c r="H32" s="90" t="str">
+      <c r="H32" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#identifying-insecure-andor-deprecated-cryptographic-algorithms-mstg-crypto-4"),"Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)")</f>
         <v>Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)</v>
       </c>
@@ -7797,7 +7805,7 @@
         <v>64</v>
       </c>
       <c r="G33" s="70"/>
-      <c r="H33" s="90" t="str">
+      <c r="H33" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
@@ -7822,7 +7830,7 @@
         <v>64</v>
       </c>
       <c r="G34" s="70"/>
-      <c r="H34" s="90" t="str">
+      <c r="H34" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-random-number-generation-mstg-crypto-6")," Testing Random Number Generation (MSTG-CRYPTO-6)")</f>
         <v> Testing Random Number Generation (MSTG-CRYPTO-6)</v>
       </c>
@@ -7863,7 +7871,7 @@
         <v>64</v>
       </c>
       <c r="G36" s="70"/>
-      <c r="H36" s="90" t="str">
+      <c r="H36" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
         <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
@@ -7871,7 +7879,7 @@
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
-      <c r="J36" s="137"/>
+      <c r="J36" s="139"/>
       <c r="K36" s="125"/>
     </row>
     <row r="37" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7891,7 +7899,7 @@
         <v>64</v>
       </c>
       <c r="G37" s="70"/>
-      <c r="H37" s="90" t="str">
+      <c r="H37" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateful-session-management-mstg-auth-2"),"Testing Stateful Session Management (MSTG-AUTH-2)")</f>
         <v>Testing Stateful Session Management (MSTG-AUTH-2)</v>
       </c>
@@ -7916,7 +7924,7 @@
         <v>64</v>
       </c>
       <c r="G38" s="70"/>
-      <c r="H38" s="90" t="str">
+      <c r="H38" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateless-token-based-authentication-mstg-auth-3"),"Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)")</f>
         <v>Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)</v>
       </c>
@@ -7924,7 +7932,7 @@
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
-      <c r="J38" s="137"/>
+      <c r="J38" s="139"/>
       <c r="K38" s="125"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7940,7 +7948,7 @@
       <c r="E39" s="68"/>
       <c r="F39" s="69"/>
       <c r="G39" s="70"/>
-      <c r="H39" s="90" t="str">
+      <c r="H39" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-user-logout-mstg-auth-4"),"Testing User Logout (MSTG-AUTH-4)")</f>
         <v>Testing User Logout (MSTG-AUTH-4)</v>
       </c>
@@ -7966,7 +7974,7 @@
         <v>64</v>
       </c>
       <c r="G40" s="70"/>
-      <c r="H40" s="90" t="str">
+      <c r="H40" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
         <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
@@ -7992,7 +8000,7 @@
         <v>64</v>
       </c>
       <c r="G41" s="70"/>
-      <c r="H41" s="90" t="str">
+      <c r="H41" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
         <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
@@ -8000,7 +8008,7 @@
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#dynamic-testing-mstg-auth-6"),"Dynamic Testing (MSTG-AUTH-6)")</f>
         <v>Dynamic Testing (MSTG-AUTH-6)</v>
       </c>
-      <c r="J41" s="137"/>
+      <c r="J41" s="139"/>
       <c r="K41" s="125"/>
     </row>
     <row r="42" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8020,12 +8028,12 @@
         <v>64</v>
       </c>
       <c r="G42" s="70"/>
-      <c r="H42" s="90" t="str">
+      <c r="H42" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-session-timeout-mstg-auth-7"),"Testing Session Timeout (MSTG-AUTH-7)")</f>
         <v>Testing Session Timeout (MSTG-AUTH-7)</v>
       </c>
       <c r="I42" s="97"/>
-      <c r="J42" s="138"/>
+      <c r="J42" s="140"/>
       <c r="K42" s="99"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8045,12 +8053,12 @@
       <c r="G43" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H43" s="90" t="str">
+      <c r="H43" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06f-Testing-Local-Authentication.md#testing-local-authentication-mstg-auth-8-and-mstg-storage-11"),"Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)")</f>
         <v>Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)</v>
       </c>
       <c r="I43" s="90"/>
-      <c r="J43" s="137"/>
+      <c r="J43" s="139"/>
       <c r="K43" s="125"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8070,7 +8078,7 @@
       <c r="G44" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H44" s="89" t="str">
+      <c r="H44" s="137" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
@@ -8095,7 +8103,7 @@
       <c r="G45" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H45" s="89" t="str">
+      <c r="H45" s="137" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
@@ -8161,7 +8169,7 @@
         <v>64</v>
       </c>
       <c r="G48" s="70"/>
-      <c r="H48" s="89" t="str">
+      <c r="H48" s="137" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
@@ -8186,7 +8194,7 @@
         <v>64</v>
       </c>
       <c r="G49" s="70"/>
-      <c r="H49" s="89" t="str">
+      <c r="H49" s="137" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
@@ -8214,7 +8222,7 @@
         <v>64</v>
       </c>
       <c r="G50" s="70"/>
-      <c r="H50" s="90" t="str">
+      <c r="H50" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-3-and-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)")</f>
         <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)</v>
       </c>
@@ -8239,7 +8247,7 @@
       <c r="G51" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H51" s="90" t="str">
+      <c r="H51" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-3-and-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)")</f>
         <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)</v>
       </c>
@@ -8264,7 +8272,7 @@
       <c r="G52" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H52" s="89" t="str">
+      <c r="H52" s="137" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels-mstg-network-5"),"Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)")</f>
         <v>Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)</v>
       </c>
@@ -8289,7 +8297,7 @@
       <c r="G53" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H53" s="90" t="str">
+      <c r="H53" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x06i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"), "Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
         <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
       </c>
@@ -8330,7 +8338,7 @@
         <v>64</v>
       </c>
       <c r="G55" s="70"/>
-      <c r="H55" s="90" t="str">
+      <c r="H55" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-app-permissions-mstg-platform-1"),"Testing App Permissions (MSTG-PLATFORM-1)")</f>
         <v>Testing App Permissions (MSTG-PLATFORM-1)</v>
       </c>
@@ -8355,7 +8363,7 @@
         <v>64</v>
       </c>
       <c r="G56" s="70"/>
-      <c r="H56" s="90" t="str">
+      <c r="H56" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"),"Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
         <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
@@ -8380,7 +8388,7 @@
         <v>64</v>
       </c>
       <c r="G57" s="70"/>
-      <c r="H57" s="90" t="str">
+      <c r="H57" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-custom-url-schemes-mstg-platform-3"),"Testing Custom URL Schemes (MSTG-PLATFORM-3)")</f>
         <v>Testing Custom URL Schemes (MSTG-PLATFORM-3)</v>
       </c>
@@ -8430,7 +8438,7 @@
         <v>64</v>
       </c>
       <c r="G59" s="70"/>
-      <c r="H59" s="90" t="str">
+      <c r="H59" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-ios-webviews-mstg-platform-5"),"Testing iOS WebViews (MSTG-PLATFORM-5)")</f>
         <v>Testing iOS WebViews (MSTG-PLATFORM-5)</v>
       </c>
@@ -8455,7 +8463,7 @@
         <v>64</v>
       </c>
       <c r="G60" s="70"/>
-      <c r="H60" s="90" t="str">
+      <c r="H60" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-webview-protocol-handlers-mstg-platform-6"),"Testing WebView Protocol Handlers (MSTG-PLATFORM-6)")</f>
         <v>Testing WebView Protocol Handlers (MSTG-PLATFORM-6)</v>
       </c>
@@ -8480,7 +8488,7 @@
         <v>64</v>
       </c>
       <c r="G61" s="70"/>
-      <c r="H61" s="90" t="str">
+      <c r="H61" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#determining-whether-native-methods-are-exposed-through-webviews-mstg-platform-7"),"Determining Whether Native Methods Are Exposed Through WebViews (MSTG-PLATFORM-7)")</f>
         <v>Determining Whether Native Methods Are Exposed Through WebViews (MSTG-PLATFORM-7)</v>
       </c>
@@ -8505,7 +8513,7 @@
         <v>64</v>
       </c>
       <c r="G62" s="70"/>
-      <c r="H62" s="90" t="str">
+      <c r="H62" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-object-persistence-mstg-platform-8"),"Testing Object Persistence (MSTG-PLATFORM-8)")</f>
         <v>Testing Object Persistence (MSTG-PLATFORM-8)</v>
       </c>
@@ -8546,7 +8554,7 @@
         <v>64</v>
       </c>
       <c r="G64" s="70"/>
-      <c r="H64" s="90" t="str">
+      <c r="H64" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#making-sure-that-the-app-is-properly-signed-mstg-code-1"),"Making Sure that the App Is Properly Signed (MSTG-CODE-1)")</f>
         <v>Making Sure that the App Is Properly Signed (MSTG-CODE-1)</v>
       </c>
@@ -8571,7 +8579,7 @@
         <v>64</v>
       </c>
       <c r="G65" s="70"/>
-      <c r="H65" s="90" t="str">
+      <c r="H65" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#determining-whether-the-app-is-debuggable-mstg-code-2"),"Determining Whether the App is Debuggable (MSTG-CODE-2)")</f>
         <v>Determining Whether the App is Debuggable (MSTG-CODE-2)</v>
       </c>
@@ -8596,7 +8604,7 @@
         <v>64</v>
       </c>
       <c r="G66" s="70"/>
-      <c r="H66" s="90" t="str">
+      <c r="H66" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-symbols-mstg-code-3"),"Finding Debugging Symbols (MSTG-CODE-3)")</f>
         <v>Finding Debugging Symbols (MSTG-CODE-3)</v>
       </c>
@@ -8621,7 +8629,7 @@
         <v>64</v>
       </c>
       <c r="G67" s="70"/>
-      <c r="H67" s="90" t="str">
+      <c r="H67" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-code-and-verbose-error-logging-mstg-code-4"),"Finding Debugging Code and Verbose Error Logging (MSTG-CODE-4)")</f>
         <v>Finding Debugging Code and Verbose Error Logging (MSTG-CODE-4)</v>
       </c>
@@ -8671,7 +8679,7 @@
         <v>64</v>
       </c>
       <c r="G69" s="70"/>
-      <c r="H69" s="90" t="str">
+      <c r="H69" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6"),"Testing Exception Handling (MSTG-CODE-6)")</f>
         <v>Testing Exception Handling (MSTG-CODE-6)</v>
       </c>
@@ -8696,7 +8704,7 @@
         <v>64</v>
       </c>
       <c r="G70" s="70"/>
-      <c r="H70" s="90" t="str">
+      <c r="H70" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6"),"Testing Exception Handling (MSTG-CODE-6)")</f>
         <v>Testing Exception Handling (MSTG-CODE-6)</v>
       </c>
@@ -8721,7 +8729,7 @@
         <v>64</v>
       </c>
       <c r="G71" s="70"/>
-      <c r="H71" s="90" t="str">
+      <c r="H71" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#memory-corruption-bugs-mstg-code-8"),"Memory Corruption Bugs (MSTG-CODE-8)")</f>
         <v>Memory Corruption Bugs (MSTG-CODE-8)</v>
       </c>
@@ -8746,7 +8754,7 @@
         <v>64</v>
       </c>
       <c r="G72" s="70"/>
-      <c r="H72" s="90" t="str">
+      <c r="H72" s="135" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#make-sure-that-free-security-features-are-activated-mstg-code-9"),"Make Sure That Free Security Features Are Activated (MSTG-CODE-9)")</f>
         <v>Make Sure That Free Security Features Are Activated (MSTG-CODE-9)</v>
       </c>
@@ -8763,12 +8771,12 @@
       <c r="G73" s="108"/>
       <c r="H73" s="108"/>
       <c r="I73" s="109"/>
-      <c r="J73" s="139"/>
-      <c r="K73" s="140"/>
+      <c r="J73" s="141"/>
+      <c r="K73" s="142"/>
     </row>
     <row r="74" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="141"/>
-      <c r="C74" s="141"/>
+      <c r="B74" s="143"/>
+      <c r="C74" s="143"/>
       <c r="D74" s="92"/>
       <c r="E74" s="114"/>
       <c r="F74" s="114"/>
@@ -8779,8 +8787,8 @@
       <c r="K74" s="92"/>
     </row>
     <row r="75" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="141"/>
-      <c r="C75" s="141"/>
+      <c r="B75" s="143"/>
+      <c r="C75" s="143"/>
       <c r="D75" s="92"/>
       <c r="E75" s="114"/>
       <c r="F75" s="114"/>
@@ -8791,8 +8799,8 @@
       <c r="K75" s="92"/>
     </row>
     <row r="76" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="141"/>
-      <c r="C76" s="141"/>
+      <c r="B76" s="143"/>
+      <c r="C76" s="143"/>
       <c r="D76" s="92"/>
       <c r="E76" s="114"/>
       <c r="F76" s="114"/>
@@ -8881,8 +8889,8 @@
       <c r="K81" s="92"/>
     </row>
     <row r="82" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="141"/>
-      <c r="C82" s="141"/>
+      <c r="B82" s="143"/>
+      <c r="C82" s="143"/>
       <c r="D82" s="92"/>
       <c r="E82" s="114"/>
       <c r="F82" s="114"/>
@@ -8893,8 +8901,8 @@
       <c r="K82" s="92"/>
     </row>
     <row r="83" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="141"/>
-      <c r="C83" s="141"/>
+      <c r="B83" s="143"/>
+      <c r="C83" s="143"/>
       <c r="D83" s="92"/>
       <c r="E83" s="114"/>
       <c r="F83" s="114"/>
@@ -8905,8 +8913,8 @@
       <c r="K83" s="92"/>
     </row>
     <row r="84" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="141"/>
-      <c r="C84" s="141"/>
+      <c r="B84" s="143"/>
+      <c r="C84" s="143"/>
       <c r="D84" s="92"/>
       <c r="E84" s="114"/>
       <c r="F84" s="114"/>
@@ -8917,8 +8925,8 @@
       <c r="K84" s="92"/>
     </row>
     <row r="85" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="141"/>
-      <c r="C85" s="141"/>
+      <c r="B85" s="143"/>
+      <c r="C85" s="143"/>
       <c r="D85" s="92"/>
       <c r="E85" s="114"/>
       <c r="F85" s="114"/>
@@ -9127,7 +9135,7 @@
       <c r="F8" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="142" t="s">
+      <c r="G8" s="144" t="s">
         <v>301</v>
       </c>
       <c r="H8" s="125"/>
@@ -9148,7 +9156,7 @@
       <c r="F9" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G9" s="142" t="s">
+      <c r="G9" s="144" t="s">
         <v>301</v>
       </c>
       <c r="H9" s="125"/>
@@ -9169,7 +9177,7 @@
       <c r="F10" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="142" t="s">
+      <c r="G10" s="144" t="s">
         <v>301</v>
       </c>
       <c r="H10" s="125"/>
@@ -9232,7 +9240,7 @@
       <c r="F13" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="142" t="s">
+      <c r="G13" s="144" t="s">
         <v>301</v>
       </c>
       <c r="H13" s="125"/>
@@ -9297,7 +9305,7 @@
       <c r="F17" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="143" t="str">
+      <c r="G17" s="145" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks-mstg-resilience-3-and-mstg-resilience-11"),"File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)")</f>
         <v>File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)</v>
       </c>
@@ -9334,8 +9342,8 @@
       <c r="H19" s="110"/>
     </row>
     <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="141"/>
-      <c r="C20" s="141"/>
+      <c r="B20" s="143"/>
+      <c r="C20" s="143"/>
       <c r="D20" s="92"/>
       <c r="E20" s="114"/>
       <c r="F20" s="114"/>
@@ -9343,8 +9351,8 @@
       <c r="H20" s="92"/>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="141"/>
-      <c r="C21" s="141"/>
+      <c r="B21" s="143"/>
+      <c r="C21" s="143"/>
       <c r="D21" s="92"/>
       <c r="E21" s="114"/>
       <c r="F21" s="114"/>
@@ -9415,8 +9423,8 @@
       <c r="H26" s="92"/>
     </row>
     <row r="27" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="141"/>
-      <c r="C27" s="141"/>
+      <c r="B27" s="143"/>
+      <c r="C27" s="143"/>
       <c r="D27" s="92"/>
       <c r="E27" s="114"/>
       <c r="F27" s="114"/>
@@ -9424,8 +9432,8 @@
       <c r="H27" s="92"/>
     </row>
     <row r="28" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="141"/>
-      <c r="C28" s="141"/>
+      <c r="B28" s="143"/>
+      <c r="C28" s="143"/>
       <c r="D28" s="92"/>
       <c r="E28" s="114"/>
       <c r="F28" s="114"/>
@@ -9433,8 +9441,8 @@
       <c r="H28" s="92"/>
     </row>
     <row r="29" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="141"/>
-      <c r="C29" s="141"/>
+      <c r="B29" s="143"/>
+      <c r="C29" s="143"/>
       <c r="D29" s="92"/>
       <c r="E29" s="114"/>
       <c r="F29" s="114"/>
@@ -9442,22 +9450,22 @@
       <c r="H29" s="92"/>
     </row>
     <row r="30" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="141"/>
-      <c r="C30" s="141"/>
+      <c r="B30" s="143"/>
+      <c r="C30" s="143"/>
       <c r="D30" s="92"/>
       <c r="E30" s="114"/>
       <c r="F30" s="114"/>
     </row>
     <row r="31" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="141"/>
-      <c r="C31" s="141"/>
+      <c r="B31" s="143"/>
+      <c r="C31" s="143"/>
       <c r="D31" s="92"/>
       <c r="E31" s="114"/>
       <c r="F31" s="114"/>
     </row>
     <row r="32" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="141"/>
-      <c r="C32" s="141"/>
+      <c r="B32" s="143"/>
+      <c r="C32" s="143"/>
       <c r="D32" s="92"/>
       <c r="E32" s="114"/>
       <c r="F32" s="114"/>
@@ -9538,412 +9546,412 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="146" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="145"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="147"/>
       <c r="D1" s="52"/>
       <c r="E1" s="52"/>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="148" t="s">
         <v>319</v>
       </c>
-      <c r="B2" s="146" t="s">
+      <c r="B2" s="148" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="146" t="s">
+      <c r="C2" s="148" t="s">
         <v>321</v>
       </c>
-      <c r="D2" s="146" t="s">
+      <c r="D2" s="148" t="s">
         <v>322</v>
       </c>
-      <c r="E2" s="146" t="s">
+      <c r="E2" s="148" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="147" t="s">
+      <c r="A3" s="149" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="148" t="n">
+      <c r="B3" s="150" t="n">
         <v>0.1</v>
       </c>
-      <c r="C3" s="148"/>
-      <c r="D3" s="149" t="n">
+      <c r="C3" s="150"/>
+      <c r="D3" s="151" t="n">
         <v>42765</v>
       </c>
-      <c r="E3" s="150" t="s">
+      <c r="E3" s="152" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="150" t="s">
+      <c r="A4" s="152" t="s">
         <v>325</v>
       </c>
-      <c r="B4" s="148" t="n">
+      <c r="B4" s="150" t="n">
         <v>0.2</v>
       </c>
-      <c r="C4" s="148"/>
-      <c r="D4" s="149" t="n">
+      <c r="C4" s="150"/>
+      <c r="D4" s="151" t="n">
         <v>42766</v>
       </c>
-      <c r="E4" s="150" t="s">
+      <c r="E4" s="152" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="150" t="s">
+      <c r="A5" s="152" t="s">
         <v>327</v>
       </c>
-      <c r="B5" s="148" t="n">
+      <c r="B5" s="150" t="n">
         <v>0.3</v>
       </c>
-      <c r="C5" s="148"/>
-      <c r="D5" s="149" t="n">
+      <c r="C5" s="150"/>
+      <c r="D5" s="151" t="n">
         <v>42778</v>
       </c>
-      <c r="E5" s="150" t="s">
+      <c r="E5" s="152" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="150" t="s">
+      <c r="A6" s="152" t="s">
         <v>329</v>
       </c>
-      <c r="B6" s="148" t="s">
+      <c r="B6" s="150" t="s">
         <v>330</v>
       </c>
-      <c r="C6" s="148"/>
-      <c r="D6" s="149" t="n">
+      <c r="C6" s="150"/>
+      <c r="D6" s="151" t="n">
         <v>42780</v>
       </c>
-      <c r="E6" s="150" t="s">
+      <c r="E6" s="152" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="150" t="s">
+      <c r="A7" s="152" t="s">
         <v>325</v>
       </c>
-      <c r="B7" s="151" t="s">
+      <c r="B7" s="153" t="s">
         <v>332</v>
       </c>
-      <c r="C7" s="151"/>
-      <c r="D7" s="149" t="n">
+      <c r="C7" s="153"/>
+      <c r="D7" s="151" t="n">
         <v>42781</v>
       </c>
-      <c r="E7" s="150" t="s">
+      <c r="E7" s="152" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="150" t="s">
+      <c r="A8" s="152" t="s">
         <v>329</v>
       </c>
-      <c r="B8" s="151" t="s">
+      <c r="B8" s="153" t="s">
         <v>334</v>
       </c>
-      <c r="C8" s="151"/>
-      <c r="D8" s="149" t="n">
+      <c r="C8" s="153"/>
+      <c r="D8" s="151" t="n">
         <v>42829</v>
       </c>
-      <c r="E8" s="150" t="s">
+      <c r="E8" s="152" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="150" t="s">
+      <c r="A9" s="152" t="s">
         <v>325</v>
       </c>
-      <c r="B9" s="151" t="s">
+      <c r="B9" s="153" t="s">
         <v>334</v>
       </c>
-      <c r="C9" s="151"/>
-      <c r="D9" s="149" t="n">
+      <c r="C9" s="153"/>
+      <c r="D9" s="151" t="n">
         <v>42919</v>
       </c>
-      <c r="E9" s="150" t="s">
+      <c r="E9" s="152" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="150" t="s">
+      <c r="A10" s="152" t="s">
         <v>325</v>
       </c>
-      <c r="B10" s="151" t="s">
+      <c r="B10" s="153" t="s">
         <v>337</v>
       </c>
-      <c r="C10" s="151"/>
-      <c r="D10" s="149" t="n">
+      <c r="C10" s="153"/>
+      <c r="D10" s="151" t="n">
         <v>42963</v>
       </c>
-      <c r="E10" s="150" t="s">
+      <c r="E10" s="152" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="150" t="s">
+      <c r="A11" s="152" t="s">
         <v>325</v>
       </c>
-      <c r="B11" s="151" t="s">
+      <c r="B11" s="153" t="s">
         <v>339</v>
       </c>
-      <c r="C11" s="151"/>
-      <c r="D11" s="149" t="n">
+      <c r="C11" s="153"/>
+      <c r="D11" s="151" t="n">
         <v>43113</v>
       </c>
-      <c r="E11" s="150" t="s">
+      <c r="E11" s="152" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="150" t="s">
+      <c r="A12" s="152" t="s">
         <v>325</v>
       </c>
-      <c r="B12" s="151" t="n">
+      <c r="B12" s="153" t="n">
         <v>1.1</v>
       </c>
-      <c r="C12" s="151"/>
-      <c r="D12" s="149" t="n">
+      <c r="C12" s="153"/>
+      <c r="D12" s="151" t="n">
         <v>43289</v>
       </c>
-      <c r="E12" s="150" t="s">
+      <c r="E12" s="152" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="150" t="s">
+      <c r="A13" s="152" t="s">
         <v>342</v>
       </c>
-      <c r="B13" s="152" t="s">
+      <c r="B13" s="154" t="s">
         <v>343</v>
       </c>
-      <c r="C13" s="153"/>
-      <c r="D13" s="149" t="n">
+      <c r="C13" s="155"/>
+      <c r="D13" s="151" t="n">
         <v>43464</v>
       </c>
-      <c r="E13" s="154" t="s">
+      <c r="E13" s="156" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="150" t="s">
+      <c r="A14" s="152" t="s">
         <v>345</v>
       </c>
-      <c r="B14" s="152" t="s">
+      <c r="B14" s="154" t="s">
         <v>346</v>
       </c>
-      <c r="C14" s="153"/>
-      <c r="D14" s="149" t="n">
+      <c r="C14" s="155"/>
+      <c r="D14" s="151" t="n">
         <v>43469</v>
       </c>
-      <c r="E14" s="154" t="s">
+      <c r="E14" s="156" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="409.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="155" t="s">
+      <c r="A15" s="157" t="s">
         <v>347</v>
       </c>
-      <c r="B15" s="151" t="s">
+      <c r="B15" s="153" t="s">
         <v>348</v>
       </c>
-      <c r="C15" s="151" t="s">
+      <c r="C15" s="153" t="s">
         <v>349</v>
       </c>
-      <c r="D15" s="149" t="n">
+      <c r="D15" s="151" t="n">
         <v>43471</v>
       </c>
-      <c r="E15" s="156" t="s">
+      <c r="E15" s="158" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="150" t="s">
+      <c r="A16" s="152" t="s">
         <v>342</v>
       </c>
-      <c r="B16" s="152" t="s">
+      <c r="B16" s="154" t="s">
         <v>351</v>
       </c>
-      <c r="C16" s="151" t="s">
+      <c r="C16" s="153" t="s">
         <v>349</v>
       </c>
-      <c r="D16" s="157" t="n">
+      <c r="D16" s="159" t="n">
         <v>43475</v>
       </c>
-      <c r="E16" s="154" t="s">
+      <c r="E16" s="156" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="78" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="155" t="s">
+      <c r="A17" s="157" t="s">
         <v>347</v>
       </c>
-      <c r="B17" s="152" t="s">
+      <c r="B17" s="154" t="s">
         <v>353</v>
       </c>
-      <c r="C17" s="151" t="s">
+      <c r="C17" s="153" t="s">
         <v>349</v>
       </c>
-      <c r="D17" s="149" t="n">
+      <c r="D17" s="151" t="n">
         <v>43476</v>
       </c>
-      <c r="E17" s="155" t="s">
+      <c r="E17" s="157" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="155" t="s">
+      <c r="A18" s="157" t="s">
         <v>347</v>
       </c>
-      <c r="B18" s="152" t="s">
+      <c r="B18" s="154" t="s">
         <v>355</v>
       </c>
-      <c r="C18" s="151" t="s">
+      <c r="C18" s="153" t="s">
         <v>349</v>
       </c>
-      <c r="D18" s="149" t="n">
+      <c r="D18" s="151" t="n">
         <v>43478</v>
       </c>
-      <c r="E18" s="155" t="s">
+      <c r="E18" s="157" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="155" t="s">
+      <c r="A19" s="157" t="s">
         <v>347</v>
       </c>
-      <c r="B19" s="152" t="s">
+      <c r="B19" s="154" t="s">
         <v>357</v>
       </c>
-      <c r="C19" s="151" t="s">
+      <c r="C19" s="153" t="s">
         <v>349</v>
       </c>
-      <c r="D19" s="149" t="n">
+      <c r="D19" s="151" t="n">
         <v>43478</v>
       </c>
-      <c r="E19" s="155" t="s">
+      <c r="E19" s="157" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="109.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="155" t="s">
+      <c r="A20" s="157" t="s">
         <v>342</v>
       </c>
-      <c r="B20" s="152" t="s">
+      <c r="B20" s="154" t="s">
         <v>359</v>
       </c>
-      <c r="C20" s="151" t="s">
+      <c r="C20" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="149" t="n">
+      <c r="D20" s="151" t="n">
         <v>43641</v>
       </c>
-      <c r="E20" s="156" t="s">
+      <c r="E20" s="158" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="155" t="s">
+      <c r="A21" s="157" t="s">
         <v>342</v>
       </c>
-      <c r="B21" s="152" t="s">
+      <c r="B21" s="154" t="s">
         <v>361</v>
       </c>
-      <c r="C21" s="151" t="s">
+      <c r="C21" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="149" t="n">
+      <c r="D21" s="151" t="n">
         <v>43642</v>
       </c>
-      <c r="E21" s="155" t="s">
+      <c r="E21" s="157" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="155" t="s">
+      <c r="A22" s="157" t="s">
         <v>342</v>
       </c>
-      <c r="B22" s="152" t="s">
+      <c r="B22" s="154" t="s">
         <v>363</v>
       </c>
-      <c r="C22" s="151" t="s">
+      <c r="C22" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="149" t="n">
+      <c r="D22" s="151" t="n">
         <v>43649</v>
       </c>
-      <c r="E22" s="155" t="s">
+      <c r="E22" s="157" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="155" t="s">
+      <c r="A23" s="157" t="s">
         <v>342</v>
       </c>
-      <c r="B23" s="152" t="s">
+      <c r="B23" s="154" t="s">
         <v>363</v>
       </c>
-      <c r="C23" s="151" t="s">
+      <c r="C23" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="149" t="n">
+      <c r="D23" s="151" t="n">
         <v>43672</v>
       </c>
-      <c r="E23" s="155" t="s">
+      <c r="E23" s="157" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="155" t="s">
+      <c r="A24" s="157" t="s">
         <v>342</v>
       </c>
-      <c r="B24" s="152" t="s">
+      <c r="B24" s="154" t="s">
         <v>363</v>
       </c>
-      <c r="C24" s="151" t="s">
+      <c r="C24" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="149" t="n">
+      <c r="D24" s="151" t="n">
         <v>43674</v>
       </c>
-      <c r="E24" s="155" t="s">
+      <c r="E24" s="157" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="155" t="s">
+      <c r="A25" s="157" t="s">
         <v>342</v>
       </c>
-      <c r="B25" s="152" t="s">
+      <c r="B25" s="154" t="s">
         <v>367</v>
       </c>
-      <c r="C25" s="151" t="s">
+      <c r="C25" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="149" t="n">
+      <c r="D25" s="151" t="n">
         <v>43685</v>
       </c>
-      <c r="E25" s="155" t="s">
+      <c r="E25" s="157" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="155" t="s">
+      <c r="A26" s="157" t="s">
         <v>369</v>
       </c>
-      <c r="B26" s="152" t="s">
+      <c r="B26" s="154" t="s">
         <v>367</v>
       </c>
-      <c r="C26" s="151" t="s">
+      <c r="C26" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="149" t="n">
+      <c r="D26" s="151" t="n">
         <v>43719</v>
       </c>
-      <c r="E26" s="155" t="s">
+      <c r="E26" s="157" t="s">
         <v>370</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Android Security Requiments V3 translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -2733,7 +2733,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2913,11 +2913,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="35326757"/>
-        <c:axId val="31600279"/>
+        <c:axId val="20604495"/>
+        <c:axId val="78361298"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="35326757"/>
+        <c:axId val="20604495"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2957,7 +2957,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31600279"/>
+        <c:crossAx val="78361298"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2965,7 +2965,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31600279"/>
+        <c:axId val="78361298"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3008,7 +3008,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35326757"/>
+        <c:crossAx val="20604495"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3068,7 +3068,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3248,11 +3248,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="78372543"/>
-        <c:axId val="50379015"/>
+        <c:axId val="28333765"/>
+        <c:axId val="39605995"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="78372543"/>
+        <c:axId val="28333765"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3292,7 +3292,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50379015"/>
+        <c:crossAx val="39605995"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3300,7 +3300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50379015"/>
+        <c:axId val="39605995"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3343,7 +3343,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78372543"/>
+        <c:crossAx val="28333765"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4532,8 +4532,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J37" activeCellId="0" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5238,12 +5238,12 @@
       </c>
       <c r="G29" s="70"/>
       <c r="H29" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-key-management-mstg-storage-1-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
-        <v>Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-key-management-mstg-storage-1-mstg-crypto-1-and-mstg-crypto-5"),"Проверка системы управления ключами (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
+        <v>Проверка системы управления ключами (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
       <c r="I29" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#common-configuration-issues-mstg-crypto-1-mstg-crypto-2-and-mstg-crypto-3"),"Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
-        <v>Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#common-configuration-issues-mstg-crypto-1-mstg-crypto-2-and-mstg-crypto-3"),"Общие проблемы конфигурации (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
+        <v>Общие проблемы конфигурации (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
       <c r="J29" s="72"/>
       <c r="K29" s="73"/>
@@ -5266,17 +5266,17 @@
       </c>
       <c r="G30" s="70"/>
       <c r="H30" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#common-configuration-issues-mstg-crypto-1-mstg-crypto-2-and-mstg-crypto-3"),"Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
-        <v>Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#common-configuration-issues-mstg-crypto-1-mstg-crypto-2-and-mstg-crypto-3"),"Общие проблемы конфигурации (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
+        <v>Общие проблемы конфигурации (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
       <c r="I30" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-mstg-crypto-3-and-mstg-crypto-4"),"Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)")</f>
-        <v>Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-mstg-crypto-3-and-mstg-crypto-4"),"Тестирование конфигурации криптографических стандартных алгоритмов (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)")</f>
+        <v>Тестирование конфигурации криптографических стандартных алгоритмов (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)</v>
       </c>
       <c r="J30" s="72"/>
       <c r="K30" s="73"/>
     </row>
-    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="87" t="s">
         <v>139</v>
       </c>
@@ -5294,12 +5294,12 @@
       </c>
       <c r="G31" s="70"/>
       <c r="H31" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-mstg-crypto-3-and-mstg-crypto-4"),"Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)")</f>
-        <v>Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-mstg-crypto-3-and-mstg-crypto-4"),"Тестирование конфигурации криптографических стандартных алгоритмов (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)")</f>
+        <v>Тестирование конфигурации криптографических стандартных алгоритмов (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)</v>
       </c>
       <c r="I31" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#common-configuration-issues-mstg-crypto-1-mstg-crypto-2-and-mstg-crypto-3"),"Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
-        <v>Common Configuration Issues (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#common-configuration-issues-mstg-crypto-1-mstg-crypto-2-and-mstg-crypto-3"),"Общие проблемы конфигурации (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
+        <v>Общие проблемы конфигурации (MSTG-CRYPTO-1, MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
       <c r="J31" s="72"/>
       <c r="K31" s="73"/>
@@ -5322,12 +5322,12 @@
       </c>
       <c r="G32" s="70"/>
       <c r="H32" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#identifying-insecure-andor-deprecated-cryptographic-algorithms-mstg-crypto-4"),"Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)")</f>
-        <v>Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#identifying-insecure-andor-deprecated-cryptographic-algorithms-mstg-crypto-4"),"Поиск небезопасных и/или устаревших криптографических алгоритмов (MSTG-CRYPTO-4)")</f>
+        <v>Поиск небезопасных и/или устаревших криптографических алгоритмов (MSTG-CRYPTO-4)</v>
       </c>
       <c r="I32" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-mstg-crypto-3-and-mstg-crypto-4"),"Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)")</f>
-        <v>Testing the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-mstg-crypto-3-and-mstg-crypto-4"),"Тестирование конфигурации криптографических стандартных алгоритмов (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)")</f>
+        <v>Тестирование конфигурации криптографических стандартных алгоритмов (MSTG-CRYPTO-2, MSTG-CRYPTO-3 and MSTG-CRYPTO-4)</v>
       </c>
       <c r="J32" s="72"/>
       <c r="K32" s="73"/>
@@ -5350,8 +5350,8 @@
       </c>
       <c r="G33" s="70"/>
       <c r="H33" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-key-management-mstg-storage-1-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
-        <v>Testing Key Management (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-key-management-mstg-storage-1-mstg-crypto-1-and-mstg-crypto-5"),"Проверка системы управления ключами (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
+        <v>Проверка системы управления ключами (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
       <c r="I33" s="76"/>
       <c r="J33" s="76"/>
@@ -5375,8 +5375,8 @@
       </c>
       <c r="G34" s="70"/>
       <c r="H34" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-random-number-generation-mstg-crypto-6"),"Testing Random Number Generation (MSTG-CRYPTO-6)")</f>
-        <v>Testing Random Number Generation (MSTG-CRYPTO-6)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-random-number-generation-mstg-crypto-6"),"Проверка системы генерации случайных чисел (MSTG-CRYPTO-6)")</f>
+        <v>Проверка системы генерации случайных чисел (MSTG-CRYPTO-6)</v>
       </c>
       <c r="I34" s="76"/>
       <c r="J34" s="76"/>
@@ -5416,16 +5416,16 @@
       </c>
       <c r="G36" s="70"/>
       <c r="H36" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05f-Testing-Local-Authentication.md#testing-confirm-credentials-mstg-auth-1-and-mstg-storage-11"),"Testing Confirm Credentials (MSTG-AUTH-1 and MSTG-STORAGE-11)")</f>
-        <v>Testing Confirm Credentials (MSTG-AUTH-1 and MSTG-STORAGE-11)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05f-Testing-Local-Authentication.md#testing-confirm-credentials-mstg-auth-1-and-mstg-storage-11"),"Проверка учетных данных (MSTG-AUTH-1 and MSTG-STORAGE-11)")</f>
+        <v>Проверка учетных данных (MSTG-AUTH-1 and MSTG-STORAGE-11)</v>
       </c>
       <c r="I36" s="75" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
-        <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Проверка наличия соответствующей аутентификации (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
+        <v>Проверка наличия соответствующей аутентификации (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
       <c r="J36" s="75" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
-        <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Проверка потоков OAuth 2.0 (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
+        <v>Проверка потоков OAuth 2.0 (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
       <c r="K36" s="73"/>
     </row>
@@ -5447,8 +5447,8 @@
       </c>
       <c r="G37" s="70"/>
       <c r="H37" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateful-session-management-mstg-auth-2"),"Testing Stateful Session Management (MSTG-AUTH-2)")</f>
-        <v>Testing Stateful Session Management (MSTG-AUTH-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateful-session-management-mstg-auth-2"),"Тестирование аутентификации на основе сессии(MSTG-AUTH-2)")</f>
+        <v>Тестирование аутентификации на основе сессии(MSTG-AUTH-2)</v>
       </c>
       <c r="I37" s="76"/>
       <c r="J37" s="76"/>

</xml_diff>

<commit_message>
Android Security Requiments V4 translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -1915,7 +1915,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="161">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2316,7 +2316,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2477,6 +2477,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="28" fillId="0" borderId="19" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2733,7 +2737,342 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike" u="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFillTx/>
+                <a:latin typeface="Trebuchet MS"/>
+                <a:ea typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike" u="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFillTx/>
+                <a:latin typeface="Trebuchet MS"/>
+                <a:ea typeface="Arial"/>
+              </a:rPr>
+              <a:t>Диаграмма соответствия 
+MASVS - iOS</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.648866193526052"/>
+          <c:y val="0.0247349823321555"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25560">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.221438462870002"/>
+          <c:y val="0.112632508833922"/>
+          <c:w val="0.502423403150424"/>
+          <c:h val="0.840768551236749"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:radarChart>
+        <c:radarStyle val="filled"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>"IOS"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IOS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="dddddd"/>
+            </a:solidFill>
+            <a:ln w="25560">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Сводная по ИБ'!$C$43:$C$50</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>V1: Требования к архитектуре, дизайну и модели угроз</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>V2: Требования к конфиденциальности и хранению данных</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>V3: Требования к криптографии</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>V4: Требования к аутентификации и управлению сессиями</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>V5: Требования к сетевому взаимодействию</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>V6: Требования к взаимодействию с операционной системой</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>V7: Требования к качеству кода и настройкам сборки</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>V8: Требования к устойчивости к атакам на стороне клиента</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Сводная по ИБ'!$K$43:$K$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="67702425"/>
+        <c:axId val="63184890"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="67702425"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="3240">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="63184890"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="63184890"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="3240">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.00_);\(#,##0.00\)" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3240">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="67702425"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25560">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.823556052033288"/>
+          <c:y val="0.0867538179349203"/>
+          <c:w val="0.044674738528106"/>
+          <c:h val="0.0390752020396546"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25560">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="845" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:ea typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="6480">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2913,11 +3252,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="20604495"/>
-        <c:axId val="78361298"/>
+        <c:axId val="51309013"/>
+        <c:axId val="45456944"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="20604495"/>
+        <c:axId val="51309013"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2957,7 +3296,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78361298"/>
+        <c:crossAx val="45456944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2965,7 +3304,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78361298"/>
+        <c:axId val="45456944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3008,7 +3347,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20604495"/>
+        <c:crossAx val="51309013"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3029,341 +3368,6 @@
           <c:y val="0.0867538179349203"/>
           <c:w val="0.152253978633294"/>
           <c:h val="0.0463334650736225"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="25560">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="845" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:ea typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="6480">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike" u="sng">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFillTx/>
-                <a:latin typeface="Trebuchet MS"/>
-                <a:ea typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike" u="sng">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFillTx/>
-                <a:latin typeface="Trebuchet MS"/>
-                <a:ea typeface="Arial"/>
-              </a:rPr>
-              <a:t>Диаграмма соответствия 
-MASVS - iOS</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.648866193526052"/>
-          <c:y val="0.0247349823321555"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="25560">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.221438462870002"/>
-          <c:y val="0.112632508833922"/>
-          <c:w val="0.502423403150424"/>
-          <c:h val="0.840768551236749"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:radarChart>
-        <c:radarStyle val="filled"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>"IOS"</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>IOS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="dddddd"/>
-            </a:solidFill>
-            <a:ln w="25560">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                    <a:ea typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Сводная по ИБ'!$C$43:$C$50</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>V1: Требования к архитектуре, дизайну и модели угроз</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>V2: Требования к конфиденциальности и хранению данных</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>V3: Требования к криптографии</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>V4: Требования к аутентификации и управлению сессиями</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>V5: Требования к сетевому взаимодействию</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>V6: Требования к взаимодействию с операционной системой</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>V7: Требования к качеству кода и настройкам сборки</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>V8: Требования к устойчивости к атакам на стороне клиента</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Сводная по ИБ'!$K$43:$K$50</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="28333765"/>
-        <c:axId val="39605995"/>
-      </c:radarChart>
-      <c:catAx>
-        <c:axId val="28333765"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="3240">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="39605995"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="39605995"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="3240">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="#,##0.00_);\(#,##0.00\)" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="3240">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="28333765"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="25560">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.823556052033288"/>
-          <c:y val="0.0867538179349203"/>
-          <c:w val="0.044674738528106"/>
-          <c:h val="0.0390752020396546"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4532,8 +4536,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J37" activeCellId="0" sqref="J37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I40" activeCellId="0" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5472,12 +5476,12 @@
       </c>
       <c r="G38" s="70"/>
       <c r="H38" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateless-token-based-authentication-mstg-auth-3"),"Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)")</f>
-        <v>Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateless-token-based-authentication-mstg-auth-3"),"Тестирование аутентификации на основе токена (MSTG-AUTH-3)")</f>
+        <v>Тестирование аутентификации на основе токена (MSTG-AUTH-3)</v>
       </c>
       <c r="I38" s="75" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
-        <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Проверка потоков OAuth 2.0  (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
+        <v>Проверка потоков OAuth 2.0  (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
       <c r="J38" s="76"/>
       <c r="K38" s="73"/>
@@ -5497,8 +5501,8 @@
       <c r="F39" s="69"/>
       <c r="G39" s="70"/>
       <c r="H39" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-user-logout-mstg-auth-4"),"Testing User Logout (MSTG-AUTH-4)")</f>
-        <v>Testing User Logout (MSTG-AUTH-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-user-logout-mstg-auth-4"),"Тестирование деаутентификации пользователя (MSTG-AUTH-4)")</f>
+        <v>Тестирование деаутентификации пользователя (MSTG-AUTH-4)</v>
       </c>
       <c r="I39" s="76"/>
       <c r="J39" s="76"/>
@@ -5523,8 +5527,8 @@
       </c>
       <c r="G40" s="70"/>
       <c r="H40" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
-        <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Проверка на лучшие практики для пароля (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
+        <v>Проверка на лучшие практики для пароля (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
       <c r="I40" s="76"/>
       <c r="J40" s="76"/>
@@ -5548,12 +5552,12 @@
       </c>
       <c r="G41" s="70"/>
       <c r="H41" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
-        <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Проверка на лучшие практики для пароля (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
+        <v>Проверка на лучшие практики для пароля (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
       <c r="I41" s="75" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#dynamic-testing-mstg-auth-6"),"Dynamic Testing (MSTG-AUTH-6)")</f>
-        <v>Dynamic Testing (MSTG-AUTH-6)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#dynamic-testing-mstg-auth-6"),"Динамическое тестирование (MSTG-AUTH-6)")</f>
+        <v>Динамическое тестирование (MSTG-AUTH-6)</v>
       </c>
       <c r="J41" s="72"/>
       <c r="K41" s="73"/>
@@ -5576,8 +5580,8 @@
       </c>
       <c r="G42" s="70"/>
       <c r="H42" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-session-timeout-mstg-auth-7"),"Testing Session Timeout (MSTG-AUTH-7)")</f>
-        <v>Testing Session Timeout (MSTG-AUTH-7)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-session-timeout-mstg-auth-7"),"Тестирование таймаута сессии (MSTG-AUTH-7)")</f>
+        <v>Тестирование таймаута сессии (MSTG-AUTH-7)</v>
       </c>
       <c r="I42" s="97"/>
       <c r="J42" s="98"/>
@@ -5601,8 +5605,8 @@
         <v>77</v>
       </c>
       <c r="H43" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05f-Testing-Local-Authentication.md#testing-biometric-authentication-mstg-auth-8"),"Testing Biometric Authentication (MSTG-AUTH-8)")</f>
-        <v>Testing Biometric Authentication (MSTG-AUTH-8)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05f-Testing-Local-Authentication.md#testing-biometric-authentication-mstg-auth-8"),"Тестирование биометрической аутентификации (MSTG-AUTH-8)")</f>
+        <v>Тестирование биометрической аутентификации (MSTG-AUTH-8)</v>
       </c>
       <c r="I43" s="76"/>
       <c r="J43" s="72"/>
@@ -5626,8 +5630,8 @@
         <v>77</v>
       </c>
       <c r="H44" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
-        <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Тестирование двухфакторной и повышающей аутентификации(MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
+        <v>Тестирование двухфакторной и повышающей аутентификации(MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
       <c r="I44" s="76"/>
       <c r="J44" s="76"/>
@@ -5651,8 +5655,8 @@
         <v>77</v>
       </c>
       <c r="H45" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
-        <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Тестирование двухфакторной и повышающей аутентификации(MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
+        <v>Тестирование двухфакторной и повышающей аутентификации(MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
       <c r="I45" s="76"/>
       <c r="J45" s="76"/>
@@ -5676,8 +5680,8 @@
         <v>77</v>
       </c>
       <c r="H46" s="100" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-login-activity-and-device-blocking-mstg-auth-11"),"Testing Login Activity and Device Blocking (MSTG-AUTH-11)")</f>
-        <v>Testing Login Activity and Device Blocking (MSTG-AUTH-11)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-login-activity-and-device-blocking-mstg-auth-11"),"Тестирование активности входа и блокировки устройства (MSTG-AUTH-11)")</f>
+        <v>Тестирование активности входа и блокировки устройства (MSTG-AUTH-11)</v>
       </c>
       <c r="I46" s="76"/>
       <c r="J46" s="76"/>
@@ -8128,7 +8132,7 @@
       <c r="G46" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H46" s="100" t="str">
+      <c r="H46" s="141" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04e-Testing-Authentication-and-Session-Management.md#testing-login-activity-and-device-blocking-mstg-auth-11"), "Testing Login Activity and Device Blocking (MSTG-AUTH-11)")</f>
         <v>Testing Login Activity and Device Blocking (MSTG-AUTH-11)</v>
       </c>
@@ -8654,7 +8658,7 @@
         <v>64</v>
       </c>
       <c r="G68" s="70"/>
-      <c r="H68" s="100" t="str">
+      <c r="H68" s="141" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"),"Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
         <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
       </c>
@@ -8771,12 +8775,12 @@
       <c r="G73" s="108"/>
       <c r="H73" s="108"/>
       <c r="I73" s="109"/>
-      <c r="J73" s="141"/>
-      <c r="K73" s="142"/>
+      <c r="J73" s="142"/>
+      <c r="K73" s="143"/>
     </row>
     <row r="74" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="143"/>
-      <c r="C74" s="143"/>
+      <c r="B74" s="144"/>
+      <c r="C74" s="144"/>
       <c r="D74" s="92"/>
       <c r="E74" s="114"/>
       <c r="F74" s="114"/>
@@ -8787,8 +8791,8 @@
       <c r="K74" s="92"/>
     </row>
     <row r="75" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="143"/>
-      <c r="C75" s="143"/>
+      <c r="B75" s="144"/>
+      <c r="C75" s="144"/>
       <c r="D75" s="92"/>
       <c r="E75" s="114"/>
       <c r="F75" s="114"/>
@@ -8799,8 +8803,8 @@
       <c r="K75" s="92"/>
     </row>
     <row r="76" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="143"/>
-      <c r="C76" s="143"/>
+      <c r="B76" s="144"/>
+      <c r="C76" s="144"/>
       <c r="D76" s="92"/>
       <c r="E76" s="114"/>
       <c r="F76" s="114"/>
@@ -8889,8 +8893,8 @@
       <c r="K81" s="92"/>
     </row>
     <row r="82" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="143"/>
-      <c r="C82" s="143"/>
+      <c r="B82" s="144"/>
+      <c r="C82" s="144"/>
       <c r="D82" s="92"/>
       <c r="E82" s="114"/>
       <c r="F82" s="114"/>
@@ -8901,8 +8905,8 @@
       <c r="K82" s="92"/>
     </row>
     <row r="83" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="143"/>
-      <c r="C83" s="143"/>
+      <c r="B83" s="144"/>
+      <c r="C83" s="144"/>
       <c r="D83" s="92"/>
       <c r="E83" s="114"/>
       <c r="F83" s="114"/>
@@ -8913,8 +8917,8 @@
       <c r="K83" s="92"/>
     </row>
     <row r="84" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="143"/>
-      <c r="C84" s="143"/>
+      <c r="B84" s="144"/>
+      <c r="C84" s="144"/>
       <c r="D84" s="92"/>
       <c r="E84" s="114"/>
       <c r="F84" s="114"/>
@@ -8925,8 +8929,8 @@
       <c r="K84" s="92"/>
     </row>
     <row r="85" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="143"/>
-      <c r="C85" s="143"/>
+      <c r="B85" s="144"/>
+      <c r="C85" s="144"/>
       <c r="D85" s="92"/>
       <c r="E85" s="114"/>
       <c r="F85" s="114"/>
@@ -9135,7 +9139,7 @@
       <c r="F8" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="144" t="s">
+      <c r="G8" s="145" t="s">
         <v>301</v>
       </c>
       <c r="H8" s="125"/>
@@ -9156,7 +9160,7 @@
       <c r="F9" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G9" s="144" t="s">
+      <c r="G9" s="145" t="s">
         <v>301</v>
       </c>
       <c r="H9" s="125"/>
@@ -9177,7 +9181,7 @@
       <c r="F10" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="144" t="s">
+      <c r="G10" s="145" t="s">
         <v>301</v>
       </c>
       <c r="H10" s="125"/>
@@ -9240,7 +9244,7 @@
       <c r="F13" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="144" t="s">
+      <c r="G13" s="145" t="s">
         <v>301</v>
       </c>
       <c r="H13" s="125"/>
@@ -9305,7 +9309,7 @@
       <c r="F17" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="145" t="str">
+      <c r="G17" s="146" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks-mstg-resilience-3-and-mstg-resilience-11"),"File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)")</f>
         <v>File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)</v>
       </c>
@@ -9342,8 +9346,8 @@
       <c r="H19" s="110"/>
     </row>
     <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="143"/>
-      <c r="C20" s="143"/>
+      <c r="B20" s="144"/>
+      <c r="C20" s="144"/>
       <c r="D20" s="92"/>
       <c r="E20" s="114"/>
       <c r="F20" s="114"/>
@@ -9351,8 +9355,8 @@
       <c r="H20" s="92"/>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="143"/>
-      <c r="C21" s="143"/>
+      <c r="B21" s="144"/>
+      <c r="C21" s="144"/>
       <c r="D21" s="92"/>
       <c r="E21" s="114"/>
       <c r="F21" s="114"/>
@@ -9423,8 +9427,8 @@
       <c r="H26" s="92"/>
     </row>
     <row r="27" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="143"/>
-      <c r="C27" s="143"/>
+      <c r="B27" s="144"/>
+      <c r="C27" s="144"/>
       <c r="D27" s="92"/>
       <c r="E27" s="114"/>
       <c r="F27" s="114"/>
@@ -9432,8 +9436,8 @@
       <c r="H27" s="92"/>
     </row>
     <row r="28" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="143"/>
-      <c r="C28" s="143"/>
+      <c r="B28" s="144"/>
+      <c r="C28" s="144"/>
       <c r="D28" s="92"/>
       <c r="E28" s="114"/>
       <c r="F28" s="114"/>
@@ -9441,8 +9445,8 @@
       <c r="H28" s="92"/>
     </row>
     <row r="29" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="143"/>
-      <c r="C29" s="143"/>
+      <c r="B29" s="144"/>
+      <c r="C29" s="144"/>
       <c r="D29" s="92"/>
       <c r="E29" s="114"/>
       <c r="F29" s="114"/>
@@ -9450,22 +9454,22 @@
       <c r="H29" s="92"/>
     </row>
     <row r="30" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="143"/>
-      <c r="C30" s="143"/>
+      <c r="B30" s="144"/>
+      <c r="C30" s="144"/>
       <c r="D30" s="92"/>
       <c r="E30" s="114"/>
       <c r="F30" s="114"/>
     </row>
     <row r="31" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="143"/>
-      <c r="C31" s="143"/>
+      <c r="B31" s="144"/>
+      <c r="C31" s="144"/>
       <c r="D31" s="92"/>
       <c r="E31" s="114"/>
       <c r="F31" s="114"/>
     </row>
     <row r="32" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="143"/>
-      <c r="C32" s="143"/>
+      <c r="B32" s="144"/>
+      <c r="C32" s="144"/>
       <c r="D32" s="92"/>
       <c r="E32" s="114"/>
       <c r="F32" s="114"/>
@@ -9546,412 +9550,412 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="147" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="147"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="148"/>
       <c r="D1" s="52"/>
       <c r="E1" s="52"/>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="149" t="s">
         <v>319</v>
       </c>
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="149" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="148" t="s">
+      <c r="C2" s="149" t="s">
         <v>321</v>
       </c>
-      <c r="D2" s="148" t="s">
+      <c r="D2" s="149" t="s">
         <v>322</v>
       </c>
-      <c r="E2" s="148" t="s">
+      <c r="E2" s="149" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="149" t="s">
+      <c r="A3" s="150" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="150" t="n">
+      <c r="B3" s="151" t="n">
         <v>0.1</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="151" t="n">
+      <c r="C3" s="151"/>
+      <c r="D3" s="152" t="n">
         <v>42765</v>
       </c>
-      <c r="E3" s="152" t="s">
+      <c r="E3" s="153" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="152" t="s">
+      <c r="A4" s="153" t="s">
         <v>325</v>
       </c>
-      <c r="B4" s="150" t="n">
+      <c r="B4" s="151" t="n">
         <v>0.2</v>
       </c>
-      <c r="C4" s="150"/>
-      <c r="D4" s="151" t="n">
+      <c r="C4" s="151"/>
+      <c r="D4" s="152" t="n">
         <v>42766</v>
       </c>
-      <c r="E4" s="152" t="s">
+      <c r="E4" s="153" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="152" t="s">
+      <c r="A5" s="153" t="s">
         <v>327</v>
       </c>
-      <c r="B5" s="150" t="n">
+      <c r="B5" s="151" t="n">
         <v>0.3</v>
       </c>
-      <c r="C5" s="150"/>
-      <c r="D5" s="151" t="n">
+      <c r="C5" s="151"/>
+      <c r="D5" s="152" t="n">
         <v>42778</v>
       </c>
-      <c r="E5" s="152" t="s">
+      <c r="E5" s="153" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="152" t="s">
+      <c r="A6" s="153" t="s">
         <v>329</v>
       </c>
-      <c r="B6" s="150" t="s">
+      <c r="B6" s="151" t="s">
         <v>330</v>
       </c>
-      <c r="C6" s="150"/>
-      <c r="D6" s="151" t="n">
+      <c r="C6" s="151"/>
+      <c r="D6" s="152" t="n">
         <v>42780</v>
       </c>
-      <c r="E6" s="152" t="s">
+      <c r="E6" s="153" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="152" t="s">
+      <c r="A7" s="153" t="s">
         <v>325</v>
       </c>
-      <c r="B7" s="153" t="s">
+      <c r="B7" s="154" t="s">
         <v>332</v>
       </c>
-      <c r="C7" s="153"/>
-      <c r="D7" s="151" t="n">
+      <c r="C7" s="154"/>
+      <c r="D7" s="152" t="n">
         <v>42781</v>
       </c>
-      <c r="E7" s="152" t="s">
+      <c r="E7" s="153" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="152" t="s">
+      <c r="A8" s="153" t="s">
         <v>329</v>
       </c>
-      <c r="B8" s="153" t="s">
+      <c r="B8" s="154" t="s">
         <v>334</v>
       </c>
-      <c r="C8" s="153"/>
-      <c r="D8" s="151" t="n">
+      <c r="C8" s="154"/>
+      <c r="D8" s="152" t="n">
         <v>42829</v>
       </c>
-      <c r="E8" s="152" t="s">
+      <c r="E8" s="153" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="152" t="s">
+      <c r="A9" s="153" t="s">
         <v>325</v>
       </c>
-      <c r="B9" s="153" t="s">
+      <c r="B9" s="154" t="s">
         <v>334</v>
       </c>
-      <c r="C9" s="153"/>
-      <c r="D9" s="151" t="n">
+      <c r="C9" s="154"/>
+      <c r="D9" s="152" t="n">
         <v>42919</v>
       </c>
-      <c r="E9" s="152" t="s">
+      <c r="E9" s="153" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="152" t="s">
+      <c r="A10" s="153" t="s">
         <v>325</v>
       </c>
-      <c r="B10" s="153" t="s">
+      <c r="B10" s="154" t="s">
         <v>337</v>
       </c>
-      <c r="C10" s="153"/>
-      <c r="D10" s="151" t="n">
+      <c r="C10" s="154"/>
+      <c r="D10" s="152" t="n">
         <v>42963</v>
       </c>
-      <c r="E10" s="152" t="s">
+      <c r="E10" s="153" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="152" t="s">
+      <c r="A11" s="153" t="s">
         <v>325</v>
       </c>
-      <c r="B11" s="153" t="s">
+      <c r="B11" s="154" t="s">
         <v>339</v>
       </c>
-      <c r="C11" s="153"/>
-      <c r="D11" s="151" t="n">
+      <c r="C11" s="154"/>
+      <c r="D11" s="152" t="n">
         <v>43113</v>
       </c>
-      <c r="E11" s="152" t="s">
+      <c r="E11" s="153" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="152" t="s">
+      <c r="A12" s="153" t="s">
         <v>325</v>
       </c>
-      <c r="B12" s="153" t="n">
+      <c r="B12" s="154" t="n">
         <v>1.1</v>
       </c>
-      <c r="C12" s="153"/>
-      <c r="D12" s="151" t="n">
+      <c r="C12" s="154"/>
+      <c r="D12" s="152" t="n">
         <v>43289</v>
       </c>
-      <c r="E12" s="152" t="s">
+      <c r="E12" s="153" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="152" t="s">
+      <c r="A13" s="153" t="s">
         <v>342</v>
       </c>
-      <c r="B13" s="154" t="s">
+      <c r="B13" s="155" t="s">
         <v>343</v>
       </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="151" t="n">
+      <c r="C13" s="156"/>
+      <c r="D13" s="152" t="n">
         <v>43464</v>
       </c>
-      <c r="E13" s="156" t="s">
+      <c r="E13" s="157" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="152" t="s">
+      <c r="A14" s="153" t="s">
         <v>345</v>
       </c>
-      <c r="B14" s="154" t="s">
+      <c r="B14" s="155" t="s">
         <v>346</v>
       </c>
-      <c r="C14" s="155"/>
-      <c r="D14" s="151" t="n">
+      <c r="C14" s="156"/>
+      <c r="D14" s="152" t="n">
         <v>43469</v>
       </c>
-      <c r="E14" s="156" t="s">
+      <c r="E14" s="157" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="409.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="157" t="s">
+      <c r="A15" s="158" t="s">
         <v>347</v>
       </c>
-      <c r="B15" s="153" t="s">
+      <c r="B15" s="154" t="s">
         <v>348</v>
       </c>
-      <c r="C15" s="153" t="s">
+      <c r="C15" s="154" t="s">
         <v>349</v>
       </c>
-      <c r="D15" s="151" t="n">
+      <c r="D15" s="152" t="n">
         <v>43471</v>
       </c>
-      <c r="E15" s="158" t="s">
+      <c r="E15" s="159" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="152" t="s">
+      <c r="A16" s="153" t="s">
         <v>342</v>
       </c>
-      <c r="B16" s="154" t="s">
+      <c r="B16" s="155" t="s">
         <v>351</v>
       </c>
-      <c r="C16" s="153" t="s">
+      <c r="C16" s="154" t="s">
         <v>349</v>
       </c>
-      <c r="D16" s="159" t="n">
+      <c r="D16" s="160" t="n">
         <v>43475</v>
       </c>
-      <c r="E16" s="156" t="s">
+      <c r="E16" s="157" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="78" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="157" t="s">
+      <c r="A17" s="158" t="s">
         <v>347</v>
       </c>
-      <c r="B17" s="154" t="s">
+      <c r="B17" s="155" t="s">
         <v>353</v>
       </c>
-      <c r="C17" s="153" t="s">
+      <c r="C17" s="154" t="s">
         <v>349</v>
       </c>
-      <c r="D17" s="151" t="n">
+      <c r="D17" s="152" t="n">
         <v>43476</v>
       </c>
-      <c r="E17" s="157" t="s">
+      <c r="E17" s="158" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="157" t="s">
+      <c r="A18" s="158" t="s">
         <v>347</v>
       </c>
-      <c r="B18" s="154" t="s">
+      <c r="B18" s="155" t="s">
         <v>355</v>
       </c>
-      <c r="C18" s="153" t="s">
+      <c r="C18" s="154" t="s">
         <v>349</v>
       </c>
-      <c r="D18" s="151" t="n">
+      <c r="D18" s="152" t="n">
         <v>43478</v>
       </c>
-      <c r="E18" s="157" t="s">
+      <c r="E18" s="158" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="158" t="s">
         <v>347</v>
       </c>
-      <c r="B19" s="154" t="s">
+      <c r="B19" s="155" t="s">
         <v>357</v>
       </c>
-      <c r="C19" s="153" t="s">
+      <c r="C19" s="154" t="s">
         <v>349</v>
       </c>
-      <c r="D19" s="151" t="n">
+      <c r="D19" s="152" t="n">
         <v>43478</v>
       </c>
-      <c r="E19" s="157" t="s">
+      <c r="E19" s="158" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="109.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="157" t="s">
+      <c r="A20" s="158" t="s">
         <v>342</v>
       </c>
-      <c r="B20" s="154" t="s">
+      <c r="B20" s="155" t="s">
         <v>359</v>
       </c>
-      <c r="C20" s="153" t="s">
+      <c r="C20" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="151" t="n">
+      <c r="D20" s="152" t="n">
         <v>43641</v>
       </c>
-      <c r="E20" s="158" t="s">
+      <c r="E20" s="159" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="157" t="s">
+      <c r="A21" s="158" t="s">
         <v>342</v>
       </c>
-      <c r="B21" s="154" t="s">
+      <c r="B21" s="155" t="s">
         <v>361</v>
       </c>
-      <c r="C21" s="153" t="s">
+      <c r="C21" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="151" t="n">
+      <c r="D21" s="152" t="n">
         <v>43642</v>
       </c>
-      <c r="E21" s="157" t="s">
+      <c r="E21" s="158" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="157" t="s">
+      <c r="A22" s="158" t="s">
         <v>342</v>
       </c>
-      <c r="B22" s="154" t="s">
+      <c r="B22" s="155" t="s">
         <v>363</v>
       </c>
-      <c r="C22" s="153" t="s">
+      <c r="C22" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="151" t="n">
+      <c r="D22" s="152" t="n">
         <v>43649</v>
       </c>
-      <c r="E22" s="157" t="s">
+      <c r="E22" s="158" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="157" t="s">
+      <c r="A23" s="158" t="s">
         <v>342</v>
       </c>
-      <c r="B23" s="154" t="s">
+      <c r="B23" s="155" t="s">
         <v>363</v>
       </c>
-      <c r="C23" s="153" t="s">
+      <c r="C23" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="151" t="n">
+      <c r="D23" s="152" t="n">
         <v>43672</v>
       </c>
-      <c r="E23" s="157" t="s">
+      <c r="E23" s="158" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="157" t="s">
+      <c r="A24" s="158" t="s">
         <v>342</v>
       </c>
-      <c r="B24" s="154" t="s">
+      <c r="B24" s="155" t="s">
         <v>363</v>
       </c>
-      <c r="C24" s="153" t="s">
+      <c r="C24" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="151" t="n">
+      <c r="D24" s="152" t="n">
         <v>43674</v>
       </c>
-      <c r="E24" s="157" t="s">
+      <c r="E24" s="158" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="157" t="s">
+      <c r="A25" s="158" t="s">
         <v>342</v>
       </c>
-      <c r="B25" s="154" t="s">
+      <c r="B25" s="155" t="s">
         <v>367</v>
       </c>
-      <c r="C25" s="153" t="s">
+      <c r="C25" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="151" t="n">
+      <c r="D25" s="152" t="n">
         <v>43685</v>
       </c>
-      <c r="E25" s="157" t="s">
+      <c r="E25" s="158" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="157" t="s">
+      <c r="A26" s="158" t="s">
         <v>369</v>
       </c>
-      <c r="B26" s="154" t="s">
+      <c r="B26" s="155" t="s">
         <v>367</v>
       </c>
-      <c r="C26" s="153" t="s">
+      <c r="C26" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="151" t="n">
+      <c r="D26" s="152" t="n">
         <v>43719</v>
       </c>
-      <c r="E26" s="157" t="s">
+      <c r="E26" s="158" t="s">
         <v>370</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Android Security Requiments V5 translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -2737,7 +2737,342 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike" u="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFillTx/>
+                <a:latin typeface="Trebuchet MS"/>
+                <a:ea typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike" u="sng">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFillTx/>
+                <a:latin typeface="Trebuchet MS"/>
+                <a:ea typeface="Arial"/>
+              </a:rPr>
+              <a:t>Диаграмма соотвествия 
+MASVS - Android</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.717146540610228"/>
+          <c:y val="0.0138940211366492"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25560">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.221443919209282"/>
+          <c:y val="0.112630256448156"/>
+          <c:w val="0.502449505801461"/>
+          <c:h val="0.840736087502771"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:radarChart>
+        <c:radarStyle val="filled"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>"Android"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Android</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="c0c0c0"/>
+            </a:solidFill>
+            <a:ln w="25560">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Сводная по ИБ'!$C$43:$C$50</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>V1: Требования к архитектуре, дизайну и модели угроз</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>V2: Требования к конфиденциальности и хранению данных</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>V3: Требования к криптографии</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>V4: Требования к аутентификации и управлению сессиями</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>V5: Требования к сетевому взаимодействию</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>V6: Требования к взаимодействию с операционной системой</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>V7: Требования к качеству кода и настройкам сборки</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>V8: Требования к устойчивости к атакам на стороне клиента</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Сводная по ИБ'!$G$43:$G$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="31503159"/>
+        <c:axId val="31365405"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="31503159"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="3240">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="31365405"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="31365405"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="3240">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.00_);\(#,##0.00\)" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3240">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="31503159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25560">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.823556052033288"/>
+          <c:y val="0.0867538179349203"/>
+          <c:w val="0.152253978633294"/>
+          <c:h val="0.0463334650736225"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25560">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="845" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:ea typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="6480">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2917,11 +3252,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="67702425"/>
-        <c:axId val="63184890"/>
+        <c:axId val="56071732"/>
+        <c:axId val="85545846"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="67702425"/>
+        <c:axId val="56071732"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2961,7 +3296,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63184890"/>
+        <c:crossAx val="85545846"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2969,7 +3304,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63184890"/>
+        <c:axId val="85545846"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3012,7 +3347,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67702425"/>
+        <c:crossAx val="56071732"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3033,341 +3368,6 @@
           <c:y val="0.0867538179349203"/>
           <c:w val="0.044674738528106"/>
           <c:h val="0.0390752020396546"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="25560">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="845" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:ea typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="6480">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="1" sz="1300" spc="-1" strike="noStrike" u="sng">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFillTx/>
-                <a:latin typeface="Trebuchet MS"/>
-                <a:ea typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="1" sz="1300" spc="-1" strike="noStrike" u="sng">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFillTx/>
-                <a:latin typeface="Trebuchet MS"/>
-                <a:ea typeface="Arial"/>
-              </a:rPr>
-              <a:t>Диаграмма соотвествия 
-MASVS - Android</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.717146540610228"/>
-          <c:y val="0.0138940211366492"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="25560">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.221443919209282"/>
-          <c:y val="0.112630256448156"/>
-          <c:w val="0.502449505801461"/>
-          <c:h val="0.840736087502771"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:radarChart>
-        <c:radarStyle val="filled"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>"Android"</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Android</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="c0c0c0"/>
-            </a:solidFill>
-            <a:ln w="25560">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                    <a:ea typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Сводная по ИБ'!$C$43:$C$50</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>V1: Требования к архитектуре, дизайну и модели угроз</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>V2: Требования к конфиденциальности и хранению данных</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>V3: Требования к криптографии</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>V4: Требования к аутентификации и управлению сессиями</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>V5: Требования к сетевому взаимодействию</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>V6: Требования к взаимодействию с операционной системой</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>V7: Требования к качеству кода и настройкам сборки</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>V8: Требования к устойчивости к атакам на стороне клиента</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Сводная по ИБ'!$G$43:$G$50</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="51309013"/>
-        <c:axId val="45456944"/>
-      </c:radarChart>
-      <c:catAx>
-        <c:axId val="51309013"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="3240">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="45456944"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="45456944"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="3240">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="#,##0.00_);\(#,##0.00\)" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="3240">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="51309013"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="25560">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.823556052033288"/>
-          <c:y val="0.0867538179349203"/>
-          <c:w val="0.152253978633294"/>
-          <c:h val="0.0463334650736225"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4537,7 +4537,7 @@
   <dimension ref="B1:M85"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I40" activeCellId="0" sqref="I40"/>
+      <selection pane="topLeft" activeCell="I53" activeCellId="0" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5721,8 +5721,8 @@
       </c>
       <c r="G48" s="70"/>
       <c r="H48" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
-        <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Проверка шифрования данных в сети (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
+        <v>Проверка шифрования данных в сети (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
       <c r="I48" s="76"/>
       <c r="J48" s="76"/>
@@ -5746,8 +5746,8 @@
       </c>
       <c r="G49" s="70"/>
       <c r="H49" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
-        <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Проверка шифрования данных в сети (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
+        <v>Проверка шифрования данных в сети (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
       <c r="I49" s="76"/>
       <c r="J49" s="76"/>
@@ -5771,8 +5771,8 @@
       </c>
       <c r="G50" s="70"/>
       <c r="H50" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-endpoint-identify-verification-mstg-network-3"),"Testing Endpoint Identify Verification (MSTG-NETWORK-3)")</f>
-        <v>Testing Endpoint Identify Verification (MSTG-NETWORK-3)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-endpoint-identify-verification-mstg-network-3"),"Проверка идентификации конечной точки (MSTG-NETWORK-3)")</f>
+        <v>Проверка идентификации конечной точки (MSTG-NETWORK-3)</v>
       </c>
       <c r="I50" s="75"/>
       <c r="J50" s="101"/>
@@ -5796,12 +5796,12 @@
         <v>77</v>
       </c>
       <c r="H51" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-4)")</f>
-        <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-4"),"Тестирование пользовательских хранилищ сертификатов и сохраненных сертификатов (MSTG-NETWORK-4)")</f>
+        <v>Тестирование пользовательских хранилищ сертификатов и сохраненных сертификатов (MSTG-NETWORK-4)</v>
       </c>
       <c r="I51" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-the-network-security-configuration-settings-mstg-network-4"),"Testing the Network Security Configuration Settings (MSTG-NETWORK-4)")</f>
-        <v>Testing the Network Security Configuration Settings (MSTG-NETWORK-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-the-network-security-configuration-settings-mstg-network-4"),"Тестирование настроек конфигурации безопасности сети (MSTG-NETWORK-4)")</f>
+        <v>Тестирование настроек конфигурации безопасности сети (MSTG-NETWORK-4)</v>
       </c>
       <c r="J51" s="72"/>
       <c r="K51" s="73"/>
@@ -5824,8 +5824,8 @@
         <v>77</v>
       </c>
       <c r="H52" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels-mstg-network-5"),"Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)")</f>
-        <v>Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels-mstg-network-5"),"Убедитесь, что для критических операций используются безопасные каналы связи (MSTG-NETWORK-5)")</f>
+        <v>Убедитесь, что для критических операций используются безопасные каналы связи (MSTG-NETWORK-5)</v>
       </c>
       <c r="I52" s="76"/>
       <c r="J52" s="76"/>
@@ -5849,8 +5849,8 @@
         <v>77</v>
       </c>
       <c r="H53" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-the-security-provider-mstg-network-6"),"Testing the Security Provider (MSTG-NETWORK-6)")</f>
-        <v>Testing the Security Provider (MSTG-NETWORK-6)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-the-security-provider-mstg-network-6"),"Тестирование провайдера безопасности (MSTG-NETWORK-6)")</f>
+        <v>Тестирование провайдера безопасности (MSTG-NETWORK-6)</v>
       </c>
       <c r="I53" s="76"/>
       <c r="J53" s="76"/>

</xml_diff>

<commit_message>
Android Security Requiments translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -2737,7 +2737,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2917,11 +2917,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="31503159"/>
-        <c:axId val="31365405"/>
+        <c:axId val="41684188"/>
+        <c:axId val="78735704"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="31503159"/>
+        <c:axId val="41684188"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2961,7 +2961,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31365405"/>
+        <c:crossAx val="78735704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2969,7 +2969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31365405"/>
+        <c:axId val="78735704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3012,7 +3012,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31503159"/>
+        <c:crossAx val="41684188"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3072,7 +3072,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3252,11 +3252,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="56071732"/>
-        <c:axId val="85545846"/>
+        <c:axId val="94397152"/>
+        <c:axId val="93741098"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="56071732"/>
+        <c:axId val="94397152"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3296,7 +3296,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85545846"/>
+        <c:crossAx val="93741098"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3304,7 +3304,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85545846"/>
+        <c:axId val="93741098"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3347,7 +3347,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56071732"/>
+        <c:crossAx val="94397152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4536,8 +4536,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I53" activeCellId="0" sqref="I53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A85" activeCellId="0" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5890,8 +5890,8 @@
       </c>
       <c r="G55" s="70"/>
       <c r="H55" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-app-permissions-mstg-platform-1"),"Testing App Permissions (MSTG-PLATFORM-1)")</f>
-        <v>Testing App Permissions (MSTG-PLATFORM-1)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-app-permissions-mstg-platform-1"),"Проверка разрешений приложения (MSTG-PLATFORM-1)")</f>
+        <v>Проверка разрешений приложения (MSTG-PLATFORM-1)</v>
       </c>
       <c r="I55" s="76"/>
       <c r="J55" s="76"/>
@@ -5915,12 +5915,12 @@
       </c>
       <c r="G56" s="70"/>
       <c r="H56" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#testing-for-injection-flaws-mstg-platform-2"),"Testing for Injection Flaws (MSTG-PLATFORM-2)")</f>
-        <v>Testing for Injection Flaws (MSTG-PLATFORM-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#testing-for-injection-flaws-mstg-platform-2"),"Проверка на инъекции (MSTG-PLATFORM-2)")</f>
+        <v>Проверка на инъекции (MSTG-PLATFORM-2)</v>
       </c>
       <c r="I56" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#testing-for-fragment-injection-mstg-platform-2"),"Testing for Fragment Injection (MSTG-PLATFORM-2)")</f>
-        <v>Testing for Fragment Injection (MSTG-PLATFORM-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#testing-for-fragment-injection-mstg-platform-2"),"Проверка инъекции фрагмента (MSTG-PLATFORM-2)")</f>
+        <v>Проверка инъекции фрагмента (MSTG-PLATFORM-2)</v>
       </c>
       <c r="J56" s="72"/>
       <c r="K56" s="73"/>
@@ -5943,8 +5943,8 @@
       </c>
       <c r="G57" s="70"/>
       <c r="H57" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-custom-url-schemes-mstg-platform-3"),"Testing Custom URL Schemes (MSTG-PLATFORM-3)")</f>
-        <v>Testing Custom URL Schemes (MSTG-PLATFORM-3)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-custom-url-schemes-mstg-platform-3"),"Тестирование пользовательских схем URL (MSTG-PLATFORM-3)")</f>
+        <v>Тестирование пользовательских схем URL (MSTG-PLATFORM-3)</v>
       </c>
       <c r="I57" s="76"/>
       <c r="J57" s="76"/>
@@ -5968,8 +5968,8 @@
       </c>
       <c r="G58" s="70"/>
       <c r="H58" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-for-sensitive-functionality-exposure-through-ipc-mstg-platform-4"),"Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)")</f>
-        <v>Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-for-sensitive-functionality-exposure-through-ipc-mstg-platform-4"),"Проверка передачи конфиденциальных данных при обмене данными между потоками (IPC) (MSTG-PLATFORM-4)")</f>
+        <v>Проверка передачи конфиденциальных данных при обмене данными между потоками (IPC) (MSTG-PLATFORM-4)</v>
       </c>
       <c r="I58" s="76"/>
       <c r="J58" s="76"/>
@@ -5993,8 +5993,8 @@
       </c>
       <c r="G59" s="70"/>
       <c r="H59" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-javascript-execution-in-webviews-mstg-platform-5"),"Testing JavaScript Execution in WebViews (MSTG-PLATFORM-5)")</f>
-        <v>Testing JavaScript Execution in WebViews (MSTG-PLATFORM-5)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-javascript-execution-in-webviews-mstg-platform-5"),"Проверка исполнения JavaScript-кода в WebViews (MSTG-PLATFORM-5)")</f>
+        <v>Проверка исполнения JavaScript-кода в WebViews (MSTG-PLATFORM-5)</v>
       </c>
       <c r="I59" s="76"/>
       <c r="J59" s="76"/>
@@ -6018,8 +6018,8 @@
       </c>
       <c r="G60" s="70"/>
       <c r="H60" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-webview-protocol-handlers-mstg-platform-6"),"Testing WebView Protocol Handlers (MSTG-PLATFORM-6)")</f>
-        <v>Testing WebView Protocol Handlers (MSTG-PLATFORM-6)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-webview-protocol-handlers-mstg-platform-6"),"Тестирование обработчиков протокола WebView (MSTG-PLATFORM-6)")</f>
+        <v>Тестирование обработчиков протокола WebView (MSTG-PLATFORM-6)</v>
       </c>
       <c r="I60" s="76"/>
       <c r="J60" s="76"/>
@@ -6043,8 +6043,8 @@
       </c>
       <c r="G61" s="70"/>
       <c r="H61" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#determining-whether-java-objects-are-exposed-through-webviews-mstg-platform-7"),"Determining Whether Java Objects Are Exposed Through WebViews (MSTG-PLATFORM-7)")</f>
-        <v>Determining Whether Java Objects Are Exposed Through WebViews (MSTG-PLATFORM-7)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#determining-whether-java-objects-are-exposed-through-webviews-mstg-platform-7"),"Проверка на раскрытие Java-объектов в WebViews (MSTG-PLATFORM-7)")</f>
+        <v>Проверка на раскрытие Java-объектов в WebViews (MSTG-PLATFORM-7)</v>
       </c>
       <c r="I61" s="76"/>
       <c r="J61" s="76"/>
@@ -6068,8 +6068,8 @@
       </c>
       <c r="G62" s="70"/>
       <c r="H62" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-object-persistence-mstg-platform-8"),"Testing Object Persistence (MSTG-PLATFORM-8)")</f>
-        <v>Testing Object Persistence (MSTG-PLATFORM-8)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05h-Testing-Platform-Interaction.md#testing-object-persistence-mstg-platform-8"),"Стабильность объекта тестирования (MSTG-PLATFORM-8)")</f>
+        <v>Стабильность объекта тестирования (MSTG-PLATFORM-8)</v>
       </c>
       <c r="I62" s="76"/>
       <c r="J62" s="76"/>
@@ -6109,8 +6109,8 @@
       </c>
       <c r="G64" s="70"/>
       <c r="H64" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#making-sure-that-the-app-is-properly-signed-mstg-code-1"),"Making Sure That the App is Properly Signed (MSTG-CODE-1)")</f>
-        <v>Making Sure That the App is Properly Signed (MSTG-CODE-1)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#making-sure-that-the-app-is-properly-signed-mstg-code-1"),"Убедитесь, что приложение правильно подписано (MSTG-CODE-1)")</f>
+        <v>Убедитесь, что приложение правильно подписано (MSTG-CODE-1)</v>
       </c>
       <c r="I64" s="76"/>
       <c r="J64" s="76"/>
@@ -6134,8 +6134,8 @@
       </c>
       <c r="G65" s="70"/>
       <c r="H65" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-whether-the-app-is-debuggable-mstg-code-2"),"Testing Whether the App is Debuggable (MSTG-CODE-2)")</f>
-        <v>Testing Whether the App is Debuggable (MSTG-CODE-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-whether-the-app-is-debuggable-mstg-code-2"),"Проверка включенного debug-режима(MSTG-CODE-2)")</f>
+        <v>Проверка включенного debug-режима(MSTG-CODE-2)</v>
       </c>
       <c r="I65" s="76"/>
       <c r="J65" s="76"/>
@@ -6159,8 +6159,8 @@
       </c>
       <c r="G66" s="70"/>
       <c r="H66" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-for-debugging-symbols-mstg-code-3"),"Testing for Debugging Symbols (MSTG-CODE-3)")</f>
-        <v>Testing for Debugging Symbols (MSTG-CODE-3)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-for-debugging-symbols-mstg-code-3"),"Проверка отладочных символов (MSTG-CODE-3)")</f>
+        <v>Проверка отладочных символов (MSTG-CODE-3)</v>
       </c>
       <c r="I66" s="76"/>
       <c r="J66" s="76"/>
@@ -6184,8 +6184,8 @@
       </c>
       <c r="G67" s="70"/>
       <c r="H67" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-for-debugging-code-and-verbose-error-logging-mstg-code-4"),"Testing for Debugging Code and Verbose Error Logging (MSTG-CODE-4)")</f>
-        <v>Testing for Debugging Code and Verbose Error Logging (MSTG-CODE-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-for-debugging-code-and-verbose-error-logging-mstg-code-4"),"Проверка наличия отладочного кода и расширенного логгирования (MSTG-CODE-4)")</f>
+        <v>Проверка наличия отладочного кода и расширенного логгирования (MSTG-CODE-4)</v>
       </c>
       <c r="I67" s="76"/>
       <c r="J67" s="76"/>
@@ -6209,8 +6209,8 @@
       </c>
       <c r="G68" s="70"/>
       <c r="H68" s="100" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"),"Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
-        <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"),"Проверка уязвимостей в сторонних библиотеках (MSTG-CODE-5)")</f>
+        <v>Проверка уязвимостей в сторонних библиотеках (MSTG-CODE-5)</v>
       </c>
       <c r="I68" s="76"/>
       <c r="J68" s="76"/>
@@ -6234,8 +6234,8 @@
       </c>
       <c r="G69" s="70"/>
       <c r="H69" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6-and-mstg-code-7"),"Testing Exception Handling (MSTG-CODE-6 and MSTG-CODE-7)")</f>
-        <v>Testing Exception Handling (MSTG-CODE-6 and MSTG-CODE-7)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6-and-mstg-code-7"),"Тестирование обработки исключений (MSTG-CODE-6 and MSTG-CODE-7)")</f>
+        <v>Тестирование обработки исключений (MSTG-CODE-6 and MSTG-CODE-7)</v>
       </c>
       <c r="I69" s="76"/>
       <c r="J69" s="76"/>
@@ -6259,8 +6259,8 @@
       </c>
       <c r="G70" s="70"/>
       <c r="H70" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6-and-mstg-code-7"),"Testing Exception Handling (MSTG-CODE-6 and MSTG-CODE-7)")</f>
-        <v>Testing Exception Handling (MSTG-CODE-6 and MSTG-CODE-7)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6-and-mstg-code-7"),"Тестирование обработки исключений (MSTG-CODE-6 and MSTG-CODE-7)")</f>
+        <v>Тестирование обработки исключений (MSTG-CODE-6 and MSTG-CODE-7)</v>
       </c>
       <c r="I70" s="76"/>
       <c r="J70" s="76"/>
@@ -6284,8 +6284,8 @@
       </c>
       <c r="G71" s="70"/>
       <c r="H71" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#memory-corruption-bugs-mstg-code-8"),"Memory Corruption Bugs (MSTG-CODE-8)")</f>
-        <v>Memory Corruption Bugs (MSTG-CODE-8)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#memory-corruption-bugs-mstg-code-8"),"Ошибки памяти (MSTG-CODE-8)")</f>
+        <v>Ошибки памяти (MSTG-CODE-8)</v>
       </c>
       <c r="I71" s="76"/>
       <c r="J71" s="76"/>
@@ -6310,8 +6310,8 @@
       </c>
       <c r="G72" s="70"/>
       <c r="H72" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#make-sure-that-free-security-features-are-activated-mstg-code-9"),"Make Sure That Free Security Features Are Activated (MSTG-CODE-9)")</f>
-        <v>Make Sure That Free Security Features Are Activated (MSTG-CODE-9)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05i-Testing-Code-Quality-and-Build-Settings.md#make-sure-that-free-security-features-are-activated-mstg-code-9"),"Убедитесь, что активированы все стандартные функции безопасности (MSTG-CODE-9)")</f>
+        <v>Убедитесь, что активированы все стандартные функции безопасности (MSTG-CODE-9)</v>
       </c>
       <c r="I72" s="76"/>
       <c r="J72" s="76"/>

</xml_diff>

<commit_message>
Android Reverse Engineering translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Информация" sheetId="1" state="visible" r:id="rId2"/>
@@ -872,6 +872,135 @@
     <t xml:space="preserve">R</t>
   </si>
   <si>
+    <t xml:space="preserve">Impede Dynamic Analysis and Tampering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSTG-RESILIENCE-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Приложение обнаруживает и реагирует на наличие root или jailbreak, либо уведомляя пользователя, либо прекращая работу.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSTG-RESILIENCE-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Приложение не позволяет использовать отладчики и/или обнаруживает и реагирует на использование отладчика. Все доступные протоколы отладки должны быть учтены.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSTG-RESILIENCE-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Приложение обнаруживает и реагирует на внесения изменений в исполняемые файлы и критичные данные в своей песочнице.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSTG-RESILIENCE-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Приложение обнаруживает и реагирует на наличие на устройстве широко используемых инструментов и фреймворков для реверс инжиниринга.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSTG-RESILIENCE-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Приложение обнаруживает и реагирует на запуск на эмуляторе.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSTG-RESILIENCE-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Приложение обнаруживает и реагирует на изменение своего кода и данных в оперативной памяти.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSTG-RESILIENCE-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Приложение реализует несколько механизмов для каждой категории защиты (с 8.1 по 8.6). Обратите внимание, что на устойчивость к атакам влияет количество, разнообразие и оригинальность используемых механизмов.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSTG-RESILIENCE-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Механизмы обнаружения инициируют ответные меры разных типов, включая отложенные и скрытые.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSTG-RESILIENCE-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Обфускация применена в том числе и к тем программным механизмам, которые препятствуют деобфускации методами динамического анализа.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Привязка к устройству</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSTG-RESILIENCE-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Приложение реализует функциональность привязки экземпляра приложения к устройству, формируя его отпечаток из нескольких свойств, уникальных для устройства.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Противодействие восстановлению логики работы приложения</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSTG-RESILIENCE-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Все исполняемые файлы и библиотеки, принадлежащие приложению, зашифрованы на файловом уровне, либо важные участки кода и данных зашифрованы внутри исполняемых файлов. Простой статический анализ не позволяет обнаружить важный код или данные.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSTG-RESILIENCE-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Если задачей обфускации является защита конфиденциальных данных, то используется схема обфускации, которая подходит не только для этой задачи, но и защищает от ручной тестирования и автоматизированных деобфускаторов и учитывает последние исследования по данной теме. Эффективность схемы обфускации должна быть проверена с помощью ручного тестирования. Обратите внимание, что использование аппаратных средств защиты (если они поддерживаются устройством) предпочтительнее обфускации.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Требования безопасности мобильного приложения - iOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Требования к устойчивости к атакам на стороне клиента — iOS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Status</t>
   </si>
   <si>
@@ -879,135 +1008,6 @@
   </si>
   <si>
     <t xml:space="preserve">Comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Impede Dynamic Analysis and Tampering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSTG-RESILIENCE-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Приложение обнаруживает и реагирует на наличие root или jailbreak, либо уведомляя пользователя, либо прекращая работу.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSTG-RESILIENCE-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Приложение не позволяет использовать отладчики и/или обнаруживает и реагирует на использование отладчика. Все доступные протоколы отладки должны быть учтены.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSTG-RESILIENCE-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Приложение обнаруживает и реагирует на внесения изменений в исполняемые файлы и критичные данные в своей песочнице.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSTG-RESILIENCE-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Приложение обнаруживает и реагирует на наличие на устройстве широко используемых инструментов и фреймворков для реверс инжиниринга.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSTG-RESILIENCE-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Приложение обнаруживает и реагирует на запуск на эмуляторе.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSTG-RESILIENCE-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Приложение обнаруживает и реагирует на изменение своего кода и данных в оперативной памяти.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSTG-RESILIENCE-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Приложение реализует несколько механизмов для каждой категории защиты (с 8.1 по 8.6). Обратите внимание, что на устойчивость к атакам влияет количество, разнообразие и оригинальность используемых механизмов.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSTG-RESILIENCE-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Механизмы обнаружения инициируют ответные меры разных типов, включая отложенные и скрытые.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSTG-RESILIENCE-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Обфускация применена в том числе и к тем программным механизмам, которые препятствуют деобфускации методами динамического анализа.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Привязка к устройству</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSTG-RESILIENCE-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Приложение реализует функциональность привязки экземпляра приложения к устройству, формируя его отпечаток из нескольких свойств, уникальных для устройства.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Противодействие восстановлению логики работы приложения</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSTG-RESILIENCE-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Все исполняемые файлы и библиотеки, принадлежащие приложению, зашифрованы на файловом уровне, либо важные участки кода и данных зашифрованы внутри исполняемых файлов. Простой статический анализ не позволяет обнаружить важный код или данные.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSTG-RESILIENCE-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Если задачей обфускации является защита конфиденциальных данных, то используется схема обфускации, которая подходит не только для этой задачи, но и защищает от ручной тестирования и автоматизированных деобфускаторов и учитывает последние исследования по данной теме. Эффективность схемы обфускации должна быть проверена с помощью ручного тестирования. Обратите внимание, что использование аппаратных средств защиты (если они поддерживаются устройством) предпочтительнее обфускации.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Требования безопасности мобильного приложения - iOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Требования к устойчивости к атакам на стороне клиента — iOS</t>
   </si>
   <si>
     <t xml:space="preserve">XLS Version History</t>
@@ -2412,7 +2412,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2420,7 +2420,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2737,7 +2737,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2917,11 +2917,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="99587974"/>
-        <c:axId val="48444403"/>
+        <c:axId val="23019189"/>
+        <c:axId val="32012398"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="99587974"/>
+        <c:axId val="23019189"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2961,7 +2961,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48444403"/>
+        <c:crossAx val="32012398"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2969,7 +2969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48444403"/>
+        <c:axId val="32012398"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3012,7 +3012,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99587974"/>
+        <c:crossAx val="23019189"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3072,7 +3072,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3252,11 +3252,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="27647826"/>
-        <c:axId val="47034447"/>
+        <c:axId val="36383839"/>
+        <c:axId val="20635637"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="27647826"/>
+        <c:axId val="36383839"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3296,7 +3296,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47034447"/>
+        <c:crossAx val="20635637"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3304,7 +3304,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47034447"/>
+        <c:axId val="20635637"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3347,7 +3347,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27647826"/>
+        <c:crossAx val="36383839"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4536,8 +4536,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D68" activeCellId="0" sqref="D68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6523,8 +6523,8 @@
   </sheetPr>
   <dimension ref="B1:H29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6574,20 +6574,20 @@
         <v>271</v>
       </c>
       <c r="F3" s="56" t="s">
-        <v>272</v>
+        <v>56</v>
       </c>
       <c r="G3" s="121" t="s">
-        <v>273</v>
+        <v>57</v>
       </c>
       <c r="H3" s="58" t="s">
-        <v>274</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="79"/>
       <c r="C4" s="80"/>
       <c r="D4" s="81" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E4" s="82"/>
       <c r="F4" s="82"/>
@@ -6596,13 +6596,13 @@
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="65" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D5" s="96" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E5" s="123" t="s">
         <v>64</v>
@@ -6611,20 +6611,20 @@
         <v>77</v>
       </c>
       <c r="G5" s="124" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-root-detection-mstg-resilience-1"),"Testing Root Detection (MSTG-RESILIENCE-1)")</f>
-        <v>Testing Root Detection (MSTG-RESILIENCE-1)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-root-detection-mstg-resilience-1"),"Проверка наличия root-прав (MSTG-RESILIENCE-1)")</f>
+        <v>Проверка наличия root-прав (MSTG-RESILIENCE-1)</v>
       </c>
       <c r="H5" s="125"/>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="65" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D6" s="96" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E6" s="123" t="s">
         <v>64</v>
@@ -6633,20 +6633,20 @@
         <v>77</v>
       </c>
       <c r="G6" s="126" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-anti-debugging-detection-mstg-resilience-2"),"Testing Anti-Debugging Detection (MSTG-RESILIENCE-2)")</f>
-        <v>Testing Anti-Debugging Detection (MSTG-RESILIENCE-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-anti-debugging-detection-mstg-resilience-2"),"Проверка определения отладчиков (MSTG-RESILIENCE-2)")</f>
+        <v>Проверка определения отладчиков (MSTG-RESILIENCE-2)</v>
       </c>
       <c r="H6" s="125"/>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="65" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D7" s="92" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E7" s="123" t="s">
         <v>64</v>
@@ -6655,20 +6655,20 @@
         <v>77</v>
       </c>
       <c r="G7" s="124" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-file-integrity-checks-mstg-resilience-3"),"Testing File Integrity Checks (MSTG-RESILIENCE-3)")</f>
-        <v>Testing File Integrity Checks (MSTG-RESILIENCE-3)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-file-integrity-checks-mstg-resilience-3"),"Проверка целостности файлов (MSTG-RESILIENCE-3)")</f>
+        <v>Проверка целостности файлов (MSTG-RESILIENCE-3)</v>
       </c>
       <c r="H7" s="125"/>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="65" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D8" s="92" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E8" s="123" t="s">
         <v>64</v>
@@ -6677,20 +6677,20 @@
         <v>77</v>
       </c>
       <c r="G8" s="124" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-reverse-engineering-tools-detection-mstg-resilience-4"),"Testing Reverse Engineering Tools Detection (MSTG-RESILIENCE-4)")</f>
-        <v>Testing Reverse Engineering Tools Detection (MSTG-RESILIENCE-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-reverse-engineering-tools-detection-mstg-resilience-4"),"Проверка определения инструментов reverse engineering (MSTG-RESILIENCE-4)")</f>
+        <v>Проверка определения инструментов reverse engineering (MSTG-RESILIENCE-4)</v>
       </c>
       <c r="H8" s="125"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="65" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D9" s="92" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E9" s="123" t="s">
         <v>64</v>
@@ -6699,20 +6699,20 @@
         <v>77</v>
       </c>
       <c r="G9" s="124" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-emulator-detection-mstg-resilience-5"),"Testing Emulator Detection (MSTG-RESILIENCE-5)")</f>
-        <v>Testing Emulator Detection (MSTG-RESILIENCE-5)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-emulator-detection-mstg-resilience-5"),"Проверка определения эмулятора (MSTG-RESILIENCE-5)")</f>
+        <v>Проверка определения эмулятора (MSTG-RESILIENCE-5)</v>
       </c>
       <c r="H9" s="125"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="65" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D10" s="92" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E10" s="123" t="s">
         <v>64</v>
@@ -6721,20 +6721,20 @@
         <v>77</v>
       </c>
       <c r="G10" s="124" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-run-time-integrity-checks-mstg-resilience-6"),"Testing Run Time Integrity Checks (MSTG-RESILIENCE-6)")</f>
-        <v>Testing Run Time Integrity Checks (MSTG-RESILIENCE-6)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-run-time-integrity-checks-mstg-resilience-6"),"Проверка целостности во время выполнения (MSTG-RESILIENCE-6)")</f>
+        <v>Проверка целостности во время выполнения (MSTG-RESILIENCE-6)</v>
       </c>
       <c r="H10" s="125"/>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="65" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D11" s="96" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E11" s="123" t="s">
         <v>64</v>
@@ -6743,19 +6743,19 @@
         <v>77</v>
       </c>
       <c r="G11" s="127" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H11" s="125"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="65" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D12" s="92" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E12" s="123" t="s">
         <v>64</v>
@@ -6764,19 +6764,19 @@
         <v>77</v>
       </c>
       <c r="G12" s="128" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H12" s="125"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="65" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C13" s="66" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D13" s="92" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E13" s="123" t="s">
         <v>64</v>
@@ -6785,8 +6785,8 @@
         <v>77</v>
       </c>
       <c r="G13" s="124" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-obfuscation-mstg-resilience-9"),"Testing Obfuscation (MSTG-RESILIENCE-9)")</f>
-        <v>Testing Obfuscation (MSTG-RESILIENCE-9)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-obfuscation-mstg-resilience-9"),"Проверка на обфускацию (MSTG-RESILIENCE-9)")</f>
+        <v>Проверка на обфускацию (MSTG-RESILIENCE-9)</v>
       </c>
       <c r="H13" s="125"/>
     </row>
@@ -6794,7 +6794,7 @@
       <c r="B14" s="79"/>
       <c r="C14" s="80"/>
       <c r="D14" s="81" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E14" s="82"/>
       <c r="F14" s="82"/>
@@ -6803,13 +6803,13 @@
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="65" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C15" s="66" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D15" s="96" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E15" s="123" t="s">
         <v>64</v>
@@ -6818,8 +6818,8 @@
         <v>77</v>
       </c>
       <c r="G15" s="124" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-device-binding-mstg-resilience-10"),"Testing Device Binding (MSTG-RESILIENCE-10)")</f>
-        <v>Testing Device Binding (MSTG-RESILIENCE-10)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-device-binding-mstg-resilience-10"),"Тестирование привязки к устройству (MSTG-RESILIENCE-10)")</f>
+        <v>Тестирование привязки к устройству (MSTG-RESILIENCE-10)</v>
       </c>
       <c r="H15" s="125"/>
     </row>
@@ -6827,7 +6827,7 @@
       <c r="B16" s="79"/>
       <c r="C16" s="80"/>
       <c r="D16" s="81" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E16" s="82"/>
       <c r="F16" s="82"/>
@@ -6836,13 +6836,13 @@
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="65" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C17" s="66" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D17" s="96" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E17" s="123" t="s">
         <v>64</v>
@@ -6851,20 +6851,20 @@
         <v>77</v>
       </c>
       <c r="G17" s="124" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-obfuscation-mstg-resilience-9"),"Testing Obfuscation (MSTG-RESILIENCE-9)")</f>
-        <v>Testing Obfuscation (MSTG-RESILIENCE-9)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-obfuscation-mstg-resilience-9"),"Проверка на обфускацию (MSTG-RESILIENCE-9)")</f>
+        <v>Проверка на обфускацию (MSTG-RESILIENCE-9)</v>
       </c>
       <c r="H17" s="125"/>
     </row>
     <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="65" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C18" s="66" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D18" s="96" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E18" s="123" t="s">
         <v>64</v>
@@ -6873,7 +6873,7 @@
         <v>77</v>
       </c>
       <c r="G18" s="128" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H18" s="125"/>
     </row>
@@ -7038,7 +7038,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="131" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C1" s="131"/>
       <c r="D1" s="132"/>
@@ -9009,7 +9009,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="120" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C1" s="120"/>
       <c r="D1" s="112"/>
@@ -9037,20 +9037,20 @@
         <v>271</v>
       </c>
       <c r="F3" s="56" t="s">
-        <v>272</v>
+        <v>315</v>
       </c>
       <c r="G3" s="121" t="s">
-        <v>273</v>
+        <v>316</v>
       </c>
       <c r="H3" s="58" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="79"/>
       <c r="C4" s="80"/>
       <c r="D4" s="81" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E4" s="82"/>
       <c r="F4" s="82"/>
@@ -9059,13 +9059,13 @@
     </row>
     <row r="5" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="65" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D5" s="96" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E5" s="123" t="s">
         <v>64</v>
@@ -9081,13 +9081,13 @@
     </row>
     <row r="6" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="65" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D6" s="96" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E6" s="123" t="s">
         <v>64</v>
@@ -9103,13 +9103,13 @@
     </row>
     <row r="7" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="65" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D7" s="92" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E7" s="123" t="s">
         <v>64</v>
@@ -9125,13 +9125,13 @@
     </row>
     <row r="8" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="65" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D8" s="92" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E8" s="123" t="s">
         <v>64</v>
@@ -9140,19 +9140,19 @@
         <v>77</v>
       </c>
       <c r="G8" s="145" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H8" s="125"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="65" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D9" s="92" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E9" s="123" t="s">
         <v>64</v>
@@ -9161,19 +9161,19 @@
         <v>77</v>
       </c>
       <c r="G9" s="145" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H9" s="125"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="65" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D10" s="92" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E10" s="123" t="s">
         <v>64</v>
@@ -9182,19 +9182,19 @@
         <v>77</v>
       </c>
       <c r="G10" s="145" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H10" s="125"/>
     </row>
     <row r="11" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="65" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D11" s="96" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E11" s="123" t="s">
         <v>64</v>
@@ -9203,19 +9203,19 @@
         <v>77</v>
       </c>
       <c r="G11" s="128" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H11" s="125"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="65" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D12" s="92" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E12" s="123" t="s">
         <v>64</v>
@@ -9224,19 +9224,19 @@
         <v>77</v>
       </c>
       <c r="G12" s="128" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H12" s="125"/>
     </row>
     <row r="13" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="65" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C13" s="66" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D13" s="92" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E13" s="123" t="s">
         <v>64</v>
@@ -9245,7 +9245,7 @@
         <v>77</v>
       </c>
       <c r="G13" s="145" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H13" s="125"/>
     </row>
@@ -9253,7 +9253,7 @@
       <c r="B14" s="79"/>
       <c r="C14" s="80"/>
       <c r="D14" s="81" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E14" s="82"/>
       <c r="F14" s="82"/>
@@ -9262,13 +9262,13 @@
     </row>
     <row r="15" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="65" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C15" s="66" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D15" s="96" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E15" s="123" t="s">
         <v>64</v>
@@ -9286,7 +9286,7 @@
       <c r="B16" s="79"/>
       <c r="C16" s="80"/>
       <c r="D16" s="81" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E16" s="82"/>
       <c r="F16" s="82"/>
@@ -9295,13 +9295,13 @@
     </row>
     <row r="17" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="65" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C17" s="66" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D17" s="96" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E17" s="123" t="s">
         <v>64</v>
@@ -9317,13 +9317,13 @@
     </row>
     <row r="18" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="65" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C18" s="66" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D18" s="96" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E18" s="123" t="s">
         <v>64</v>
@@ -9332,7 +9332,7 @@
         <v>77</v>
       </c>
       <c r="G18" s="128" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H18" s="125"/>
     </row>
@@ -9572,7 +9572,7 @@
         <v>322</v>
       </c>
       <c r="E2" s="149" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
iOS Security Requiments V1 translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Информация" sheetId="1" state="visible" r:id="rId2"/>
@@ -1915,7 +1915,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="164">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2456,11 +2456,23 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="18" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="21" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2571,7 +2583,7 @@
     <cellStyle name="Normal 3" xfId="21"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
@@ -2590,13 +2602,6 @@
       <font>
         <color rgb="FF9C0006"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -2737,7 +2742,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2917,11 +2922,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="23019189"/>
-        <c:axId val="32012398"/>
+        <c:axId val="28478417"/>
+        <c:axId val="88615930"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="23019189"/>
+        <c:axId val="28478417"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2961,7 +2966,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32012398"/>
+        <c:crossAx val="88615930"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2969,7 +2974,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32012398"/>
+        <c:axId val="88615930"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3012,7 +3017,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23019189"/>
+        <c:crossAx val="28478417"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3072,7 +3077,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3252,11 +3257,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="36383839"/>
-        <c:axId val="20635637"/>
+        <c:axId val="71759975"/>
+        <c:axId val="16537529"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="36383839"/>
+        <c:axId val="71759975"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3296,7 +3301,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20635637"/>
+        <c:crossAx val="16537529"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3304,7 +3309,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20635637"/>
+        <c:axId val="16537529"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3347,7 +3352,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36383839"/>
+        <c:crossAx val="71759975"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4536,8 +4541,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6523,7 +6528,7 @@
   </sheetPr>
   <dimension ref="B1:H29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -7018,8 +7023,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7124,8 +7129,8 @@
       </c>
       <c r="G5" s="70"/>
       <c r="H5" s="134" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#architectural-information"), "Architectural Information")</f>
-        <v>Architectural Information</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#architectural-information"), "Информация об архитектуре")</f>
+        <v>Информация об архитектуре</v>
       </c>
       <c r="I5" s="76"/>
       <c r="J5" s="76"/>
@@ -7148,15 +7153,15 @@
         <v>64</v>
       </c>
       <c r="G6" s="70"/>
-      <c r="H6" s="134" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"), "Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
-        <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
-      </c>
-      <c r="I6" s="135" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
-        <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
-      </c>
-      <c r="J6" s="136"/>
+      <c r="H6" s="135" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"), "Ошибка инъекции (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
+        <v>Ошибка инъекции (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
+      </c>
+      <c r="I6" s="136" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Проверка наличия соответствующей авторизации (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
+        <v>Проверка наличия соответствующей авторизации (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
+      </c>
+      <c r="J6" s="137"/>
       <c r="K6" s="73"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7177,8 +7182,8 @@
       </c>
       <c r="G7" s="70"/>
       <c r="H7" s="134" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#architectural-information"), "Architectural Information")</f>
-        <v>Architectural Information</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#architectural-information"), "Информация об архитектуре")</f>
+        <v>Информация об архитектуре</v>
       </c>
       <c r="I7" s="76"/>
       <c r="J7" s="76"/>
@@ -7202,8 +7207,8 @@
       </c>
       <c r="G8" s="70"/>
       <c r="H8" s="134" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#identifying-sensitive-data"), "Identifying Sensitive Data")</f>
-        <v>Identifying Sensitive Data</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#identifying-sensitive-data"), "Выявление конфиденциальных данных")</f>
+        <v>Выявление конфиденциальных данных</v>
       </c>
       <c r="I8" s="76"/>
       <c r="J8" s="76"/>
@@ -7227,8 +7232,8 @@
         <v>77</v>
       </c>
       <c r="H9" s="134" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#environmental-information"), "Environmental Information")</f>
-        <v>Environmental Information</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#environmental-information"), "Информация об окружении")</f>
+        <v>Информация об окружении</v>
       </c>
       <c r="I9" s="76"/>
       <c r="J9" s="76"/>
@@ -7252,8 +7257,8 @@
         <v>77</v>
       </c>
       <c r="H10" s="134" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#mapping-the-application"), "Mapping the Application")</f>
-        <v>Mapping the Application</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#mapping-the-application"), "Составление карты приложения")</f>
+        <v>Составление карты приложения</v>
       </c>
       <c r="I10" s="76"/>
       <c r="J10" s="76"/>
@@ -7276,13 +7281,13 @@
       <c r="G11" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H11" s="134" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#principles-of-testing"), "Principles of Testing")</f>
-        <v>Principles of Testing</v>
-      </c>
-      <c r="I11" s="75" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#penetration-testing-aka-pentesting"), "Penetration Testing (a.k.a. Pentesting)")</f>
-        <v>Penetration Testing (a.k.a. Pentesting)</v>
+      <c r="H11" s="136" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#principles-of-testing"), "Принципы тестирования")</f>
+        <v>Принципы тестирования</v>
+      </c>
+      <c r="I11" s="138" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#penetration-testing-aka-pentesting"), "Тестирование на проникновение (a.k.a. Pentesting)")</f>
+        <v>Тестирование на проникновение (a.k.a. Pentesting)</v>
       </c>
       <c r="J11" s="75"/>
       <c r="K11" s="73"/>
@@ -7305,8 +7310,8 @@
         <v>77</v>
       </c>
       <c r="H12" s="134" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04g-Testing-Cryptography.md#cryptographic-policy"), "Cryptographic policy")</f>
-        <v>Cryptographic policy</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04g-Testing-Cryptography.md#cryptographic-policy"), "Криптографическая политика")</f>
+        <v>Криптографическая политика</v>
       </c>
       <c r="I12" s="76"/>
       <c r="J12" s="76"/>
@@ -7329,9 +7334,9 @@
       <c r="G13" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H13" s="134" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x06h-Testing-Platform-Interaction.md#testing-enforced-updating-mstg-arch-9"), "Testing enforced updating (MSTG-ARCH-9)")</f>
-        <v>Testing enforced updating (MSTG-ARCH-9)</v>
+      <c r="H13" s="71" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x06h-Testing-Platform-Interaction.md#testing-enforced-updating-mstg-arch-9"), "Тест принудительного обновления (MSTG-ARCH-9)")</f>
+        <v>Тест принудительного обновления (MSTG-ARCH-9)</v>
       </c>
       <c r="I13" s="76"/>
       <c r="J13" s="76"/>
@@ -7355,8 +7360,8 @@
         <v>77</v>
       </c>
       <c r="H14" s="134" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#security-testing-and-the-sdlc"), "Security Testing and the SDLC")</f>
-        <v>Security Testing and the SDLC</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04b-Mobile-App-Security-Testing.md#security-testing-and-the-sdlc"), "Тестирование безопасности и SDLC (жизненного цикла разработки ПО)")</f>
+        <v>Тестирование безопасности и SDLC (жизненного цикла разработки ПО)</v>
       </c>
       <c r="I14" s="76"/>
       <c r="J14" s="76"/>
@@ -7395,7 +7400,7 @@
         <v>64</v>
       </c>
       <c r="G16" s="70"/>
-      <c r="H16" s="135" t="str">
+      <c r="H16" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-local-data-storage-mstg-storage-1-and-mstg-storage-2"),"Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
         <v>Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
@@ -7416,7 +7421,7 @@
       <c r="E17" s="68"/>
       <c r="F17" s="69"/>
       <c r="G17" s="70"/>
-      <c r="H17" s="135" t="str">
+      <c r="H17" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-local-data-storage-mstg-storage-1-and-mstg-storage-2"),"Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
         <v>Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
@@ -7441,7 +7446,7 @@
         <v>64</v>
       </c>
       <c r="G18" s="70"/>
-      <c r="H18" s="135" t="str">
+      <c r="H18" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#checking-logs-for-sensitive-data-mstg-storage-3"),"Checking Logs for Sensitive Data (MSTG-STORAGE-3)")</f>
         <v>Checking Logs for Sensitive Data (MSTG-STORAGE-3)</v>
       </c>
@@ -7466,7 +7471,7 @@
         <v>64</v>
       </c>
       <c r="G19" s="70"/>
-      <c r="H19" s="135" t="str">
+      <c r="H19" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-sent-to-third-parties-mstg-storage-4"),"Determining Whether Sensitive Data Is Sent to Third Parties (MSTG-STORAGE-4)")</f>
         <v>Determining Whether Sensitive Data Is Sent to Third Parties (MSTG-STORAGE-4)</v>
       </c>
@@ -7491,7 +7496,7 @@
         <v>64</v>
       </c>
       <c r="G20" s="70"/>
-      <c r="H20" s="135" t="str">
+      <c r="H20" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#finding-sensitive-data-in-the-keyboard-cache-mstg-storage-5"),"Finding Sensitive Data in the Keyboard Cache (MSTG-STORAGE-5)")</f>
         <v>Finding Sensitive Data in the Keyboard Cache (MSTG-STORAGE-5)</v>
       </c>
@@ -7516,7 +7521,7 @@
         <v>64</v>
       </c>
       <c r="G21" s="70"/>
-      <c r="H21" s="137" t="str">
+      <c r="H21" s="140" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-exposed-via-ipc-mechanisms-mstg-storage-6"),"Determining Whether Sensitive Data Is Exposed via IPC Mechanisms (MSTG-STORAGE-6)")</f>
         <v>Determining Whether Sensitive Data Is Exposed via IPC Mechanisms (MSTG-STORAGE-6)</v>
       </c>
@@ -7541,7 +7546,7 @@
         <v>64</v>
       </c>
       <c r="G22" s="70"/>
-      <c r="H22" s="135" t="str">
+      <c r="H22" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#checking-for-sensitive-data-disclosed-through-the-user-interface-mstg-storage-7"),"Checking for Sensitive Data Disclosed Through the User Interface (MSTG-STORAGE-7)")</f>
         <v>Checking for Sensitive Data Disclosed Through the User Interface (MSTG-STORAGE-7)</v>
       </c>
@@ -7566,7 +7571,7 @@
       <c r="G23" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H23" s="135" t="str">
+      <c r="H23" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-backups-for-sensitive-data-mstg-storage-8"),"Testing Backups for Sensitive Data (MSTG-STORAGE-8)")</f>
         <v>Testing Backups for Sensitive Data (MSTG-STORAGE-8)</v>
       </c>
@@ -7591,7 +7596,7 @@
       <c r="G24" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H24" s="135" t="str">
+      <c r="H24" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-auto-generated-screenshots-for-sensitive-information-mstg-storage-9"),"Testing Auto-Generated Screenshots for Sensitive Information (MSTG-STORAGE-9)")</f>
         <v>Testing Auto-Generated Screenshots for Sensitive Information (MSTG-STORAGE-9)</v>
       </c>
@@ -7616,7 +7621,7 @@
       <c r="G25" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H25" s="135" t="str">
+      <c r="H25" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-memory-for-sensitive-data-mstg-storage-10"),"Testing Memory for Sensitive Data (MSTG-STORAGE-10)")</f>
         <v>Testing Memory for Sensitive Data (MSTG-STORAGE-10)</v>
       </c>
@@ -7641,14 +7646,14 @@
       <c r="G26" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H26" s="135" t="str">
+      <c r="H26" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06f-Testing-Local-Authentication.md#testing-local-authentication-mstg-auth-8-and-mstg-storage-11"),"Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)")</f>
         <v>Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)</v>
       </c>
       <c r="I26" s="76"/>
       <c r="J26" s="76"/>
       <c r="K26" s="73"/>
-      <c r="L26" s="138"/>
+      <c r="L26" s="141"/>
     </row>
     <row r="27" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="87" t="s">
@@ -7709,7 +7714,7 @@
         <v>64</v>
       </c>
       <c r="G29" s="70"/>
-      <c r="H29" s="135" t="str">
+      <c r="H29" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
@@ -7734,7 +7739,7 @@
         <v>64</v>
       </c>
       <c r="G30" s="70"/>
-      <c r="H30" s="137" t="str">
+      <c r="H30" s="140" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#verifying-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-and-mstg-crypto-3"),"Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
@@ -7759,7 +7764,7 @@
         <v>64</v>
       </c>
       <c r="G31" s="70"/>
-      <c r="H31" s="137" t="str">
+      <c r="H31" s="140" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#verifying-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-and-mstg-crypto-3"),"Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
@@ -7784,7 +7789,7 @@
         <v>64</v>
       </c>
       <c r="G32" s="70"/>
-      <c r="H32" s="135" t="str">
+      <c r="H32" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#identifying-insecure-andor-deprecated-cryptographic-algorithms-mstg-crypto-4"),"Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)")</f>
         <v>Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)</v>
       </c>
@@ -7809,7 +7814,7 @@
         <v>64</v>
       </c>
       <c r="G33" s="70"/>
-      <c r="H33" s="135" t="str">
+      <c r="H33" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
@@ -7834,7 +7839,7 @@
         <v>64</v>
       </c>
       <c r="G34" s="70"/>
-      <c r="H34" s="135" t="str">
+      <c r="H34" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-random-number-generation-mstg-crypto-6")," Testing Random Number Generation (MSTG-CRYPTO-6)")</f>
         <v> Testing Random Number Generation (MSTG-CRYPTO-6)</v>
       </c>
@@ -7875,7 +7880,7 @@
         <v>64</v>
       </c>
       <c r="G36" s="70"/>
-      <c r="H36" s="135" t="str">
+      <c r="H36" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
         <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
@@ -7883,7 +7888,7 @@
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
-      <c r="J36" s="139"/>
+      <c r="J36" s="142"/>
       <c r="K36" s="125"/>
     </row>
     <row r="37" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7903,7 +7908,7 @@
         <v>64</v>
       </c>
       <c r="G37" s="70"/>
-      <c r="H37" s="135" t="str">
+      <c r="H37" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateful-session-management-mstg-auth-2"),"Testing Stateful Session Management (MSTG-AUTH-2)")</f>
         <v>Testing Stateful Session Management (MSTG-AUTH-2)</v>
       </c>
@@ -7928,7 +7933,7 @@
         <v>64</v>
       </c>
       <c r="G38" s="70"/>
-      <c r="H38" s="135" t="str">
+      <c r="H38" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateless-token-based-authentication-mstg-auth-3"),"Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)")</f>
         <v>Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)</v>
       </c>
@@ -7936,7 +7941,7 @@
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
-      <c r="J38" s="139"/>
+      <c r="J38" s="142"/>
       <c r="K38" s="125"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7952,7 +7957,7 @@
       <c r="E39" s="68"/>
       <c r="F39" s="69"/>
       <c r="G39" s="70"/>
-      <c r="H39" s="135" t="str">
+      <c r="H39" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-user-logout-mstg-auth-4"),"Testing User Logout (MSTG-AUTH-4)")</f>
         <v>Testing User Logout (MSTG-AUTH-4)</v>
       </c>
@@ -7978,7 +7983,7 @@
         <v>64</v>
       </c>
       <c r="G40" s="70"/>
-      <c r="H40" s="135" t="str">
+      <c r="H40" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
         <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
@@ -8004,7 +8009,7 @@
         <v>64</v>
       </c>
       <c r="G41" s="70"/>
-      <c r="H41" s="135" t="str">
+      <c r="H41" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
         <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
@@ -8012,7 +8017,7 @@
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#dynamic-testing-mstg-auth-6"),"Dynamic Testing (MSTG-AUTH-6)")</f>
         <v>Dynamic Testing (MSTG-AUTH-6)</v>
       </c>
-      <c r="J41" s="139"/>
+      <c r="J41" s="142"/>
       <c r="K41" s="125"/>
     </row>
     <row r="42" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8032,12 +8037,12 @@
         <v>64</v>
       </c>
       <c r="G42" s="70"/>
-      <c r="H42" s="135" t="str">
+      <c r="H42" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-session-timeout-mstg-auth-7"),"Testing Session Timeout (MSTG-AUTH-7)")</f>
         <v>Testing Session Timeout (MSTG-AUTH-7)</v>
       </c>
       <c r="I42" s="97"/>
-      <c r="J42" s="140"/>
+      <c r="J42" s="143"/>
       <c r="K42" s="99"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8057,12 +8062,12 @@
       <c r="G43" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H43" s="135" t="str">
+      <c r="H43" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06f-Testing-Local-Authentication.md#testing-local-authentication-mstg-auth-8-and-mstg-storage-11"),"Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)")</f>
         <v>Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)</v>
       </c>
       <c r="I43" s="90"/>
-      <c r="J43" s="139"/>
+      <c r="J43" s="142"/>
       <c r="K43" s="125"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8082,7 +8087,7 @@
       <c r="G44" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H44" s="137" t="str">
+      <c r="H44" s="140" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
@@ -8107,7 +8112,7 @@
       <c r="G45" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H45" s="137" t="str">
+      <c r="H45" s="140" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
@@ -8132,7 +8137,7 @@
       <c r="G46" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H46" s="141" t="str">
+      <c r="H46" s="144" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04e-Testing-Authentication-and-Session-Management.md#testing-login-activity-and-device-blocking-mstg-auth-11"), "Testing Login Activity and Device Blocking (MSTG-AUTH-11)")</f>
         <v>Testing Login Activity and Device Blocking (MSTG-AUTH-11)</v>
       </c>
@@ -8173,7 +8178,7 @@
         <v>64</v>
       </c>
       <c r="G48" s="70"/>
-      <c r="H48" s="137" t="str">
+      <c r="H48" s="140" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
@@ -8198,7 +8203,7 @@
         <v>64</v>
       </c>
       <c r="G49" s="70"/>
-      <c r="H49" s="137" t="str">
+      <c r="H49" s="140" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
@@ -8226,7 +8231,7 @@
         <v>64</v>
       </c>
       <c r="G50" s="70"/>
-      <c r="H50" s="135" t="str">
+      <c r="H50" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-3-and-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)")</f>
         <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)</v>
       </c>
@@ -8251,7 +8256,7 @@
       <c r="G51" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H51" s="135" t="str">
+      <c r="H51" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-3-and-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)")</f>
         <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)</v>
       </c>
@@ -8276,7 +8281,7 @@
       <c r="G52" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H52" s="137" t="str">
+      <c r="H52" s="140" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels-mstg-network-5"),"Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)")</f>
         <v>Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)</v>
       </c>
@@ -8301,7 +8306,7 @@
       <c r="G53" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H53" s="135" t="str">
+      <c r="H53" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x06i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"), "Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
         <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
       </c>
@@ -8342,7 +8347,7 @@
         <v>64</v>
       </c>
       <c r="G55" s="70"/>
-      <c r="H55" s="135" t="str">
+      <c r="H55" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-app-permissions-mstg-platform-1"),"Testing App Permissions (MSTG-PLATFORM-1)")</f>
         <v>Testing App Permissions (MSTG-PLATFORM-1)</v>
       </c>
@@ -8367,7 +8372,7 @@
         <v>64</v>
       </c>
       <c r="G56" s="70"/>
-      <c r="H56" s="135" t="str">
+      <c r="H56" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"),"Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
         <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
@@ -8392,7 +8397,7 @@
         <v>64</v>
       </c>
       <c r="G57" s="70"/>
-      <c r="H57" s="135" t="str">
+      <c r="H57" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-custom-url-schemes-mstg-platform-3"),"Testing Custom URL Schemes (MSTG-PLATFORM-3)")</f>
         <v>Testing Custom URL Schemes (MSTG-PLATFORM-3)</v>
       </c>
@@ -8417,7 +8422,7 @@
         <v>64</v>
       </c>
       <c r="G58" s="70"/>
-      <c r="H58" s="134" t="str">
+      <c r="H58" s="71" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x06h-Testing-Platform-Interaction.md#testing-for-sensitive-functionality-exposure-through-ipc-mstg-platform-4"), "Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)")</f>
         <v>Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)</v>
       </c>
@@ -8442,7 +8447,7 @@
         <v>64</v>
       </c>
       <c r="G59" s="70"/>
-      <c r="H59" s="135" t="str">
+      <c r="H59" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-ios-webviews-mstg-platform-5"),"Testing iOS WebViews (MSTG-PLATFORM-5)")</f>
         <v>Testing iOS WebViews (MSTG-PLATFORM-5)</v>
       </c>
@@ -8467,7 +8472,7 @@
         <v>64</v>
       </c>
       <c r="G60" s="70"/>
-      <c r="H60" s="135" t="str">
+      <c r="H60" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-webview-protocol-handlers-mstg-platform-6"),"Testing WebView Protocol Handlers (MSTG-PLATFORM-6)")</f>
         <v>Testing WebView Protocol Handlers (MSTG-PLATFORM-6)</v>
       </c>
@@ -8492,7 +8497,7 @@
         <v>64</v>
       </c>
       <c r="G61" s="70"/>
-      <c r="H61" s="135" t="str">
+      <c r="H61" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#determining-whether-native-methods-are-exposed-through-webviews-mstg-platform-7"),"Determining Whether Native Methods Are Exposed Through WebViews (MSTG-PLATFORM-7)")</f>
         <v>Determining Whether Native Methods Are Exposed Through WebViews (MSTG-PLATFORM-7)</v>
       </c>
@@ -8517,7 +8522,7 @@
         <v>64</v>
       </c>
       <c r="G62" s="70"/>
-      <c r="H62" s="135" t="str">
+      <c r="H62" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-object-persistence-mstg-platform-8"),"Testing Object Persistence (MSTG-PLATFORM-8)")</f>
         <v>Testing Object Persistence (MSTG-PLATFORM-8)</v>
       </c>
@@ -8558,7 +8563,7 @@
         <v>64</v>
       </c>
       <c r="G64" s="70"/>
-      <c r="H64" s="135" t="str">
+      <c r="H64" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#making-sure-that-the-app-is-properly-signed-mstg-code-1"),"Making Sure that the App Is Properly Signed (MSTG-CODE-1)")</f>
         <v>Making Sure that the App Is Properly Signed (MSTG-CODE-1)</v>
       </c>
@@ -8583,7 +8588,7 @@
         <v>64</v>
       </c>
       <c r="G65" s="70"/>
-      <c r="H65" s="135" t="str">
+      <c r="H65" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#determining-whether-the-app-is-debuggable-mstg-code-2"),"Determining Whether the App is Debuggable (MSTG-CODE-2)")</f>
         <v>Determining Whether the App is Debuggable (MSTG-CODE-2)</v>
       </c>
@@ -8608,7 +8613,7 @@
         <v>64</v>
       </c>
       <c r="G66" s="70"/>
-      <c r="H66" s="135" t="str">
+      <c r="H66" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-symbols-mstg-code-3"),"Finding Debugging Symbols (MSTG-CODE-3)")</f>
         <v>Finding Debugging Symbols (MSTG-CODE-3)</v>
       </c>
@@ -8633,7 +8638,7 @@
         <v>64</v>
       </c>
       <c r="G67" s="70"/>
-      <c r="H67" s="135" t="str">
+      <c r="H67" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-code-and-verbose-error-logging-mstg-code-4"),"Finding Debugging Code and Verbose Error Logging (MSTG-CODE-4)")</f>
         <v>Finding Debugging Code and Verbose Error Logging (MSTG-CODE-4)</v>
       </c>
@@ -8658,7 +8663,7 @@
         <v>64</v>
       </c>
       <c r="G68" s="70"/>
-      <c r="H68" s="141" t="str">
+      <c r="H68" s="144" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"),"Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
         <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
       </c>
@@ -8683,7 +8688,7 @@
         <v>64</v>
       </c>
       <c r="G69" s="70"/>
-      <c r="H69" s="135" t="str">
+      <c r="H69" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6"),"Testing Exception Handling (MSTG-CODE-6)")</f>
         <v>Testing Exception Handling (MSTG-CODE-6)</v>
       </c>
@@ -8708,7 +8713,7 @@
         <v>64</v>
       </c>
       <c r="G70" s="70"/>
-      <c r="H70" s="135" t="str">
+      <c r="H70" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6"),"Testing Exception Handling (MSTG-CODE-6)")</f>
         <v>Testing Exception Handling (MSTG-CODE-6)</v>
       </c>
@@ -8733,7 +8738,7 @@
         <v>64</v>
       </c>
       <c r="G71" s="70"/>
-      <c r="H71" s="135" t="str">
+      <c r="H71" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#memory-corruption-bugs-mstg-code-8"),"Memory Corruption Bugs (MSTG-CODE-8)")</f>
         <v>Memory Corruption Bugs (MSTG-CODE-8)</v>
       </c>
@@ -8758,7 +8763,7 @@
         <v>64</v>
       </c>
       <c r="G72" s="70"/>
-      <c r="H72" s="135" t="str">
+      <c r="H72" s="139" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#make-sure-that-free-security-features-are-activated-mstg-code-9"),"Make Sure That Free Security Features Are Activated (MSTG-CODE-9)")</f>
         <v>Make Sure That Free Security Features Are Activated (MSTG-CODE-9)</v>
       </c>
@@ -8775,12 +8780,12 @@
       <c r="G73" s="108"/>
       <c r="H73" s="108"/>
       <c r="I73" s="109"/>
-      <c r="J73" s="142"/>
-      <c r="K73" s="143"/>
+      <c r="J73" s="145"/>
+      <c r="K73" s="146"/>
     </row>
     <row r="74" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="144"/>
-      <c r="C74" s="144"/>
+      <c r="B74" s="147"/>
+      <c r="C74" s="147"/>
       <c r="D74" s="92"/>
       <c r="E74" s="114"/>
       <c r="F74" s="114"/>
@@ -8791,8 +8796,8 @@
       <c r="K74" s="92"/>
     </row>
     <row r="75" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="144"/>
-      <c r="C75" s="144"/>
+      <c r="B75" s="147"/>
+      <c r="C75" s="147"/>
       <c r="D75" s="92"/>
       <c r="E75" s="114"/>
       <c r="F75" s="114"/>
@@ -8803,8 +8808,8 @@
       <c r="K75" s="92"/>
     </row>
     <row r="76" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="144"/>
-      <c r="C76" s="144"/>
+      <c r="B76" s="147"/>
+      <c r="C76" s="147"/>
       <c r="D76" s="92"/>
       <c r="E76" s="114"/>
       <c r="F76" s="114"/>
@@ -8893,8 +8898,8 @@
       <c r="K81" s="92"/>
     </row>
     <row r="82" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="144"/>
-      <c r="C82" s="144"/>
+      <c r="B82" s="147"/>
+      <c r="C82" s="147"/>
       <c r="D82" s="92"/>
       <c r="E82" s="114"/>
       <c r="F82" s="114"/>
@@ -8905,8 +8910,8 @@
       <c r="K82" s="92"/>
     </row>
     <row r="83" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="144"/>
-      <c r="C83" s="144"/>
+      <c r="B83" s="147"/>
+      <c r="C83" s="147"/>
       <c r="D83" s="92"/>
       <c r="E83" s="114"/>
       <c r="F83" s="114"/>
@@ -8917,8 +8922,8 @@
       <c r="K83" s="92"/>
     </row>
     <row r="84" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="144"/>
-      <c r="C84" s="144"/>
+      <c r="B84" s="147"/>
+      <c r="C84" s="147"/>
       <c r="D84" s="92"/>
       <c r="E84" s="114"/>
       <c r="F84" s="114"/>
@@ -8929,8 +8934,8 @@
       <c r="K84" s="92"/>
     </row>
     <row r="85" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="144"/>
-      <c r="C85" s="144"/>
+      <c r="B85" s="147"/>
+      <c r="C85" s="147"/>
       <c r="D85" s="92"/>
       <c r="E85" s="114"/>
       <c r="F85" s="114"/>
@@ -8949,7 +8954,7 @@
       <formula>NOT(ISERROR(SEARCH("0x05",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H26 H28:H1048576 H1:H2">
+  <conditionalFormatting sqref="H15:H26 H28:H1048576 H1:H2 H4 H13">
     <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="3">
       <formula>NOT(ISERROR(SEARCH("0x05",H1)))</formula>
     </cfRule>
@@ -8957,11 +8962,6 @@
   <conditionalFormatting sqref="J6">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="4">
       <formula>NOT(ISERROR(SEARCH("0x05",J6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="5">
-      <formula>NOT(ISERROR(SEARCH("0x05",I6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -9139,7 +9139,7 @@
       <c r="F8" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="145" t="s">
+      <c r="G8" s="148" t="s">
         <v>298</v>
       </c>
       <c r="H8" s="125"/>
@@ -9160,7 +9160,7 @@
       <c r="F9" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G9" s="145" t="s">
+      <c r="G9" s="148" t="s">
         <v>298</v>
       </c>
       <c r="H9" s="125"/>
@@ -9181,7 +9181,7 @@
       <c r="F10" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="145" t="s">
+      <c r="G10" s="148" t="s">
         <v>298</v>
       </c>
       <c r="H10" s="125"/>
@@ -9244,7 +9244,7 @@
       <c r="F13" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="145" t="s">
+      <c r="G13" s="148" t="s">
         <v>298</v>
       </c>
       <c r="H13" s="125"/>
@@ -9309,7 +9309,7 @@
       <c r="F17" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="146" t="str">
+      <c r="G17" s="149" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks-mstg-resilience-3-and-mstg-resilience-11"),"File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)")</f>
         <v>File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)</v>
       </c>
@@ -9346,8 +9346,8 @@
       <c r="H19" s="110"/>
     </row>
     <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="144"/>
-      <c r="C20" s="144"/>
+      <c r="B20" s="147"/>
+      <c r="C20" s="147"/>
       <c r="D20" s="92"/>
       <c r="E20" s="114"/>
       <c r="F20" s="114"/>
@@ -9355,8 +9355,8 @@
       <c r="H20" s="92"/>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="144"/>
-      <c r="C21" s="144"/>
+      <c r="B21" s="147"/>
+      <c r="C21" s="147"/>
       <c r="D21" s="92"/>
       <c r="E21" s="114"/>
       <c r="F21" s="114"/>
@@ -9427,8 +9427,8 @@
       <c r="H26" s="92"/>
     </row>
     <row r="27" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="144"/>
-      <c r="C27" s="144"/>
+      <c r="B27" s="147"/>
+      <c r="C27" s="147"/>
       <c r="D27" s="92"/>
       <c r="E27" s="114"/>
       <c r="F27" s="114"/>
@@ -9436,8 +9436,8 @@
       <c r="H27" s="92"/>
     </row>
     <row r="28" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="144"/>
-      <c r="C28" s="144"/>
+      <c r="B28" s="147"/>
+      <c r="C28" s="147"/>
       <c r="D28" s="92"/>
       <c r="E28" s="114"/>
       <c r="F28" s="114"/>
@@ -9445,8 +9445,8 @@
       <c r="H28" s="92"/>
     </row>
     <row r="29" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="144"/>
-      <c r="C29" s="144"/>
+      <c r="B29" s="147"/>
+      <c r="C29" s="147"/>
       <c r="D29" s="92"/>
       <c r="E29" s="114"/>
       <c r="F29" s="114"/>
@@ -9454,64 +9454,64 @@
       <c r="H29" s="92"/>
     </row>
     <row r="30" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="144"/>
-      <c r="C30" s="144"/>
+      <c r="B30" s="147"/>
+      <c r="C30" s="147"/>
       <c r="D30" s="92"/>
       <c r="E30" s="114"/>
       <c r="F30" s="114"/>
     </row>
     <row r="31" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="144"/>
-      <c r="C31" s="144"/>
+      <c r="B31" s="147"/>
+      <c r="C31" s="147"/>
       <c r="D31" s="92"/>
       <c r="E31" s="114"/>
       <c r="F31" s="114"/>
     </row>
     <row r="32" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="144"/>
-      <c r="C32" s="144"/>
+      <c r="B32" s="147"/>
+      <c r="C32" s="147"/>
       <c r="D32" s="92"/>
       <c r="E32" s="114"/>
       <c r="F32" s="114"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G8">
-    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="6">
+    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="5">
       <formula>NOT(ISERROR(SEARCH("0x05",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="7">
+    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="6">
       <formula>NOT(ISERROR(SEARCH("0x05",G9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="8">
+    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="7">
       <formula>NOT(ISERROR(SEARCH("0x05",G10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="9">
+    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="8">
       <formula>NOT(ISERROR(SEARCH("0x05",G11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="10">
+    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="9">
       <formula>NOT(ISERROR(SEARCH("0x05",G12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13">
-    <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="11">
+    <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="10">
       <formula>NOT(ISERROR(SEARCH("0x05",G13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="12">
+    <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="11">
       <formula>NOT(ISERROR(SEARCH("0x05",G17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="13">
+    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="12">
       <formula>NOT(ISERROR(SEARCH("0x05",G18)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9550,412 +9550,412 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="150" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="148"/>
+      <c r="B1" s="150"/>
+      <c r="C1" s="151"/>
       <c r="D1" s="52"/>
       <c r="E1" s="52"/>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="149" t="s">
+      <c r="A2" s="152" t="s">
         <v>319</v>
       </c>
-      <c r="B2" s="149" t="s">
+      <c r="B2" s="152" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="152" t="s">
         <v>321</v>
       </c>
-      <c r="D2" s="149" t="s">
+      <c r="D2" s="152" t="s">
         <v>322</v>
       </c>
-      <c r="E2" s="149" t="s">
+      <c r="E2" s="152" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="150" t="s">
+      <c r="A3" s="153" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="151" t="n">
+      <c r="B3" s="154" t="n">
         <v>0.1</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152" t="n">
+      <c r="C3" s="154"/>
+      <c r="D3" s="155" t="n">
         <v>42765</v>
       </c>
-      <c r="E3" s="153" t="s">
+      <c r="E3" s="156" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="153" t="s">
+      <c r="A4" s="156" t="s">
         <v>325</v>
       </c>
-      <c r="B4" s="151" t="n">
+      <c r="B4" s="154" t="n">
         <v>0.2</v>
       </c>
-      <c r="C4" s="151"/>
-      <c r="D4" s="152" t="n">
+      <c r="C4" s="154"/>
+      <c r="D4" s="155" t="n">
         <v>42766</v>
       </c>
-      <c r="E4" s="153" t="s">
+      <c r="E4" s="156" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="153" t="s">
+      <c r="A5" s="156" t="s">
         <v>327</v>
       </c>
-      <c r="B5" s="151" t="n">
+      <c r="B5" s="154" t="n">
         <v>0.3</v>
       </c>
-      <c r="C5" s="151"/>
-      <c r="D5" s="152" t="n">
+      <c r="C5" s="154"/>
+      <c r="D5" s="155" t="n">
         <v>42778</v>
       </c>
-      <c r="E5" s="153" t="s">
+      <c r="E5" s="156" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="153" t="s">
+      <c r="A6" s="156" t="s">
         <v>329</v>
       </c>
-      <c r="B6" s="151" t="s">
+      <c r="B6" s="154" t="s">
         <v>330</v>
       </c>
-      <c r="C6" s="151"/>
-      <c r="D6" s="152" t="n">
+      <c r="C6" s="154"/>
+      <c r="D6" s="155" t="n">
         <v>42780</v>
       </c>
-      <c r="E6" s="153" t="s">
+      <c r="E6" s="156" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="153" t="s">
+      <c r="A7" s="156" t="s">
         <v>325</v>
       </c>
-      <c r="B7" s="154" t="s">
+      <c r="B7" s="157" t="s">
         <v>332</v>
       </c>
-      <c r="C7" s="154"/>
-      <c r="D7" s="152" t="n">
+      <c r="C7" s="157"/>
+      <c r="D7" s="155" t="n">
         <v>42781</v>
       </c>
-      <c r="E7" s="153" t="s">
+      <c r="E7" s="156" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="153" t="s">
+      <c r="A8" s="156" t="s">
         <v>329</v>
       </c>
-      <c r="B8" s="154" t="s">
+      <c r="B8" s="157" t="s">
         <v>334</v>
       </c>
-      <c r="C8" s="154"/>
-      <c r="D8" s="152" t="n">
+      <c r="C8" s="157"/>
+      <c r="D8" s="155" t="n">
         <v>42829</v>
       </c>
-      <c r="E8" s="153" t="s">
+      <c r="E8" s="156" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="153" t="s">
+      <c r="A9" s="156" t="s">
         <v>325</v>
       </c>
-      <c r="B9" s="154" t="s">
+      <c r="B9" s="157" t="s">
         <v>334</v>
       </c>
-      <c r="C9" s="154"/>
-      <c r="D9" s="152" t="n">
+      <c r="C9" s="157"/>
+      <c r="D9" s="155" t="n">
         <v>42919</v>
       </c>
-      <c r="E9" s="153" t="s">
+      <c r="E9" s="156" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="153" t="s">
+      <c r="A10" s="156" t="s">
         <v>325</v>
       </c>
-      <c r="B10" s="154" t="s">
+      <c r="B10" s="157" t="s">
         <v>337</v>
       </c>
-      <c r="C10" s="154"/>
-      <c r="D10" s="152" t="n">
+      <c r="C10" s="157"/>
+      <c r="D10" s="155" t="n">
         <v>42963</v>
       </c>
-      <c r="E10" s="153" t="s">
+      <c r="E10" s="156" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="153" t="s">
+      <c r="A11" s="156" t="s">
         <v>325</v>
       </c>
-      <c r="B11" s="154" t="s">
+      <c r="B11" s="157" t="s">
         <v>339</v>
       </c>
-      <c r="C11" s="154"/>
-      <c r="D11" s="152" t="n">
+      <c r="C11" s="157"/>
+      <c r="D11" s="155" t="n">
         <v>43113</v>
       </c>
-      <c r="E11" s="153" t="s">
+      <c r="E11" s="156" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="153" t="s">
+      <c r="A12" s="156" t="s">
         <v>325</v>
       </c>
-      <c r="B12" s="154" t="n">
+      <c r="B12" s="157" t="n">
         <v>1.1</v>
       </c>
-      <c r="C12" s="154"/>
-      <c r="D12" s="152" t="n">
+      <c r="C12" s="157"/>
+      <c r="D12" s="155" t="n">
         <v>43289</v>
       </c>
-      <c r="E12" s="153" t="s">
+      <c r="E12" s="156" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="153" t="s">
+      <c r="A13" s="156" t="s">
         <v>342</v>
       </c>
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="158" t="s">
         <v>343</v>
       </c>
-      <c r="C13" s="156"/>
-      <c r="D13" s="152" t="n">
+      <c r="C13" s="159"/>
+      <c r="D13" s="155" t="n">
         <v>43464</v>
       </c>
-      <c r="E13" s="157" t="s">
+      <c r="E13" s="160" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="153" t="s">
+      <c r="A14" s="156" t="s">
         <v>345</v>
       </c>
-      <c r="B14" s="155" t="s">
+      <c r="B14" s="158" t="s">
         <v>346</v>
       </c>
-      <c r="C14" s="156"/>
-      <c r="D14" s="152" t="n">
+      <c r="C14" s="159"/>
+      <c r="D14" s="155" t="n">
         <v>43469</v>
       </c>
-      <c r="E14" s="157" t="s">
+      <c r="E14" s="160" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="409.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="158" t="s">
+      <c r="A15" s="161" t="s">
         <v>347</v>
       </c>
-      <c r="B15" s="154" t="s">
+      <c r="B15" s="157" t="s">
         <v>348</v>
       </c>
-      <c r="C15" s="154" t="s">
+      <c r="C15" s="157" t="s">
         <v>349</v>
       </c>
-      <c r="D15" s="152" t="n">
+      <c r="D15" s="155" t="n">
         <v>43471</v>
       </c>
-      <c r="E15" s="159" t="s">
+      <c r="E15" s="162" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="156" t="s">
         <v>342</v>
       </c>
-      <c r="B16" s="155" t="s">
+      <c r="B16" s="158" t="s">
         <v>351</v>
       </c>
-      <c r="C16" s="154" t="s">
+      <c r="C16" s="157" t="s">
         <v>349</v>
       </c>
-      <c r="D16" s="160" t="n">
+      <c r="D16" s="163" t="n">
         <v>43475</v>
       </c>
-      <c r="E16" s="157" t="s">
+      <c r="E16" s="160" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="78" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="158" t="s">
+      <c r="A17" s="161" t="s">
         <v>347</v>
       </c>
-      <c r="B17" s="155" t="s">
+      <c r="B17" s="158" t="s">
         <v>353</v>
       </c>
-      <c r="C17" s="154" t="s">
+      <c r="C17" s="157" t="s">
         <v>349</v>
       </c>
-      <c r="D17" s="152" t="n">
+      <c r="D17" s="155" t="n">
         <v>43476</v>
       </c>
-      <c r="E17" s="158" t="s">
+      <c r="E17" s="161" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="158" t="s">
+      <c r="A18" s="161" t="s">
         <v>347</v>
       </c>
-      <c r="B18" s="155" t="s">
+      <c r="B18" s="158" t="s">
         <v>355</v>
       </c>
-      <c r="C18" s="154" t="s">
+      <c r="C18" s="157" t="s">
         <v>349</v>
       </c>
-      <c r="D18" s="152" t="n">
+      <c r="D18" s="155" t="n">
         <v>43478</v>
       </c>
-      <c r="E18" s="158" t="s">
+      <c r="E18" s="161" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="158" t="s">
+      <c r="A19" s="161" t="s">
         <v>347</v>
       </c>
-      <c r="B19" s="155" t="s">
+      <c r="B19" s="158" t="s">
         <v>357</v>
       </c>
-      <c r="C19" s="154" t="s">
+      <c r="C19" s="157" t="s">
         <v>349</v>
       </c>
-      <c r="D19" s="152" t="n">
+      <c r="D19" s="155" t="n">
         <v>43478</v>
       </c>
-      <c r="E19" s="158" t="s">
+      <c r="E19" s="161" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="109.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="158" t="s">
+      <c r="A20" s="161" t="s">
         <v>342</v>
       </c>
-      <c r="B20" s="155" t="s">
+      <c r="B20" s="158" t="s">
         <v>359</v>
       </c>
-      <c r="C20" s="154" t="s">
+      <c r="C20" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="152" t="n">
+      <c r="D20" s="155" t="n">
         <v>43641</v>
       </c>
-      <c r="E20" s="159" t="s">
+      <c r="E20" s="162" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="158" t="s">
+      <c r="A21" s="161" t="s">
         <v>342</v>
       </c>
-      <c r="B21" s="155" t="s">
+      <c r="B21" s="158" t="s">
         <v>361</v>
       </c>
-      <c r="C21" s="154" t="s">
+      <c r="C21" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="152" t="n">
+      <c r="D21" s="155" t="n">
         <v>43642</v>
       </c>
-      <c r="E21" s="158" t="s">
+      <c r="E21" s="161" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="158" t="s">
+      <c r="A22" s="161" t="s">
         <v>342</v>
       </c>
-      <c r="B22" s="155" t="s">
+      <c r="B22" s="158" t="s">
         <v>363</v>
       </c>
-      <c r="C22" s="154" t="s">
+      <c r="C22" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="152" t="n">
+      <c r="D22" s="155" t="n">
         <v>43649</v>
       </c>
-      <c r="E22" s="158" t="s">
+      <c r="E22" s="161" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="158" t="s">
+      <c r="A23" s="161" t="s">
         <v>342</v>
       </c>
-      <c r="B23" s="155" t="s">
+      <c r="B23" s="158" t="s">
         <v>363</v>
       </c>
-      <c r="C23" s="154" t="s">
+      <c r="C23" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="152" t="n">
+      <c r="D23" s="155" t="n">
         <v>43672</v>
       </c>
-      <c r="E23" s="158" t="s">
+      <c r="E23" s="161" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="158" t="s">
+      <c r="A24" s="161" t="s">
         <v>342</v>
       </c>
-      <c r="B24" s="155" t="s">
+      <c r="B24" s="158" t="s">
         <v>363</v>
       </c>
-      <c r="C24" s="154" t="s">
+      <c r="C24" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="152" t="n">
+      <c r="D24" s="155" t="n">
         <v>43674</v>
       </c>
-      <c r="E24" s="158" t="s">
+      <c r="E24" s="161" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="158" t="s">
+      <c r="A25" s="161" t="s">
         <v>342</v>
       </c>
-      <c r="B25" s="155" t="s">
+      <c r="B25" s="158" t="s">
         <v>367</v>
       </c>
-      <c r="C25" s="154" t="s">
+      <c r="C25" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="152" t="n">
+      <c r="D25" s="155" t="n">
         <v>43685</v>
       </c>
-      <c r="E25" s="158" t="s">
+      <c r="E25" s="161" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="158" t="s">
+      <c r="A26" s="161" t="s">
         <v>369</v>
       </c>
-      <c r="B26" s="155" t="s">
+      <c r="B26" s="158" t="s">
         <v>367</v>
       </c>
-      <c r="C26" s="154" t="s">
+      <c r="C26" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="152" t="n">
+      <c r="D26" s="155" t="n">
         <v>43719</v>
       </c>
-      <c r="E26" s="158" t="s">
+      <c r="E26" s="161" t="s">
         <v>370</v>
       </c>
     </row>

</xml_diff>

<commit_message>
iOS Security Requiments V2 translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -1915,7 +1915,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="166">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2472,15 +2472,23 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2742,7 +2750,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2922,11 +2930,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="28478417"/>
-        <c:axId val="88615930"/>
+        <c:axId val="61365850"/>
+        <c:axId val="10755112"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="28478417"/>
+        <c:axId val="61365850"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2966,7 +2974,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88615930"/>
+        <c:crossAx val="10755112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2974,7 +2982,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88615930"/>
+        <c:axId val="10755112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3017,7 +3025,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28478417"/>
+        <c:crossAx val="61365850"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3077,7 +3085,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3257,11 +3265,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="71759975"/>
-        <c:axId val="16537529"/>
+        <c:axId val="42571708"/>
+        <c:axId val="65343306"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="71759975"/>
+        <c:axId val="42571708"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3301,7 +3309,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16537529"/>
+        <c:crossAx val="65343306"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3309,7 +3317,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="16537529"/>
+        <c:axId val="65343306"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3352,7 +3360,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71759975"/>
+        <c:crossAx val="42571708"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4542,7 +4550,7 @@
   <dimension ref="B1:M85"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4929,8 +4937,8 @@
       </c>
       <c r="G16" s="70"/>
       <c r="H16" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-local-storage-for-sensitive-data-mstg-storage-1-and-mstg-storage-2"),"Проверка наличия конфиденциальных даннх на локальном хранилище (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
-        <v>Проверка наличия конфиденциальных даннх на локальном хранилище (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05d-Testing-Data-Storage.md#testing-local-storage-for-sensitive-data-mstg-storage-1-and-mstg-storage-2"),"Проверка наличия конфиденциальных данных на локальном хранилище (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
+        <v>Проверка наличия конфиденциальных данных на локальном хранилище (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
       <c r="I16" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x05e-Testing-Cryptography.md#testing-key-management-mstg-storage-1-mstg-crypto-1-and-mstg-crypto-5"),"Проверка системы управления ключами (MSTG-STORAGE-1, MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
@@ -7023,8 +7031,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7383,7 +7391,7 @@
       <c r="J15" s="85"/>
       <c r="K15" s="95"/>
     </row>
-    <row r="16" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="87" t="s">
         <v>95</v>
       </c>
@@ -7400,9 +7408,9 @@
         <v>64</v>
       </c>
       <c r="G16" s="70"/>
-      <c r="H16" s="139" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-local-data-storage-mstg-storage-1-and-mstg-storage-2"),"Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
-        <v>Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
+      <c r="H16" s="90" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-local-data-storage-mstg-storage-1-and-mstg-storage-2"),"Проверка наличия конфиденциальных данных на локальном хранилище (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
+        <v>Проверка наличия конфиденциальных данных на локальном хранилище (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
       <c r="I16" s="76"/>
       <c r="J16" s="76"/>
@@ -7421,9 +7429,9 @@
       <c r="E17" s="68"/>
       <c r="F17" s="69"/>
       <c r="G17" s="70"/>
-      <c r="H17" s="139" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-local-data-storage-mstg-storage-1-and-mstg-storage-2"),"Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
-        <v>Testing Local Data Storage (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
+      <c r="H17" s="90" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-local-data-storage-mstg-storage-1-and-mstg-storage-2"),"Проверка наличия конфиденциальных данных на локальном хранилище (MSTG-STORAGE-1 and MSTG-STORAGE-2)")</f>
+        <v>Проверка наличия конфиденциальных данных на локальном хранилище (MSTG-STORAGE-1 and MSTG-STORAGE-2)</v>
       </c>
       <c r="I17" s="76"/>
       <c r="J17" s="76"/>
@@ -7446,15 +7454,15 @@
         <v>64</v>
       </c>
       <c r="G18" s="70"/>
-      <c r="H18" s="139" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#checking-logs-for-sensitive-data-mstg-storage-3"),"Checking Logs for Sensitive Data (MSTG-STORAGE-3)")</f>
-        <v>Checking Logs for Sensitive Data (MSTG-STORAGE-3)</v>
+      <c r="H18" s="90" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#checking-logs-for-sensitive-data-mstg-storage-3"),"Проверка наличия конфиденциальных данных в записях лога (MSTG-STORAGE-3)")</f>
+        <v>Проверка наличия конфиденциальных данных в записях лога (MSTG-STORAGE-3)</v>
       </c>
       <c r="I18" s="76"/>
       <c r="J18" s="76"/>
       <c r="K18" s="73"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="87" t="s">
         <v>104</v>
       </c>
@@ -7472,8 +7480,8 @@
       </c>
       <c r="G19" s="70"/>
       <c r="H19" s="139" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-sent-to-third-parties-mstg-storage-4"),"Determining Whether Sensitive Data Is Sent to Third Parties (MSTG-STORAGE-4)")</f>
-        <v>Determining Whether Sensitive Data Is Sent to Third Parties (MSTG-STORAGE-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-sent-to-third-parties-mstg-storage-4"),"Проверка передачи конфиденциальных данных третим сторонам (MSTG-STORAGE-4)")</f>
+        <v>Проверка передачи конфиденциальных данных третим сторонам (MSTG-STORAGE-4)</v>
       </c>
       <c r="I19" s="76"/>
       <c r="J19" s="76"/>
@@ -7497,14 +7505,14 @@
       </c>
       <c r="G20" s="70"/>
       <c r="H20" s="139" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#finding-sensitive-data-in-the-keyboard-cache-mstg-storage-5"),"Finding Sensitive Data in the Keyboard Cache (MSTG-STORAGE-5)")</f>
-        <v>Finding Sensitive Data in the Keyboard Cache (MSTG-STORAGE-5)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#finding-sensitive-data-in-the-keyboard-cache-mstg-storage-5"),"Проверка отключения кэша клавиатуры для полей ввода текста (MSTG-STORAGE-5)")</f>
+        <v>Проверка отключения кэша клавиатуры для полей ввода текста (MSTG-STORAGE-5)</v>
       </c>
       <c r="I20" s="76"/>
       <c r="J20" s="76"/>
       <c r="K20" s="73"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="87" t="s">
         <v>110</v>
       </c>
@@ -7521,9 +7529,9 @@
         <v>64</v>
       </c>
       <c r="G21" s="70"/>
-      <c r="H21" s="140" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-exposed-via-ipc-mechanisms-mstg-storage-6"),"Determining Whether Sensitive Data Is Exposed via IPC Mechanisms (MSTG-STORAGE-6)")</f>
-        <v>Determining Whether Sensitive Data Is Exposed via IPC Mechanisms (MSTG-STORAGE-6)</v>
+      <c r="H21" s="139" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-exposed-via-ipc-mechanisms-mstg-storage-6"),"Проверка передачи конфиденциальных данных при обмене данными между потоками (IPC) (MSTG-STORAGE-6)")</f>
+        <v>Проверка передачи конфиденциальных данных при обмене данными между потоками (IPC) (MSTG-STORAGE-6)</v>
       </c>
       <c r="I21" s="76"/>
       <c r="J21" s="76"/>
@@ -7546,9 +7554,9 @@
         <v>64</v>
       </c>
       <c r="G22" s="70"/>
-      <c r="H22" s="139" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#checking-for-sensitive-data-disclosed-through-the-user-interface-mstg-storage-7"),"Checking for Sensitive Data Disclosed Through the User Interface (MSTG-STORAGE-7)")</f>
-        <v>Checking for Sensitive Data Disclosed Through the User Interface (MSTG-STORAGE-7)</v>
+      <c r="H22" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#checking-for-sensitive-data-disclosed-through-the-user-interface-mstg-storage-7"),"Проверка раскрытия конфиденциальных данных через пользовательский интерфейс (MSTG-STORAGE-7)")</f>
+        <v>Проверка раскрытия конфиденциальных данных через пользовательский интерфейс (MSTG-STORAGE-7)</v>
       </c>
       <c r="I22" s="76"/>
       <c r="J22" s="76"/>
@@ -7571,9 +7579,9 @@
       <c r="G23" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H23" s="139" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-backups-for-sensitive-data-mstg-storage-8"),"Testing Backups for Sensitive Data (MSTG-STORAGE-8)")</f>
-        <v>Testing Backups for Sensitive Data (MSTG-STORAGE-8)</v>
+      <c r="H23" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-backups-for-sensitive-data-mstg-storage-8"),"Тестирование бэкапов на наличие конфиденциальных данных (MSTG-STORAGE-8)")</f>
+        <v>Тестирование бэкапов на наличие конфиденциальных данных (MSTG-STORAGE-8)</v>
       </c>
       <c r="I23" s="76"/>
       <c r="J23" s="76"/>
@@ -7596,9 +7604,9 @@
       <c r="G24" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H24" s="139" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-auto-generated-screenshots-for-sensitive-information-mstg-storage-9"),"Testing Auto-Generated Screenshots for Sensitive Information (MSTG-STORAGE-9)")</f>
-        <v>Testing Auto-Generated Screenshots for Sensitive Information (MSTG-STORAGE-9)</v>
+      <c r="H24" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-auto-generated-screenshots-for-sensitive-information-mstg-storage-9"),"Поиск конфиденциальных данных в автоматически генерируемых снимках экрана (MSTG-STORAGE-9)")</f>
+        <v>Поиск конфиденциальных данных в автоматически генерируемых снимках экрана (MSTG-STORAGE-9)</v>
       </c>
       <c r="I24" s="76"/>
       <c r="J24" s="76"/>
@@ -7621,9 +7629,9 @@
       <c r="G25" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H25" s="139" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-memory-for-sensitive-data-mstg-storage-10"),"Testing Memory for Sensitive Data (MSTG-STORAGE-10)")</f>
-        <v>Testing Memory for Sensitive Data (MSTG-STORAGE-10)</v>
+      <c r="H25" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06d-Testing-Data-Storage.md#testing-memory-for-sensitive-data-mstg-storage-10"),"Проверка памяти на конфиденциальные данные (MSTG-STORAGE-10)")</f>
+        <v>Проверка памяти на конфиденциальные данные (MSTG-STORAGE-10)</v>
       </c>
       <c r="I25" s="76"/>
       <c r="J25" s="76"/>
@@ -7646,9 +7654,9 @@
       <c r="G26" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H26" s="139" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06f-Testing-Local-Authentication.md#testing-local-authentication-mstg-auth-8-and-mstg-storage-11"),"Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)")</f>
-        <v>Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)</v>
+      <c r="H26" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06f-Testing-Local-Authentication.md#testing-local-authentication-mstg-auth-8-and-mstg-storage-11"),"Проверка политики безопасности доступа к устройству (MSTG-STORAGE-11)")</f>
+        <v>Проверка политики безопасности доступа к устройству (MSTG-STORAGE-11)</v>
       </c>
       <c r="I26" s="76"/>
       <c r="J26" s="76"/>
@@ -7672,9 +7680,9 @@
       <c r="G27" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H27" s="100" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04i-Testing-user-interaction.md#testing-user-education-mstg-storage-12"),"Testing User Education (MSTG-STORAGE-12)")</f>
-        <v>Testing User Education (MSTG-STORAGE-12)</v>
+      <c r="H27" s="142" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04i-Testing-user-interaction.md#testing-user-education-mstg-storage-12"),"Проверка знаний пользователей (MSTG-STORAGE-12)")</f>
+        <v>Проверка знаний пользователей (MSTG-STORAGE-12)</v>
       </c>
       <c r="I27" s="76"/>
       <c r="J27" s="76"/>
@@ -7714,7 +7722,7 @@
         <v>64</v>
       </c>
       <c r="G29" s="70"/>
-      <c r="H29" s="139" t="str">
+      <c r="H29" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
@@ -7739,7 +7747,7 @@
         <v>64</v>
       </c>
       <c r="G30" s="70"/>
-      <c r="H30" s="140" t="str">
+      <c r="H30" s="143" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#verifying-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-and-mstg-crypto-3"),"Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
@@ -7764,7 +7772,7 @@
         <v>64</v>
       </c>
       <c r="G31" s="70"/>
-      <c r="H31" s="140" t="str">
+      <c r="H31" s="143" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#verifying-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-and-mstg-crypto-3"),"Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
         <v>Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
@@ -7789,7 +7797,7 @@
         <v>64</v>
       </c>
       <c r="G32" s="70"/>
-      <c r="H32" s="139" t="str">
+      <c r="H32" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#identifying-insecure-andor-deprecated-cryptographic-algorithms-mstg-crypto-4"),"Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)")</f>
         <v>Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)</v>
       </c>
@@ -7814,7 +7822,7 @@
         <v>64</v>
       </c>
       <c r="G33" s="70"/>
-      <c r="H33" s="139" t="str">
+      <c r="H33" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
         <v>Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
@@ -7839,7 +7847,7 @@
         <v>64</v>
       </c>
       <c r="G34" s="70"/>
-      <c r="H34" s="139" t="str">
+      <c r="H34" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-random-number-generation-mstg-crypto-6")," Testing Random Number Generation (MSTG-CRYPTO-6)")</f>
         <v> Testing Random Number Generation (MSTG-CRYPTO-6)</v>
       </c>
@@ -7880,7 +7888,7 @@
         <v>64</v>
       </c>
       <c r="G36" s="70"/>
-      <c r="H36" s="139" t="str">
+      <c r="H36" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
         <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
       </c>
@@ -7888,7 +7896,7 @@
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
-      <c r="J36" s="142"/>
+      <c r="J36" s="144"/>
       <c r="K36" s="125"/>
     </row>
     <row r="37" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7908,7 +7916,7 @@
         <v>64</v>
       </c>
       <c r="G37" s="70"/>
-      <c r="H37" s="139" t="str">
+      <c r="H37" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateful-session-management-mstg-auth-2"),"Testing Stateful Session Management (MSTG-AUTH-2)")</f>
         <v>Testing Stateful Session Management (MSTG-AUTH-2)</v>
       </c>
@@ -7933,7 +7941,7 @@
         <v>64</v>
       </c>
       <c r="G38" s="70"/>
-      <c r="H38" s="139" t="str">
+      <c r="H38" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateless-token-based-authentication-mstg-auth-3"),"Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)")</f>
         <v>Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)</v>
       </c>
@@ -7941,7 +7949,7 @@
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
         <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
-      <c r="J38" s="142"/>
+      <c r="J38" s="144"/>
       <c r="K38" s="125"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7957,7 +7965,7 @@
       <c r="E39" s="68"/>
       <c r="F39" s="69"/>
       <c r="G39" s="70"/>
-      <c r="H39" s="139" t="str">
+      <c r="H39" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-user-logout-mstg-auth-4"),"Testing User Logout (MSTG-AUTH-4)")</f>
         <v>Testing User Logout (MSTG-AUTH-4)</v>
       </c>
@@ -7983,7 +7991,7 @@
         <v>64</v>
       </c>
       <c r="G40" s="70"/>
-      <c r="H40" s="139" t="str">
+      <c r="H40" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
         <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
@@ -8009,7 +8017,7 @@
         <v>64</v>
       </c>
       <c r="G41" s="70"/>
-      <c r="H41" s="139" t="str">
+      <c r="H41" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
         <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
@@ -8017,7 +8025,7 @@
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#dynamic-testing-mstg-auth-6"),"Dynamic Testing (MSTG-AUTH-6)")</f>
         <v>Dynamic Testing (MSTG-AUTH-6)</v>
       </c>
-      <c r="J41" s="142"/>
+      <c r="J41" s="144"/>
       <c r="K41" s="125"/>
     </row>
     <row r="42" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8037,12 +8045,12 @@
         <v>64</v>
       </c>
       <c r="G42" s="70"/>
-      <c r="H42" s="139" t="str">
+      <c r="H42" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-session-timeout-mstg-auth-7"),"Testing Session Timeout (MSTG-AUTH-7)")</f>
         <v>Testing Session Timeout (MSTG-AUTH-7)</v>
       </c>
       <c r="I42" s="97"/>
-      <c r="J42" s="143"/>
+      <c r="J42" s="145"/>
       <c r="K42" s="99"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8062,12 +8070,12 @@
       <c r="G43" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H43" s="139" t="str">
+      <c r="H43" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06f-Testing-Local-Authentication.md#testing-local-authentication-mstg-auth-8-and-mstg-storage-11"),"Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)")</f>
         <v>Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)</v>
       </c>
       <c r="I43" s="90"/>
-      <c r="J43" s="142"/>
+      <c r="J43" s="144"/>
       <c r="K43" s="125"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8087,7 +8095,7 @@
       <c r="G44" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H44" s="140" t="str">
+      <c r="H44" s="143" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
@@ -8112,7 +8120,7 @@
       <c r="G45" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H45" s="140" t="str">
+      <c r="H45" s="143" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
@@ -8137,7 +8145,7 @@
       <c r="G46" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H46" s="144" t="str">
+      <c r="H46" s="146" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04e-Testing-Authentication-and-Session-Management.md#testing-login-activity-and-device-blocking-mstg-auth-11"), "Testing Login Activity and Device Blocking (MSTG-AUTH-11)")</f>
         <v>Testing Login Activity and Device Blocking (MSTG-AUTH-11)</v>
       </c>
@@ -8178,7 +8186,7 @@
         <v>64</v>
       </c>
       <c r="G48" s="70"/>
-      <c r="H48" s="140" t="str">
+      <c r="H48" s="143" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
@@ -8203,7 +8211,7 @@
         <v>64</v>
       </c>
       <c r="G49" s="70"/>
-      <c r="H49" s="140" t="str">
+      <c r="H49" s="143" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
@@ -8231,7 +8239,7 @@
         <v>64</v>
       </c>
       <c r="G50" s="70"/>
-      <c r="H50" s="139" t="str">
+      <c r="H50" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-3-and-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)")</f>
         <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)</v>
       </c>
@@ -8256,7 +8264,7 @@
       <c r="G51" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H51" s="139" t="str">
+      <c r="H51" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-3-and-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)")</f>
         <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)</v>
       </c>
@@ -8281,7 +8289,7 @@
       <c r="G52" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H52" s="140" t="str">
+      <c r="H52" s="143" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels-mstg-network-5"),"Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)")</f>
         <v>Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)</v>
       </c>
@@ -8306,7 +8314,7 @@
       <c r="G53" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H53" s="139" t="str">
+      <c r="H53" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x06i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"), "Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
         <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
       </c>
@@ -8347,7 +8355,7 @@
         <v>64</v>
       </c>
       <c r="G55" s="70"/>
-      <c r="H55" s="139" t="str">
+      <c r="H55" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-app-permissions-mstg-platform-1"),"Testing App Permissions (MSTG-PLATFORM-1)")</f>
         <v>Testing App Permissions (MSTG-PLATFORM-1)</v>
       </c>
@@ -8372,7 +8380,7 @@
         <v>64</v>
       </c>
       <c r="G56" s="70"/>
-      <c r="H56" s="139" t="str">
+      <c r="H56" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"),"Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
         <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
@@ -8397,7 +8405,7 @@
         <v>64</v>
       </c>
       <c r="G57" s="70"/>
-      <c r="H57" s="139" t="str">
+      <c r="H57" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-custom-url-schemes-mstg-platform-3"),"Testing Custom URL Schemes (MSTG-PLATFORM-3)")</f>
         <v>Testing Custom URL Schemes (MSTG-PLATFORM-3)</v>
       </c>
@@ -8447,7 +8455,7 @@
         <v>64</v>
       </c>
       <c r="G59" s="70"/>
-      <c r="H59" s="139" t="str">
+      <c r="H59" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-ios-webviews-mstg-platform-5"),"Testing iOS WebViews (MSTG-PLATFORM-5)")</f>
         <v>Testing iOS WebViews (MSTG-PLATFORM-5)</v>
       </c>
@@ -8472,7 +8480,7 @@
         <v>64</v>
       </c>
       <c r="G60" s="70"/>
-      <c r="H60" s="139" t="str">
+      <c r="H60" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-webview-protocol-handlers-mstg-platform-6"),"Testing WebView Protocol Handlers (MSTG-PLATFORM-6)")</f>
         <v>Testing WebView Protocol Handlers (MSTG-PLATFORM-6)</v>
       </c>
@@ -8497,7 +8505,7 @@
         <v>64</v>
       </c>
       <c r="G61" s="70"/>
-      <c r="H61" s="139" t="str">
+      <c r="H61" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#determining-whether-native-methods-are-exposed-through-webviews-mstg-platform-7"),"Determining Whether Native Methods Are Exposed Through WebViews (MSTG-PLATFORM-7)")</f>
         <v>Determining Whether Native Methods Are Exposed Through WebViews (MSTG-PLATFORM-7)</v>
       </c>
@@ -8522,7 +8530,7 @@
         <v>64</v>
       </c>
       <c r="G62" s="70"/>
-      <c r="H62" s="139" t="str">
+      <c r="H62" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-object-persistence-mstg-platform-8"),"Testing Object Persistence (MSTG-PLATFORM-8)")</f>
         <v>Testing Object Persistence (MSTG-PLATFORM-8)</v>
       </c>
@@ -8563,7 +8571,7 @@
         <v>64</v>
       </c>
       <c r="G64" s="70"/>
-      <c r="H64" s="139" t="str">
+      <c r="H64" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#making-sure-that-the-app-is-properly-signed-mstg-code-1"),"Making Sure that the App Is Properly Signed (MSTG-CODE-1)")</f>
         <v>Making Sure that the App Is Properly Signed (MSTG-CODE-1)</v>
       </c>
@@ -8588,7 +8596,7 @@
         <v>64</v>
       </c>
       <c r="G65" s="70"/>
-      <c r="H65" s="139" t="str">
+      <c r="H65" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#determining-whether-the-app-is-debuggable-mstg-code-2"),"Determining Whether the App is Debuggable (MSTG-CODE-2)")</f>
         <v>Determining Whether the App is Debuggable (MSTG-CODE-2)</v>
       </c>
@@ -8613,7 +8621,7 @@
         <v>64</v>
       </c>
       <c r="G66" s="70"/>
-      <c r="H66" s="139" t="str">
+      <c r="H66" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-symbols-mstg-code-3"),"Finding Debugging Symbols (MSTG-CODE-3)")</f>
         <v>Finding Debugging Symbols (MSTG-CODE-3)</v>
       </c>
@@ -8638,7 +8646,7 @@
         <v>64</v>
       </c>
       <c r="G67" s="70"/>
-      <c r="H67" s="139" t="str">
+      <c r="H67" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-code-and-verbose-error-logging-mstg-code-4"),"Finding Debugging Code and Verbose Error Logging (MSTG-CODE-4)")</f>
         <v>Finding Debugging Code and Verbose Error Logging (MSTG-CODE-4)</v>
       </c>
@@ -8663,7 +8671,7 @@
         <v>64</v>
       </c>
       <c r="G68" s="70"/>
-      <c r="H68" s="144" t="str">
+      <c r="H68" s="146" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"),"Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
         <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
       </c>
@@ -8688,7 +8696,7 @@
         <v>64</v>
       </c>
       <c r="G69" s="70"/>
-      <c r="H69" s="139" t="str">
+      <c r="H69" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6"),"Testing Exception Handling (MSTG-CODE-6)")</f>
         <v>Testing Exception Handling (MSTG-CODE-6)</v>
       </c>
@@ -8713,7 +8721,7 @@
         <v>64</v>
       </c>
       <c r="G70" s="70"/>
-      <c r="H70" s="139" t="str">
+      <c r="H70" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6"),"Testing Exception Handling (MSTG-CODE-6)")</f>
         <v>Testing Exception Handling (MSTG-CODE-6)</v>
       </c>
@@ -8738,7 +8746,7 @@
         <v>64</v>
       </c>
       <c r="G71" s="70"/>
-      <c r="H71" s="139" t="str">
+      <c r="H71" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#memory-corruption-bugs-mstg-code-8"),"Memory Corruption Bugs (MSTG-CODE-8)")</f>
         <v>Memory Corruption Bugs (MSTG-CODE-8)</v>
       </c>
@@ -8763,7 +8771,7 @@
         <v>64</v>
       </c>
       <c r="G72" s="70"/>
-      <c r="H72" s="139" t="str">
+      <c r="H72" s="90" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#make-sure-that-free-security-features-are-activated-mstg-code-9"),"Make Sure That Free Security Features Are Activated (MSTG-CODE-9)")</f>
         <v>Make Sure That Free Security Features Are Activated (MSTG-CODE-9)</v>
       </c>
@@ -8780,12 +8788,12 @@
       <c r="G73" s="108"/>
       <c r="H73" s="108"/>
       <c r="I73" s="109"/>
-      <c r="J73" s="145"/>
-      <c r="K73" s="146"/>
+      <c r="J73" s="147"/>
+      <c r="K73" s="148"/>
     </row>
     <row r="74" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="147"/>
-      <c r="C74" s="147"/>
+      <c r="B74" s="149"/>
+      <c r="C74" s="149"/>
       <c r="D74" s="92"/>
       <c r="E74" s="114"/>
       <c r="F74" s="114"/>
@@ -8796,8 +8804,8 @@
       <c r="K74" s="92"/>
     </row>
     <row r="75" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="147"/>
-      <c r="C75" s="147"/>
+      <c r="B75" s="149"/>
+      <c r="C75" s="149"/>
       <c r="D75" s="92"/>
       <c r="E75" s="114"/>
       <c r="F75" s="114"/>
@@ -8808,8 +8816,8 @@
       <c r="K75" s="92"/>
     </row>
     <row r="76" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="147"/>
-      <c r="C76" s="147"/>
+      <c r="B76" s="149"/>
+      <c r="C76" s="149"/>
       <c r="D76" s="92"/>
       <c r="E76" s="114"/>
       <c r="F76" s="114"/>
@@ -8898,8 +8906,8 @@
       <c r="K81" s="92"/>
     </row>
     <row r="82" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="147"/>
-      <c r="C82" s="147"/>
+      <c r="B82" s="149"/>
+      <c r="C82" s="149"/>
       <c r="D82" s="92"/>
       <c r="E82" s="114"/>
       <c r="F82" s="114"/>
@@ -8910,8 +8918,8 @@
       <c r="K82" s="92"/>
     </row>
     <row r="83" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="147"/>
-      <c r="C83" s="147"/>
+      <c r="B83" s="149"/>
+      <c r="C83" s="149"/>
       <c r="D83" s="92"/>
       <c r="E83" s="114"/>
       <c r="F83" s="114"/>
@@ -8922,8 +8930,8 @@
       <c r="K83" s="92"/>
     </row>
     <row r="84" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="147"/>
-      <c r="C84" s="147"/>
+      <c r="B84" s="149"/>
+      <c r="C84" s="149"/>
       <c r="D84" s="92"/>
       <c r="E84" s="114"/>
       <c r="F84" s="114"/>
@@ -8934,8 +8942,8 @@
       <c r="K84" s="92"/>
     </row>
     <row r="85" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="147"/>
-      <c r="C85" s="147"/>
+      <c r="B85" s="149"/>
+      <c r="C85" s="149"/>
       <c r="D85" s="92"/>
       <c r="E85" s="114"/>
       <c r="F85" s="114"/>
@@ -8954,7 +8962,7 @@
       <formula>NOT(ISERROR(SEARCH("0x05",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15:H26 H28:H1048576 H1:H2 H4 H13">
+  <conditionalFormatting sqref="H28:H1048576 H1:H2 H4 H13 H15:H18">
     <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="3">
       <formula>NOT(ISERROR(SEARCH("0x05",H1)))</formula>
     </cfRule>
@@ -9139,7 +9147,7 @@
       <c r="F8" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="148" t="s">
+      <c r="G8" s="150" t="s">
         <v>298</v>
       </c>
       <c r="H8" s="125"/>
@@ -9160,7 +9168,7 @@
       <c r="F9" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G9" s="148" t="s">
+      <c r="G9" s="150" t="s">
         <v>298</v>
       </c>
       <c r="H9" s="125"/>
@@ -9181,7 +9189,7 @@
       <c r="F10" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="148" t="s">
+      <c r="G10" s="150" t="s">
         <v>298</v>
       </c>
       <c r="H10" s="125"/>
@@ -9244,7 +9252,7 @@
       <c r="F13" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="148" t="s">
+      <c r="G13" s="150" t="s">
         <v>298</v>
       </c>
       <c r="H13" s="125"/>
@@ -9309,7 +9317,7 @@
       <c r="F17" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="149" t="str">
+      <c r="G17" s="151" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks-mstg-resilience-3-and-mstg-resilience-11"),"File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)")</f>
         <v>File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)</v>
       </c>
@@ -9346,8 +9354,8 @@
       <c r="H19" s="110"/>
     </row>
     <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="147"/>
-      <c r="C20" s="147"/>
+      <c r="B20" s="149"/>
+      <c r="C20" s="149"/>
       <c r="D20" s="92"/>
       <c r="E20" s="114"/>
       <c r="F20" s="114"/>
@@ -9355,8 +9363,8 @@
       <c r="H20" s="92"/>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="147"/>
-      <c r="C21" s="147"/>
+      <c r="B21" s="149"/>
+      <c r="C21" s="149"/>
       <c r="D21" s="92"/>
       <c r="E21" s="114"/>
       <c r="F21" s="114"/>
@@ -9427,8 +9435,8 @@
       <c r="H26" s="92"/>
     </row>
     <row r="27" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="147"/>
-      <c r="C27" s="147"/>
+      <c r="B27" s="149"/>
+      <c r="C27" s="149"/>
       <c r="D27" s="92"/>
       <c r="E27" s="114"/>
       <c r="F27" s="114"/>
@@ -9436,8 +9444,8 @@
       <c r="H27" s="92"/>
     </row>
     <row r="28" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="147"/>
-      <c r="C28" s="147"/>
+      <c r="B28" s="149"/>
+      <c r="C28" s="149"/>
       <c r="D28" s="92"/>
       <c r="E28" s="114"/>
       <c r="F28" s="114"/>
@@ -9445,8 +9453,8 @@
       <c r="H28" s="92"/>
     </row>
     <row r="29" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="147"/>
-      <c r="C29" s="147"/>
+      <c r="B29" s="149"/>
+      <c r="C29" s="149"/>
       <c r="D29" s="92"/>
       <c r="E29" s="114"/>
       <c r="F29" s="114"/>
@@ -9454,22 +9462,22 @@
       <c r="H29" s="92"/>
     </row>
     <row r="30" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="147"/>
-      <c r="C30" s="147"/>
+      <c r="B30" s="149"/>
+      <c r="C30" s="149"/>
       <c r="D30" s="92"/>
       <c r="E30" s="114"/>
       <c r="F30" s="114"/>
     </row>
     <row r="31" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="147"/>
-      <c r="C31" s="147"/>
+      <c r="B31" s="149"/>
+      <c r="C31" s="149"/>
       <c r="D31" s="92"/>
       <c r="E31" s="114"/>
       <c r="F31" s="114"/>
     </row>
     <row r="32" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="147"/>
-      <c r="C32" s="147"/>
+      <c r="B32" s="149"/>
+      <c r="C32" s="149"/>
       <c r="D32" s="92"/>
       <c r="E32" s="114"/>
       <c r="F32" s="114"/>
@@ -9550,412 +9558,412 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="152" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="151"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="153"/>
       <c r="D1" s="52"/>
       <c r="E1" s="52"/>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="152" t="s">
+      <c r="A2" s="154" t="s">
         <v>319</v>
       </c>
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="154" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="152" t="s">
+      <c r="C2" s="154" t="s">
         <v>321</v>
       </c>
-      <c r="D2" s="152" t="s">
+      <c r="D2" s="154" t="s">
         <v>322</v>
       </c>
-      <c r="E2" s="152" t="s">
+      <c r="E2" s="154" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="153" t="s">
+      <c r="A3" s="155" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="154" t="n">
+      <c r="B3" s="156" t="n">
         <v>0.1</v>
       </c>
-      <c r="C3" s="154"/>
-      <c r="D3" s="155" t="n">
+      <c r="C3" s="156"/>
+      <c r="D3" s="157" t="n">
         <v>42765</v>
       </c>
-      <c r="E3" s="156" t="s">
+      <c r="E3" s="158" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="156" t="s">
+      <c r="A4" s="158" t="s">
         <v>325</v>
       </c>
-      <c r="B4" s="154" t="n">
+      <c r="B4" s="156" t="n">
         <v>0.2</v>
       </c>
-      <c r="C4" s="154"/>
-      <c r="D4" s="155" t="n">
+      <c r="C4" s="156"/>
+      <c r="D4" s="157" t="n">
         <v>42766</v>
       </c>
-      <c r="E4" s="156" t="s">
+      <c r="E4" s="158" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="156" t="s">
+      <c r="A5" s="158" t="s">
         <v>327</v>
       </c>
-      <c r="B5" s="154" t="n">
+      <c r="B5" s="156" t="n">
         <v>0.3</v>
       </c>
-      <c r="C5" s="154"/>
-      <c r="D5" s="155" t="n">
+      <c r="C5" s="156"/>
+      <c r="D5" s="157" t="n">
         <v>42778</v>
       </c>
-      <c r="E5" s="156" t="s">
+      <c r="E5" s="158" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="158" t="s">
         <v>329</v>
       </c>
-      <c r="B6" s="154" t="s">
+      <c r="B6" s="156" t="s">
         <v>330</v>
       </c>
-      <c r="C6" s="154"/>
-      <c r="D6" s="155" t="n">
+      <c r="C6" s="156"/>
+      <c r="D6" s="157" t="n">
         <v>42780</v>
       </c>
-      <c r="E6" s="156" t="s">
+      <c r="E6" s="158" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="156" t="s">
+      <c r="A7" s="158" t="s">
         <v>325</v>
       </c>
-      <c r="B7" s="157" t="s">
+      <c r="B7" s="159" t="s">
         <v>332</v>
       </c>
-      <c r="C7" s="157"/>
-      <c r="D7" s="155" t="n">
+      <c r="C7" s="159"/>
+      <c r="D7" s="157" t="n">
         <v>42781</v>
       </c>
-      <c r="E7" s="156" t="s">
+      <c r="E7" s="158" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="156" t="s">
+      <c r="A8" s="158" t="s">
         <v>329</v>
       </c>
-      <c r="B8" s="157" t="s">
+      <c r="B8" s="159" t="s">
         <v>334</v>
       </c>
-      <c r="C8" s="157"/>
-      <c r="D8" s="155" t="n">
+      <c r="C8" s="159"/>
+      <c r="D8" s="157" t="n">
         <v>42829</v>
       </c>
-      <c r="E8" s="156" t="s">
+      <c r="E8" s="158" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="156" t="s">
+      <c r="A9" s="158" t="s">
         <v>325</v>
       </c>
-      <c r="B9" s="157" t="s">
+      <c r="B9" s="159" t="s">
         <v>334</v>
       </c>
-      <c r="C9" s="157"/>
-      <c r="D9" s="155" t="n">
+      <c r="C9" s="159"/>
+      <c r="D9" s="157" t="n">
         <v>42919</v>
       </c>
-      <c r="E9" s="156" t="s">
+      <c r="E9" s="158" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="156" t="s">
+      <c r="A10" s="158" t="s">
         <v>325</v>
       </c>
-      <c r="B10" s="157" t="s">
+      <c r="B10" s="159" t="s">
         <v>337</v>
       </c>
-      <c r="C10" s="157"/>
-      <c r="D10" s="155" t="n">
+      <c r="C10" s="159"/>
+      <c r="D10" s="157" t="n">
         <v>42963</v>
       </c>
-      <c r="E10" s="156" t="s">
+      <c r="E10" s="158" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="156" t="s">
+      <c r="A11" s="158" t="s">
         <v>325</v>
       </c>
-      <c r="B11" s="157" t="s">
+      <c r="B11" s="159" t="s">
         <v>339</v>
       </c>
-      <c r="C11" s="157"/>
-      <c r="D11" s="155" t="n">
+      <c r="C11" s="159"/>
+      <c r="D11" s="157" t="n">
         <v>43113</v>
       </c>
-      <c r="E11" s="156" t="s">
+      <c r="E11" s="158" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="156" t="s">
+      <c r="A12" s="158" t="s">
         <v>325</v>
       </c>
-      <c r="B12" s="157" t="n">
+      <c r="B12" s="159" t="n">
         <v>1.1</v>
       </c>
-      <c r="C12" s="157"/>
-      <c r="D12" s="155" t="n">
+      <c r="C12" s="159"/>
+      <c r="D12" s="157" t="n">
         <v>43289</v>
       </c>
-      <c r="E12" s="156" t="s">
+      <c r="E12" s="158" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="156" t="s">
+      <c r="A13" s="158" t="s">
         <v>342</v>
       </c>
-      <c r="B13" s="158" t="s">
+      <c r="B13" s="160" t="s">
         <v>343</v>
       </c>
-      <c r="C13" s="159"/>
-      <c r="D13" s="155" t="n">
+      <c r="C13" s="161"/>
+      <c r="D13" s="157" t="n">
         <v>43464</v>
       </c>
-      <c r="E13" s="160" t="s">
+      <c r="E13" s="162" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="156" t="s">
+      <c r="A14" s="158" t="s">
         <v>345</v>
       </c>
-      <c r="B14" s="158" t="s">
+      <c r="B14" s="160" t="s">
         <v>346</v>
       </c>
-      <c r="C14" s="159"/>
-      <c r="D14" s="155" t="n">
+      <c r="C14" s="161"/>
+      <c r="D14" s="157" t="n">
         <v>43469</v>
       </c>
-      <c r="E14" s="160" t="s">
+      <c r="E14" s="162" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="409.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="161" t="s">
+      <c r="A15" s="163" t="s">
         <v>347</v>
       </c>
-      <c r="B15" s="157" t="s">
+      <c r="B15" s="159" t="s">
         <v>348</v>
       </c>
-      <c r="C15" s="157" t="s">
+      <c r="C15" s="159" t="s">
         <v>349</v>
       </c>
-      <c r="D15" s="155" t="n">
+      <c r="D15" s="157" t="n">
         <v>43471</v>
       </c>
-      <c r="E15" s="162" t="s">
+      <c r="E15" s="164" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="156" t="s">
+      <c r="A16" s="158" t="s">
         <v>342</v>
       </c>
-      <c r="B16" s="158" t="s">
+      <c r="B16" s="160" t="s">
         <v>351</v>
       </c>
-      <c r="C16" s="157" t="s">
+      <c r="C16" s="159" t="s">
         <v>349</v>
       </c>
-      <c r="D16" s="163" t="n">
+      <c r="D16" s="165" t="n">
         <v>43475</v>
       </c>
-      <c r="E16" s="160" t="s">
+      <c r="E16" s="162" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="78" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="161" t="s">
+      <c r="A17" s="163" t="s">
         <v>347</v>
       </c>
-      <c r="B17" s="158" t="s">
+      <c r="B17" s="160" t="s">
         <v>353</v>
       </c>
-      <c r="C17" s="157" t="s">
+      <c r="C17" s="159" t="s">
         <v>349</v>
       </c>
-      <c r="D17" s="155" t="n">
+      <c r="D17" s="157" t="n">
         <v>43476</v>
       </c>
-      <c r="E17" s="161" t="s">
+      <c r="E17" s="163" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="161" t="s">
+      <c r="A18" s="163" t="s">
         <v>347</v>
       </c>
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="160" t="s">
         <v>355</v>
       </c>
-      <c r="C18" s="157" t="s">
+      <c r="C18" s="159" t="s">
         <v>349</v>
       </c>
-      <c r="D18" s="155" t="n">
+      <c r="D18" s="157" t="n">
         <v>43478</v>
       </c>
-      <c r="E18" s="161" t="s">
+      <c r="E18" s="163" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="161" t="s">
+      <c r="A19" s="163" t="s">
         <v>347</v>
       </c>
-      <c r="B19" s="158" t="s">
+      <c r="B19" s="160" t="s">
         <v>357</v>
       </c>
-      <c r="C19" s="157" t="s">
+      <c r="C19" s="159" t="s">
         <v>349</v>
       </c>
-      <c r="D19" s="155" t="n">
+      <c r="D19" s="157" t="n">
         <v>43478</v>
       </c>
-      <c r="E19" s="161" t="s">
+      <c r="E19" s="163" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="109.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="161" t="s">
+      <c r="A20" s="163" t="s">
         <v>342</v>
       </c>
-      <c r="B20" s="158" t="s">
+      <c r="B20" s="160" t="s">
         <v>359</v>
       </c>
-      <c r="C20" s="157" t="s">
+      <c r="C20" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="155" t="n">
+      <c r="D20" s="157" t="n">
         <v>43641</v>
       </c>
-      <c r="E20" s="162" t="s">
+      <c r="E20" s="164" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="161" t="s">
+      <c r="A21" s="163" t="s">
         <v>342</v>
       </c>
-      <c r="B21" s="158" t="s">
+      <c r="B21" s="160" t="s">
         <v>361</v>
       </c>
-      <c r="C21" s="157" t="s">
+      <c r="C21" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="155" t="n">
+      <c r="D21" s="157" t="n">
         <v>43642</v>
       </c>
-      <c r="E21" s="161" t="s">
+      <c r="E21" s="163" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="161" t="s">
+      <c r="A22" s="163" t="s">
         <v>342</v>
       </c>
-      <c r="B22" s="158" t="s">
+      <c r="B22" s="160" t="s">
         <v>363</v>
       </c>
-      <c r="C22" s="157" t="s">
+      <c r="C22" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="155" t="n">
+      <c r="D22" s="157" t="n">
         <v>43649</v>
       </c>
-      <c r="E22" s="161" t="s">
+      <c r="E22" s="163" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="161" t="s">
+      <c r="A23" s="163" t="s">
         <v>342</v>
       </c>
-      <c r="B23" s="158" t="s">
+      <c r="B23" s="160" t="s">
         <v>363</v>
       </c>
-      <c r="C23" s="157" t="s">
+      <c r="C23" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="155" t="n">
+      <c r="D23" s="157" t="n">
         <v>43672</v>
       </c>
-      <c r="E23" s="161" t="s">
+      <c r="E23" s="163" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="161" t="s">
+      <c r="A24" s="163" t="s">
         <v>342</v>
       </c>
-      <c r="B24" s="158" t="s">
+      <c r="B24" s="160" t="s">
         <v>363</v>
       </c>
-      <c r="C24" s="157" t="s">
+      <c r="C24" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="155" t="n">
+      <c r="D24" s="157" t="n">
         <v>43674</v>
       </c>
-      <c r="E24" s="161" t="s">
+      <c r="E24" s="163" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="161" t="s">
+      <c r="A25" s="163" t="s">
         <v>342</v>
       </c>
-      <c r="B25" s="158" t="s">
+      <c r="B25" s="160" t="s">
         <v>367</v>
       </c>
-      <c r="C25" s="157" t="s">
+      <c r="C25" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="155" t="n">
+      <c r="D25" s="157" t="n">
         <v>43685</v>
       </c>
-      <c r="E25" s="161" t="s">
+      <c r="E25" s="163" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="161" t="s">
+      <c r="A26" s="163" t="s">
         <v>369</v>
       </c>
-      <c r="B26" s="158" t="s">
+      <c r="B26" s="160" t="s">
         <v>367</v>
       </c>
-      <c r="C26" s="157" t="s">
+      <c r="C26" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="155" t="n">
+      <c r="D26" s="157" t="n">
         <v>43719</v>
       </c>
-      <c r="E26" s="161" t="s">
+      <c r="E26" s="163" t="s">
         <v>370</v>
       </c>
     </row>

</xml_diff>

<commit_message>
iOS Security Requiments V3 translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -1331,7 +1331,7 @@
     <numFmt numFmtId="171" formatCode="@"/>
     <numFmt numFmtId="172" formatCode="[$-407]dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="34">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1551,6 +1551,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color rgb="FF5F5F5F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <b val="true"/>
@@ -2488,8 +2496,8 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="19" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -2516,7 +2524,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2524,15 +2532,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2556,7 +2564,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2564,7 +2572,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2572,11 +2580,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="32" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="172" fontId="33" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2750,7 +2758,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2930,11 +2938,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="61365850"/>
-        <c:axId val="10755112"/>
+        <c:axId val="38936658"/>
+        <c:axId val="57564363"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="61365850"/>
+        <c:axId val="38936658"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2974,7 +2982,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10755112"/>
+        <c:crossAx val="57564363"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2982,7 +2990,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10755112"/>
+        <c:axId val="57564363"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3025,7 +3033,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61365850"/>
+        <c:crossAx val="38936658"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3085,7 +3093,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3265,11 +3273,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="42571708"/>
-        <c:axId val="65343306"/>
+        <c:axId val="60900482"/>
+        <c:axId val="17616543"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="42571708"/>
+        <c:axId val="60900482"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3309,7 +3317,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65343306"/>
+        <c:crossAx val="17616543"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3317,7 +3325,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65343306"/>
+        <c:axId val="17616543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3360,7 +3368,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42571708"/>
+        <c:crossAx val="60900482"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7031,8 +7039,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7705,7 +7713,7 @@
       <c r="J28" s="85"/>
       <c r="K28" s="95"/>
     </row>
-    <row r="29" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="87" t="s">
         <v>133</v>
       </c>
@@ -7723,14 +7731,14 @@
       </c>
       <c r="G29" s="70"/>
       <c r="H29" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
-        <v>Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Проверка системы управления ключами (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
+        <v>Проверка системы управления ключами (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
       <c r="I29" s="76"/>
       <c r="J29" s="76"/>
       <c r="K29" s="73"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="87" t="s">
         <v>136</v>
       </c>
@@ -7747,15 +7755,15 @@
         <v>64</v>
       </c>
       <c r="G30" s="70"/>
-      <c r="H30" s="143" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#verifying-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-and-mstg-crypto-3"),"Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
-        <v>Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
+      <c r="H30" s="89" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#verifying-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-and-mstg-crypto-3"),"Тестирование конфигурации криптографических стандартных алгоритмов (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
+        <v>Тестирование конфигурации криптографических стандартных алгоритмов (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
       <c r="I30" s="76"/>
       <c r="J30" s="76"/>
       <c r="K30" s="73"/>
     </row>
-    <row r="31" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="87" t="s">
         <v>139</v>
       </c>
@@ -7772,9 +7780,9 @@
         <v>64</v>
       </c>
       <c r="G31" s="70"/>
-      <c r="H31" s="143" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#verifying-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-and-mstg-crypto-3"),"Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
-        <v>Verifying the Configuration of Cryptographic Standard Algorithms (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
+      <c r="H31" s="89" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#verifying-the-configuration-of-cryptographic-standard-algorithms-mstg-crypto-2-and-mstg-crypto-3"),"Тестирование конфигурации криптографических стандартных алгоритмов (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)")</f>
+        <v>Тестирование конфигурации криптографических стандартных алгоритмов (MSTG-CRYPTO-2 and MSTG-CRYPTO-3)</v>
       </c>
       <c r="I31" s="76"/>
       <c r="J31" s="76"/>
@@ -7798,8 +7806,8 @@
       </c>
       <c r="G32" s="70"/>
       <c r="H32" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#identifying-insecure-andor-deprecated-cryptographic-algorithms-mstg-crypto-4"),"Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)")</f>
-        <v>Identifying Insecure and/or Deprecated Cryptographic Algorithms (MSTG-CRYPTO-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04g-Testing-Cryptography.md#identifying-insecure-andor-deprecated-cryptographic-algorithms-mstg-crypto-4"),"Поиск небезопасных и/или устаревших криптографических алгоритмов (MSTG-CRYPTO-4)")</f>
+        <v>Поиск небезопасных и/или устаревших криптографических алгоритмов (MSTG-CRYPTO-4)</v>
       </c>
       <c r="I32" s="76"/>
       <c r="J32" s="76"/>
@@ -7823,8 +7831,8 @@
       </c>
       <c r="G33" s="70"/>
       <c r="H33" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
-        <v>Testing Key Management (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Проверка системы управления ключами (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
+        <v>Проверка системы управления ключами (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
       <c r="I33" s="76"/>
       <c r="J33" s="76"/>
@@ -7847,9 +7855,9 @@
         <v>64</v>
       </c>
       <c r="G34" s="70"/>
-      <c r="H34" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-random-number-generation-mstg-crypto-6")," Testing Random Number Generation (MSTG-CRYPTO-6)")</f>
-        <v> Testing Random Number Generation (MSTG-CRYPTO-6)</v>
+      <c r="H34" s="143" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06e-Testing-Cryptography.md#testing-key-management-mstg-crypto-1-and-mstg-crypto-5"),"Проверка системы управления ключами (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)")</f>
+        <v>Проверка системы управления ключами (MSTG-CRYPTO-1 and MSTG-CRYPTO-5)</v>
       </c>
       <c r="I34" s="76"/>
       <c r="J34" s="76"/>
@@ -8095,7 +8103,7 @@
       <c r="G44" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H44" s="143" t="str">
+      <c r="H44" s="89" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
@@ -8120,7 +8128,7 @@
       <c r="G45" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H45" s="143" t="str">
+      <c r="H45" s="89" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
         <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
@@ -8186,7 +8194,7 @@
         <v>64</v>
       </c>
       <c r="G48" s="70"/>
-      <c r="H48" s="143" t="str">
+      <c r="H48" s="89" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
@@ -8211,7 +8219,7 @@
         <v>64</v>
       </c>
       <c r="G49" s="70"/>
-      <c r="H49" s="143" t="str">
+      <c r="H49" s="89" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
         <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
@@ -8289,7 +8297,7 @@
       <c r="G52" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H52" s="143" t="str">
+      <c r="H52" s="89" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels-mstg-network-5"),"Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)")</f>
         <v>Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)</v>
       </c>

</xml_diff>

<commit_message>
iOS Security Requiments V4 translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -1923,7 +1923,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="167">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2505,6 +2505,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="28" fillId="0" borderId="19" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2758,7 +2762,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2938,11 +2942,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="38936658"/>
-        <c:axId val="57564363"/>
+        <c:axId val="4589493"/>
+        <c:axId val="3279746"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="38936658"/>
+        <c:axId val="4589493"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2982,7 +2986,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57564363"/>
+        <c:crossAx val="3279746"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2990,7 +2994,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57564363"/>
+        <c:axId val="3279746"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3033,7 +3037,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38936658"/>
+        <c:crossAx val="4589493"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3093,7 +3097,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3273,11 +3277,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="60900482"/>
-        <c:axId val="17616543"/>
+        <c:axId val="5850423"/>
+        <c:axId val="68639316"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="60900482"/>
+        <c:axId val="5850423"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3317,7 +3321,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17616543"/>
+        <c:crossAx val="68639316"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3325,7 +3329,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="17616543"/>
+        <c:axId val="68639316"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3368,7 +3372,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60900482"/>
+        <c:crossAx val="5850423"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7039,8 +7043,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E25" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7896,13 +7900,13 @@
         <v>64</v>
       </c>
       <c r="G36" s="70"/>
-      <c r="H36" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
-        <v>Verifying that Appropriate Authentication is in Place (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
-      </c>
-      <c r="I36" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
-        <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
+      <c r="H36" s="136" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-appropriate-authentication-is-in-place-mstg-arch-2-and-mstg-auth-1"),"Проверка наличия соответствующей аутентификации (MSTG-ARCH-2 and MSTG-AUTH-1)")</f>
+        <v>Проверка наличия соответствующей аутентификации (MSTG-ARCH-2 and MSTG-AUTH-1)</v>
+      </c>
+      <c r="I36" s="136" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Проверка потоков OAuth 2.0 (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
+        <v>Проверка потоков OAuth 2.0 (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
       <c r="J36" s="144"/>
       <c r="K36" s="125"/>
@@ -7924,9 +7928,9 @@
         <v>64</v>
       </c>
       <c r="G37" s="70"/>
-      <c r="H37" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateful-session-management-mstg-auth-2"),"Testing Stateful Session Management (MSTG-AUTH-2)")</f>
-        <v>Testing Stateful Session Management (MSTG-AUTH-2)</v>
+      <c r="H37" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateful-session-management-mstg-auth-2"),"Тестирование аутентификации на основе сессии(MSTG-AUTH-2)")</f>
+        <v>Тестирование аутентификации на основе сессии(MSTG-AUTH-2)</v>
       </c>
       <c r="I37" s="76"/>
       <c r="J37" s="76"/>
@@ -7949,13 +7953,13 @@
         <v>64</v>
       </c>
       <c r="G38" s="70"/>
-      <c r="H38" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateless-token-based-authentication-mstg-auth-3"),"Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)")</f>
-        <v>Testing Stateless (Token-Based) Authentication (MSTG-AUTH-3)</v>
-      </c>
-      <c r="I38" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
-        <v>Testing OAuth 2.0 Flows (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
+      <c r="H38" s="139" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-stateless-token-based-authentication-mstg-auth-3"),"Тестирование аутентификации на основе токена (MSTG-AUTH-3)")</f>
+        <v>Тестирование аутентификации на основе токена (MSTG-AUTH-3)</v>
+      </c>
+      <c r="I38" s="136" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-oauth-20-flows-mstg-auth-1-and-mstg-auth-3"),"Проверка потоков OAuth 2.0 (MSTG-AUTH-1 and MSTG-AUTH-3)")</f>
+        <v>Проверка потоков OAuth 2.0 (MSTG-AUTH-1 and MSTG-AUTH-3)</v>
       </c>
       <c r="J38" s="144"/>
       <c r="K38" s="125"/>
@@ -7973,9 +7977,9 @@
       <c r="E39" s="68"/>
       <c r="F39" s="69"/>
       <c r="G39" s="70"/>
-      <c r="H39" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-user-logout-mstg-auth-4"),"Testing User Logout (MSTG-AUTH-4)")</f>
-        <v>Testing User Logout (MSTG-AUTH-4)</v>
+      <c r="H39" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-user-logout-mstg-auth-4"),"Тестирование деаутентификации пользователя (MSTG-AUTH-4)")</f>
+        <v>Тестирование деаутентификации пользователя (MSTG-AUTH-4)</v>
       </c>
       <c r="I39" s="76"/>
       <c r="J39" s="76"/>
@@ -7999,9 +8003,9 @@
         <v>64</v>
       </c>
       <c r="G40" s="70"/>
-      <c r="H40" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
-        <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
+      <c r="H40" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Проверка на лучшие практики для пароля (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
+        <v>Проверка на лучшие практики для пароля (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
       </c>
       <c r="I40" s="76"/>
       <c r="J40" s="76"/>
@@ -8025,13 +8029,13 @@
         <v>64</v>
       </c>
       <c r="G41" s="70"/>
-      <c r="H41" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
-        <v>Testing Best Practices for Passwords (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
-      </c>
-      <c r="I41" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#dynamic-testing-mstg-auth-6"),"Dynamic Testing (MSTG-AUTH-6)")</f>
-        <v>Dynamic Testing (MSTG-AUTH-6)</v>
+      <c r="H41" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-best-practices-for-passwords-mstg-auth-5-and-mstg-auth-6"),"Проверка на лучшие практики для пароля (MSTG-AUTH-5 and MSTG-AUTH-6)")</f>
+        <v>Проверка на лучшие практики для пароля (MSTG-AUTH-5 and MSTG-AUTH-6)</v>
+      </c>
+      <c r="I41" s="136" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#dynamic-testing-mstg-auth-6"),"Динамическое тестирование (MSTG-AUTH-6)")</f>
+        <v>Динамическое тестирование (MSTG-AUTH-6)</v>
       </c>
       <c r="J41" s="144"/>
       <c r="K41" s="125"/>
@@ -8053,9 +8057,9 @@
         <v>64</v>
       </c>
       <c r="G42" s="70"/>
-      <c r="H42" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-session-timeout-mstg-auth-7"),"Testing Session Timeout (MSTG-AUTH-7)")</f>
-        <v>Testing Session Timeout (MSTG-AUTH-7)</v>
+      <c r="H42" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-session-timeout-mstg-auth-7"),"Тестирование таймаута сессии (MSTG-AUTH-7)")</f>
+        <v>Тестирование таймаута сессии (MSTG-AUTH-7)</v>
       </c>
       <c r="I42" s="97"/>
       <c r="J42" s="145"/>
@@ -8079,8 +8083,8 @@
         <v>77</v>
       </c>
       <c r="H43" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06f-Testing-Local-Authentication.md#testing-local-authentication-mstg-auth-8-and-mstg-storage-11"),"Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)")</f>
-        <v>Testing Local Authentication (MSTG-AUTH-8 and MSTG-STORAGE-11)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06f-Testing-Local-Authentication.md#testing-local-authentication-mstg-auth-8-and-mstg-storage-11"),"Тестирование локальной аутентификации(MSTG-AUTH-8 and MSTG-STORAGE-11)")</f>
+        <v>Тестирование локальной аутентификации(MSTG-AUTH-8 and MSTG-STORAGE-11)</v>
       </c>
       <c r="I43" s="90"/>
       <c r="J43" s="144"/>
@@ -8103,9 +8107,9 @@
       <c r="G44" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H44" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
-        <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
+      <c r="H44" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Тестирование двухфакторной и повышающей аутентификации(MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
+        <v>Тестирование двухфакторной и повышающей аутентификации(MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
       <c r="I44" s="76"/>
       <c r="J44" s="76"/>
@@ -8128,9 +8132,9 @@
       <c r="G45" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H45" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
-        <v>Testing Two-Factor Authentication and Step-up Authentication (MSTG-AUTH-9 and MSTG-AUTH-10)</v>
+      <c r="H45" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-two-factor-authentication-and-step-up-authentication-mstg-auth-9-and-mstg-auth-10"),"Тестирование двухфакторной и повышающей аутентификации(MSTG-AUTH-9 and MSTG-AUTH-10)")</f>
+        <v>Тестирование двухфакторной и повышающей аутентификации(MSTG-AUTH-9 and MSTG-AUTH-10)</v>
       </c>
       <c r="I45" s="76"/>
       <c r="J45" s="76"/>
@@ -8154,8 +8158,8 @@
         <v>77</v>
       </c>
       <c r="H46" s="146" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x04e-Testing-Authentication-and-Session-Management.md#testing-login-activity-and-device-blocking-mstg-auth-11"), "Testing Login Activity and Device Blocking (MSTG-AUTH-11)")</f>
-        <v>Testing Login Activity and Device Blocking (MSTG-AUTH-11)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04e-Testing-Authentication-and-Session-Management.md#testing-login-activity-and-device-blocking-mstg-auth-11"),"Тестирование активности входа и блокировки устройства (MSTG-AUTH-11)")</f>
+        <v>Тестирование активности входа и блокировки устройства (MSTG-AUTH-11)</v>
       </c>
       <c r="I46" s="76"/>
       <c r="J46" s="76"/>
@@ -8679,7 +8683,7 @@
         <v>64</v>
       </c>
       <c r="G68" s="70"/>
-      <c r="H68" s="146" t="str">
+      <c r="H68" s="147" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"),"Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
         <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
       </c>
@@ -8796,12 +8800,12 @@
       <c r="G73" s="108"/>
       <c r="H73" s="108"/>
       <c r="I73" s="109"/>
-      <c r="J73" s="147"/>
-      <c r="K73" s="148"/>
+      <c r="J73" s="148"/>
+      <c r="K73" s="149"/>
     </row>
     <row r="74" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="149"/>
-      <c r="C74" s="149"/>
+      <c r="B74" s="150"/>
+      <c r="C74" s="150"/>
       <c r="D74" s="92"/>
       <c r="E74" s="114"/>
       <c r="F74" s="114"/>
@@ -8812,8 +8816,8 @@
       <c r="K74" s="92"/>
     </row>
     <row r="75" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="149"/>
-      <c r="C75" s="149"/>
+      <c r="B75" s="150"/>
+      <c r="C75" s="150"/>
       <c r="D75" s="92"/>
       <c r="E75" s="114"/>
       <c r="F75" s="114"/>
@@ -8824,8 +8828,8 @@
       <c r="K75" s="92"/>
     </row>
     <row r="76" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="149"/>
-      <c r="C76" s="149"/>
+      <c r="B76" s="150"/>
+      <c r="C76" s="150"/>
       <c r="D76" s="92"/>
       <c r="E76" s="114"/>
       <c r="F76" s="114"/>
@@ -8914,8 +8918,8 @@
       <c r="K81" s="92"/>
     </row>
     <row r="82" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="149"/>
-      <c r="C82" s="149"/>
+      <c r="B82" s="150"/>
+      <c r="C82" s="150"/>
       <c r="D82" s="92"/>
       <c r="E82" s="114"/>
       <c r="F82" s="114"/>
@@ -8926,8 +8930,8 @@
       <c r="K82" s="92"/>
     </row>
     <row r="83" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="149"/>
-      <c r="C83" s="149"/>
+      <c r="B83" s="150"/>
+      <c r="C83" s="150"/>
       <c r="D83" s="92"/>
       <c r="E83" s="114"/>
       <c r="F83" s="114"/>
@@ -8938,8 +8942,8 @@
       <c r="K83" s="92"/>
     </row>
     <row r="84" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="149"/>
-      <c r="C84" s="149"/>
+      <c r="B84" s="150"/>
+      <c r="C84" s="150"/>
       <c r="D84" s="92"/>
       <c r="E84" s="114"/>
       <c r="F84" s="114"/>
@@ -8950,8 +8954,8 @@
       <c r="K84" s="92"/>
     </row>
     <row r="85" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="149"/>
-      <c r="C85" s="149"/>
+      <c r="B85" s="150"/>
+      <c r="C85" s="150"/>
       <c r="D85" s="92"/>
       <c r="E85" s="114"/>
       <c r="F85" s="114"/>
@@ -8970,7 +8974,7 @@
       <formula>NOT(ISERROR(SEARCH("0x05",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H28:H1048576 H1:H2 H4 H13 H15:H18">
+  <conditionalFormatting sqref="H47:H1048576 H1:H2 H4 H13 H15:H18 H43 H28:H35 H40:H41">
     <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="3">
       <formula>NOT(ISERROR(SEARCH("0x05",H1)))</formula>
     </cfRule>
@@ -9155,7 +9159,7 @@
       <c r="F8" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="150" t="s">
+      <c r="G8" s="151" t="s">
         <v>298</v>
       </c>
       <c r="H8" s="125"/>
@@ -9176,7 +9180,7 @@
       <c r="F9" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G9" s="150" t="s">
+      <c r="G9" s="151" t="s">
         <v>298</v>
       </c>
       <c r="H9" s="125"/>
@@ -9197,7 +9201,7 @@
       <c r="F10" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="150" t="s">
+      <c r="G10" s="151" t="s">
         <v>298</v>
       </c>
       <c r="H10" s="125"/>
@@ -9260,7 +9264,7 @@
       <c r="F13" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="150" t="s">
+      <c r="G13" s="151" t="s">
         <v>298</v>
       </c>
       <c r="H13" s="125"/>
@@ -9325,7 +9329,7 @@
       <c r="F17" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="151" t="str">
+      <c r="G17" s="152" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks-mstg-resilience-3-and-mstg-resilience-11"),"File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)")</f>
         <v>File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)</v>
       </c>
@@ -9362,8 +9366,8 @@
       <c r="H19" s="110"/>
     </row>
     <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="149"/>
-      <c r="C20" s="149"/>
+      <c r="B20" s="150"/>
+      <c r="C20" s="150"/>
       <c r="D20" s="92"/>
       <c r="E20" s="114"/>
       <c r="F20" s="114"/>
@@ -9371,8 +9375,8 @@
       <c r="H20" s="92"/>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="149"/>
-      <c r="C21" s="149"/>
+      <c r="B21" s="150"/>
+      <c r="C21" s="150"/>
       <c r="D21" s="92"/>
       <c r="E21" s="114"/>
       <c r="F21" s="114"/>
@@ -9443,8 +9447,8 @@
       <c r="H26" s="92"/>
     </row>
     <row r="27" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="149"/>
-      <c r="C27" s="149"/>
+      <c r="B27" s="150"/>
+      <c r="C27" s="150"/>
       <c r="D27" s="92"/>
       <c r="E27" s="114"/>
       <c r="F27" s="114"/>
@@ -9452,8 +9456,8 @@
       <c r="H27" s="92"/>
     </row>
     <row r="28" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="149"/>
-      <c r="C28" s="149"/>
+      <c r="B28" s="150"/>
+      <c r="C28" s="150"/>
       <c r="D28" s="92"/>
       <c r="E28" s="114"/>
       <c r="F28" s="114"/>
@@ -9461,8 +9465,8 @@
       <c r="H28" s="92"/>
     </row>
     <row r="29" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="149"/>
-      <c r="C29" s="149"/>
+      <c r="B29" s="150"/>
+      <c r="C29" s="150"/>
       <c r="D29" s="92"/>
       <c r="E29" s="114"/>
       <c r="F29" s="114"/>
@@ -9470,22 +9474,22 @@
       <c r="H29" s="92"/>
     </row>
     <row r="30" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="149"/>
-      <c r="C30" s="149"/>
+      <c r="B30" s="150"/>
+      <c r="C30" s="150"/>
       <c r="D30" s="92"/>
       <c r="E30" s="114"/>
       <c r="F30" s="114"/>
     </row>
     <row r="31" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="149"/>
-      <c r="C31" s="149"/>
+      <c r="B31" s="150"/>
+      <c r="C31" s="150"/>
       <c r="D31" s="92"/>
       <c r="E31" s="114"/>
       <c r="F31" s="114"/>
     </row>
     <row r="32" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="149"/>
-      <c r="C32" s="149"/>
+      <c r="B32" s="150"/>
+      <c r="C32" s="150"/>
       <c r="D32" s="92"/>
       <c r="E32" s="114"/>
       <c r="F32" s="114"/>
@@ -9566,412 +9570,412 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="152" t="s">
+      <c r="A1" s="153" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="153"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="154"/>
       <c r="D1" s="52"/>
       <c r="E1" s="52"/>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="154" t="s">
+      <c r="A2" s="155" t="s">
         <v>319</v>
       </c>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="155" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="154" t="s">
+      <c r="C2" s="155" t="s">
         <v>321</v>
       </c>
-      <c r="D2" s="154" t="s">
+      <c r="D2" s="155" t="s">
         <v>322</v>
       </c>
-      <c r="E2" s="154" t="s">
+      <c r="E2" s="155" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="155" t="s">
+      <c r="A3" s="156" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="156" t="n">
+      <c r="B3" s="157" t="n">
         <v>0.1</v>
       </c>
-      <c r="C3" s="156"/>
-      <c r="D3" s="157" t="n">
+      <c r="C3" s="157"/>
+      <c r="D3" s="158" t="n">
         <v>42765</v>
       </c>
-      <c r="E3" s="158" t="s">
+      <c r="E3" s="159" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="158" t="s">
+      <c r="A4" s="159" t="s">
         <v>325</v>
       </c>
-      <c r="B4" s="156" t="n">
+      <c r="B4" s="157" t="n">
         <v>0.2</v>
       </c>
-      <c r="C4" s="156"/>
-      <c r="D4" s="157" t="n">
+      <c r="C4" s="157"/>
+      <c r="D4" s="158" t="n">
         <v>42766</v>
       </c>
-      <c r="E4" s="158" t="s">
+      <c r="E4" s="159" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="158" t="s">
+      <c r="A5" s="159" t="s">
         <v>327</v>
       </c>
-      <c r="B5" s="156" t="n">
+      <c r="B5" s="157" t="n">
         <v>0.3</v>
       </c>
-      <c r="C5" s="156"/>
-      <c r="D5" s="157" t="n">
+      <c r="C5" s="157"/>
+      <c r="D5" s="158" t="n">
         <v>42778</v>
       </c>
-      <c r="E5" s="158" t="s">
+      <c r="E5" s="159" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="158" t="s">
+      <c r="A6" s="159" t="s">
         <v>329</v>
       </c>
-      <c r="B6" s="156" t="s">
+      <c r="B6" s="157" t="s">
         <v>330</v>
       </c>
-      <c r="C6" s="156"/>
-      <c r="D6" s="157" t="n">
+      <c r="C6" s="157"/>
+      <c r="D6" s="158" t="n">
         <v>42780</v>
       </c>
-      <c r="E6" s="158" t="s">
+      <c r="E6" s="159" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="158" t="s">
+      <c r="A7" s="159" t="s">
         <v>325</v>
       </c>
-      <c r="B7" s="159" t="s">
+      <c r="B7" s="160" t="s">
         <v>332</v>
       </c>
-      <c r="C7" s="159"/>
-      <c r="D7" s="157" t="n">
+      <c r="C7" s="160"/>
+      <c r="D7" s="158" t="n">
         <v>42781</v>
       </c>
-      <c r="E7" s="158" t="s">
+      <c r="E7" s="159" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="158" t="s">
+      <c r="A8" s="159" t="s">
         <v>329</v>
       </c>
-      <c r="B8" s="159" t="s">
+      <c r="B8" s="160" t="s">
         <v>334</v>
       </c>
-      <c r="C8" s="159"/>
-      <c r="D8" s="157" t="n">
+      <c r="C8" s="160"/>
+      <c r="D8" s="158" t="n">
         <v>42829</v>
       </c>
-      <c r="E8" s="158" t="s">
+      <c r="E8" s="159" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="158" t="s">
+      <c r="A9" s="159" t="s">
         <v>325</v>
       </c>
-      <c r="B9" s="159" t="s">
+      <c r="B9" s="160" t="s">
         <v>334</v>
       </c>
-      <c r="C9" s="159"/>
-      <c r="D9" s="157" t="n">
+      <c r="C9" s="160"/>
+      <c r="D9" s="158" t="n">
         <v>42919</v>
       </c>
-      <c r="E9" s="158" t="s">
+      <c r="E9" s="159" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="158" t="s">
+      <c r="A10" s="159" t="s">
         <v>325</v>
       </c>
-      <c r="B10" s="159" t="s">
+      <c r="B10" s="160" t="s">
         <v>337</v>
       </c>
-      <c r="C10" s="159"/>
-      <c r="D10" s="157" t="n">
+      <c r="C10" s="160"/>
+      <c r="D10" s="158" t="n">
         <v>42963</v>
       </c>
-      <c r="E10" s="158" t="s">
+      <c r="E10" s="159" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="158" t="s">
+      <c r="A11" s="159" t="s">
         <v>325</v>
       </c>
-      <c r="B11" s="159" t="s">
+      <c r="B11" s="160" t="s">
         <v>339</v>
       </c>
-      <c r="C11" s="159"/>
-      <c r="D11" s="157" t="n">
+      <c r="C11" s="160"/>
+      <c r="D11" s="158" t="n">
         <v>43113</v>
       </c>
-      <c r="E11" s="158" t="s">
+      <c r="E11" s="159" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="158" t="s">
+      <c r="A12" s="159" t="s">
         <v>325</v>
       </c>
-      <c r="B12" s="159" t="n">
+      <c r="B12" s="160" t="n">
         <v>1.1</v>
       </c>
-      <c r="C12" s="159"/>
-      <c r="D12" s="157" t="n">
+      <c r="C12" s="160"/>
+      <c r="D12" s="158" t="n">
         <v>43289</v>
       </c>
-      <c r="E12" s="158" t="s">
+      <c r="E12" s="159" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="158" t="s">
+      <c r="A13" s="159" t="s">
         <v>342</v>
       </c>
-      <c r="B13" s="160" t="s">
+      <c r="B13" s="161" t="s">
         <v>343</v>
       </c>
-      <c r="C13" s="161"/>
-      <c r="D13" s="157" t="n">
+      <c r="C13" s="162"/>
+      <c r="D13" s="158" t="n">
         <v>43464</v>
       </c>
-      <c r="E13" s="162" t="s">
+      <c r="E13" s="163" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="158" t="s">
+      <c r="A14" s="159" t="s">
         <v>345</v>
       </c>
-      <c r="B14" s="160" t="s">
+      <c r="B14" s="161" t="s">
         <v>346</v>
       </c>
-      <c r="C14" s="161"/>
-      <c r="D14" s="157" t="n">
+      <c r="C14" s="162"/>
+      <c r="D14" s="158" t="n">
         <v>43469</v>
       </c>
-      <c r="E14" s="162" t="s">
+      <c r="E14" s="163" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="409.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="163" t="s">
+      <c r="A15" s="164" t="s">
         <v>347</v>
       </c>
-      <c r="B15" s="159" t="s">
+      <c r="B15" s="160" t="s">
         <v>348</v>
       </c>
-      <c r="C15" s="159" t="s">
+      <c r="C15" s="160" t="s">
         <v>349</v>
       </c>
-      <c r="D15" s="157" t="n">
+      <c r="D15" s="158" t="n">
         <v>43471</v>
       </c>
-      <c r="E15" s="164" t="s">
+      <c r="E15" s="165" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>342</v>
       </c>
-      <c r="B16" s="160" t="s">
+      <c r="B16" s="161" t="s">
         <v>351</v>
       </c>
-      <c r="C16" s="159" t="s">
+      <c r="C16" s="160" t="s">
         <v>349</v>
       </c>
-      <c r="D16" s="165" t="n">
+      <c r="D16" s="166" t="n">
         <v>43475</v>
       </c>
-      <c r="E16" s="162" t="s">
+      <c r="E16" s="163" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="78" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="163" t="s">
+      <c r="A17" s="164" t="s">
         <v>347</v>
       </c>
-      <c r="B17" s="160" t="s">
+      <c r="B17" s="161" t="s">
         <v>353</v>
       </c>
-      <c r="C17" s="159" t="s">
+      <c r="C17" s="160" t="s">
         <v>349</v>
       </c>
-      <c r="D17" s="157" t="n">
+      <c r="D17" s="158" t="n">
         <v>43476</v>
       </c>
-      <c r="E17" s="163" t="s">
+      <c r="E17" s="164" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="163" t="s">
+      <c r="A18" s="164" t="s">
         <v>347</v>
       </c>
-      <c r="B18" s="160" t="s">
+      <c r="B18" s="161" t="s">
         <v>355</v>
       </c>
-      <c r="C18" s="159" t="s">
+      <c r="C18" s="160" t="s">
         <v>349</v>
       </c>
-      <c r="D18" s="157" t="n">
+      <c r="D18" s="158" t="n">
         <v>43478</v>
       </c>
-      <c r="E18" s="163" t="s">
+      <c r="E18" s="164" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="163" t="s">
+      <c r="A19" s="164" t="s">
         <v>347</v>
       </c>
-      <c r="B19" s="160" t="s">
+      <c r="B19" s="161" t="s">
         <v>357</v>
       </c>
-      <c r="C19" s="159" t="s">
+      <c r="C19" s="160" t="s">
         <v>349</v>
       </c>
-      <c r="D19" s="157" t="n">
+      <c r="D19" s="158" t="n">
         <v>43478</v>
       </c>
-      <c r="E19" s="163" t="s">
+      <c r="E19" s="164" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="109.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="163" t="s">
+      <c r="A20" s="164" t="s">
         <v>342</v>
       </c>
-      <c r="B20" s="160" t="s">
+      <c r="B20" s="161" t="s">
         <v>359</v>
       </c>
-      <c r="C20" s="159" t="s">
+      <c r="C20" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="157" t="n">
+      <c r="D20" s="158" t="n">
         <v>43641</v>
       </c>
-      <c r="E20" s="164" t="s">
+      <c r="E20" s="165" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="163" t="s">
+      <c r="A21" s="164" t="s">
         <v>342</v>
       </c>
-      <c r="B21" s="160" t="s">
+      <c r="B21" s="161" t="s">
         <v>361</v>
       </c>
-      <c r="C21" s="159" t="s">
+      <c r="C21" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="157" t="n">
+      <c r="D21" s="158" t="n">
         <v>43642</v>
       </c>
-      <c r="E21" s="163" t="s">
+      <c r="E21" s="164" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="163" t="s">
+      <c r="A22" s="164" t="s">
         <v>342</v>
       </c>
-      <c r="B22" s="160" t="s">
+      <c r="B22" s="161" t="s">
         <v>363</v>
       </c>
-      <c r="C22" s="159" t="s">
+      <c r="C22" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="157" t="n">
+      <c r="D22" s="158" t="n">
         <v>43649</v>
       </c>
-      <c r="E22" s="163" t="s">
+      <c r="E22" s="164" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="163" t="s">
+      <c r="A23" s="164" t="s">
         <v>342</v>
       </c>
-      <c r="B23" s="160" t="s">
+      <c r="B23" s="161" t="s">
         <v>363</v>
       </c>
-      <c r="C23" s="159" t="s">
+      <c r="C23" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="157" t="n">
+      <c r="D23" s="158" t="n">
         <v>43672</v>
       </c>
-      <c r="E23" s="163" t="s">
+      <c r="E23" s="164" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="163" t="s">
+      <c r="A24" s="164" t="s">
         <v>342</v>
       </c>
-      <c r="B24" s="160" t="s">
+      <c r="B24" s="161" t="s">
         <v>363</v>
       </c>
-      <c r="C24" s="159" t="s">
+      <c r="C24" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="157" t="n">
+      <c r="D24" s="158" t="n">
         <v>43674</v>
       </c>
-      <c r="E24" s="163" t="s">
+      <c r="E24" s="164" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="163" t="s">
+      <c r="A25" s="164" t="s">
         <v>342</v>
       </c>
-      <c r="B25" s="160" t="s">
+      <c r="B25" s="161" t="s">
         <v>367</v>
       </c>
-      <c r="C25" s="159" t="s">
+      <c r="C25" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="157" t="n">
+      <c r="D25" s="158" t="n">
         <v>43685</v>
       </c>
-      <c r="E25" s="163" t="s">
+      <c r="E25" s="164" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="163" t="s">
+      <c r="A26" s="164" t="s">
         <v>369</v>
       </c>
-      <c r="B26" s="160" t="s">
+      <c r="B26" s="161" t="s">
         <v>367</v>
       </c>
-      <c r="C26" s="159" t="s">
+      <c r="C26" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="157" t="n">
+      <c r="D26" s="158" t="n">
         <v>43719</v>
       </c>
-      <c r="E26" s="163" t="s">
+      <c r="E26" s="164" t="s">
         <v>370</v>
       </c>
     </row>

</xml_diff>

<commit_message>
iOS Security Requiments V5 translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -2762,7 +2762,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2942,11 +2942,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="4589493"/>
-        <c:axId val="3279746"/>
+        <c:axId val="76135889"/>
+        <c:axId val="32746437"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="4589493"/>
+        <c:axId val="76135889"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2986,7 +2986,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3279746"/>
+        <c:crossAx val="32746437"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2994,7 +2994,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3279746"/>
+        <c:axId val="32746437"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3037,7 +3037,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4589493"/>
+        <c:crossAx val="76135889"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3097,7 +3097,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3277,11 +3277,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="5850423"/>
-        <c:axId val="68639316"/>
+        <c:axId val="50188874"/>
+        <c:axId val="24202078"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="5850423"/>
+        <c:axId val="50188874"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3321,7 +3321,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68639316"/>
+        <c:crossAx val="24202078"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3329,7 +3329,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68639316"/>
+        <c:axId val="24202078"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3372,7 +3372,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5850423"/>
+        <c:crossAx val="50188874"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7043,8 +7043,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E25" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H25" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H54" activeCellId="0" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8198,9 +8198,9 @@
         <v>64</v>
       </c>
       <c r="G48" s="70"/>
-      <c r="H48" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
-        <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
+      <c r="H48" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Проверка шифрования данных в сети (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
+        <v>Проверка шифрования данных в сети (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
       <c r="I48" s="75"/>
       <c r="J48" s="75"/>
@@ -8223,9 +8223,9 @@
         <v>64</v>
       </c>
       <c r="G49" s="70"/>
-      <c r="H49" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
-        <v>Verifying Data Encryption on the Network (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
+      <c r="H49" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network-mstg-network-1-and-mstg-network-2"),"Проверка шифрования данных в сети (MSTG-NETWORK-1 and MSTG-NETWORK-2)")</f>
+        <v>Проверка шифрования данных в сети (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
       <c r="I49" s="75" t="str">
         <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#app-transport-security-mstg-network-2"),"App Transport Security (MSTG-NETWORK-2)")</f>
@@ -8234,7 +8234,7 @@
       <c r="J49" s="75"/>
       <c r="K49" s="102"/>
     </row>
-    <row r="50" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="87" t="s">
         <v>194</v>
       </c>
@@ -8252,14 +8252,14 @@
       </c>
       <c r="G50" s="70"/>
       <c r="H50" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-3-and-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)")</f>
-        <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-3-and-mstg-network-4"),"Тестирование пользовательских хранилищ сертификатов и сохраненных сертификатов (MSTG-NETWORK-3 and MSTG-NETWORK-4)")</f>
+        <v>Тестирование пользовательских хранилищ сертификатов и сохраненных сертификатов (MSTG-NETWORK-3 and MSTG-NETWORK-4)</v>
       </c>
       <c r="I50" s="76"/>
       <c r="J50" s="76"/>
       <c r="K50" s="102"/>
     </row>
-    <row r="51" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="87" t="s">
         <v>197</v>
       </c>
@@ -8277,8 +8277,8 @@
         <v>77</v>
       </c>
       <c r="H51" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-3-and-mstg-network-4"),"Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)")</f>
-        <v>Testing Custom Certificate Stores and Certificate Pinning (MSTG-NETWORK-3 and MSTG-NETWORK-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning-mstg-network-3-and-mstg-network-4"),"Тестирование пользовательских хранилищ сертификатов и сохраненных сертификатов (MSTG-NETWORK-3 and MSTG-NETWORK-4)")</f>
+        <v>Тестирование пользовательских хранилищ сертификатов и сохраненных сертификатов (MSTG-NETWORK-3 and MSTG-NETWORK-4)</v>
       </c>
       <c r="I51" s="76"/>
       <c r="J51" s="76"/>
@@ -8301,15 +8301,15 @@
       <c r="G52" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="H52" s="89" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels-mstg-network-5"),"Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)")</f>
-        <v>Making Sure that Critical Operations Use Secure Communication Channels (MSTG-NETWORK-5)</v>
+      <c r="H52" s="140" t="str">
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels-mstg-network-5"),"Убедитесь, что для критических операций используются безопасные каналы связи (MSTG-NETWORK-5)")</f>
+        <v>Убедитесь, что для критических операций используются безопасные каналы связи (MSTG-NETWORK-5)</v>
       </c>
       <c r="I52" s="76"/>
       <c r="J52" s="76"/>
       <c r="K52" s="73"/>
     </row>
-    <row r="53" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="87" t="s">
         <v>203</v>
       </c>
@@ -8327,8 +8327,8 @@
         <v>77</v>
       </c>
       <c r="H53" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x06i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"), "Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)")</f>
-        <v>Checking for Weaknesses in Third Party Libraries (MSTG-CODE-5)</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x06i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries-mstg-code-5"), "Проверка уязвимостей в сторонних библиотеках (MSTG-CODE-5)")</f>
+        <v>Проверка уязвимостей в сторонних библиотеках (MSTG-CODE-5)</v>
       </c>
       <c r="I53" s="76"/>
       <c r="J53" s="76"/>
@@ -8974,7 +8974,7 @@
       <formula>NOT(ISERROR(SEARCH("0x05",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47:H1048576 H1:H2 H4 H13 H15:H18 H43 H28:H35 H40:H41">
+  <conditionalFormatting sqref="H53:H1048576 H1:H2 H4 H13 H15:H18 H43 H28:H35 H40:H41 H47 H50:H51">
     <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="0x05" dxfId="3">
       <formula>NOT(ISERROR(SEARCH("0x05",H1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
iOS Security Requiments V6 translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -2762,7 +2762,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2942,11 +2942,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="76135889"/>
-        <c:axId val="32746437"/>
+        <c:axId val="26905769"/>
+        <c:axId val="92520310"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="76135889"/>
+        <c:axId val="26905769"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2986,7 +2986,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32746437"/>
+        <c:crossAx val="92520310"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2994,7 +2994,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32746437"/>
+        <c:axId val="92520310"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3037,7 +3037,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76135889"/>
+        <c:crossAx val="26905769"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3097,7 +3097,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3277,11 +3277,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50188874"/>
-        <c:axId val="24202078"/>
+        <c:axId val="97759489"/>
+        <c:axId val="13697535"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="50188874"/>
+        <c:axId val="97759489"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3321,7 +3321,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24202078"/>
+        <c:crossAx val="13697535"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3329,7 +3329,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="24202078"/>
+        <c:axId val="13697535"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3372,7 +3372,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50188874"/>
+        <c:crossAx val="97759489"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3546,7 +3546,7 @@
   </sheetPr>
   <dimension ref="B1:D50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -3949,7 +3949,7 @@
   </sheetPr>
   <dimension ref="B1:X50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -4561,7 +4561,7 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -6548,7 +6548,7 @@
   </sheetPr>
   <dimension ref="B1:H29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -7043,8 +7043,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H25" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H54" activeCellId="0" sqref="H54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H55" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H62" activeCellId="0" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8206,7 +8206,7 @@
       <c r="J48" s="75"/>
       <c r="K48" s="102"/>
     </row>
-    <row r="49" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="87" t="s">
         <v>191</v>
       </c>
@@ -8228,8 +8228,8 @@
         <v>Проверка шифрования данных в сети (MSTG-NETWORK-1 and MSTG-NETWORK-2)</v>
       </c>
       <c r="I49" s="75" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#app-transport-security-mstg-network-2"),"App Transport Security (MSTG-NETWORK-2)")</f>
-        <v>App Transport Security (MSTG-NETWORK-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06g-Testing-Network-Communication.md#app-transport-security-mstg-network-2"),"Проверка работы App Transport Security (MSTG-NETWORK-2)")</f>
+        <v>Проверка работы App Transport Security (MSTG-NETWORK-2)</v>
       </c>
       <c r="J49" s="75"/>
       <c r="K49" s="102"/>
@@ -8350,7 +8350,7 @@
       <c r="J54" s="85"/>
       <c r="K54" s="95"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="87" t="s">
         <v>208</v>
       </c>
@@ -8368,14 +8368,14 @@
       </c>
       <c r="G55" s="70"/>
       <c r="H55" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-app-permissions-mstg-platform-1"),"Testing App Permissions (MSTG-PLATFORM-1)")</f>
-        <v>Testing App Permissions (MSTG-PLATFORM-1)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-app-permissions-mstg-platform-1"),"Проверка разрешений приложения (MSTG-PLATFORM-1)")</f>
+        <v>Проверка разрешений приложения (MSTG-PLATFORM-1)</v>
       </c>
       <c r="I55" s="76"/>
       <c r="J55" s="76"/>
       <c r="K55" s="73"/>
     </row>
-    <row r="56" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="87" t="s">
         <v>211</v>
       </c>
@@ -8393,14 +8393,14 @@
       </c>
       <c r="G56" s="70"/>
       <c r="H56" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"),"Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
-        <v>Injection Flaws (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x04h-Testing-Code-Quality.md#injection-flaws-mstg-arch-2-and-mstg-platform-2"),"Проверка на инъекции (MSTG-ARCH-2 and MSTG-PLATFORM-2)")</f>
+        <v>Проверка на инъекции (MSTG-ARCH-2 and MSTG-PLATFORM-2)</v>
       </c>
       <c r="I56" s="76"/>
       <c r="J56" s="76"/>
       <c r="K56" s="73"/>
     </row>
-    <row r="57" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="87" t="s">
         <v>214</v>
       </c>
@@ -8418,14 +8418,14 @@
       </c>
       <c r="G57" s="70"/>
       <c r="H57" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-custom-url-schemes-mstg-platform-3"),"Testing Custom URL Schemes (MSTG-PLATFORM-3)")</f>
-        <v>Testing Custom URL Schemes (MSTG-PLATFORM-3)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-custom-url-schemes-mstg-platform-3"),"Тестирование пользовательских схем URL (MSTG-PLATFORM-3)")</f>
+        <v>Тестирование пользовательских схем URL (MSTG-PLATFORM-3)</v>
       </c>
       <c r="I57" s="76"/>
       <c r="J57" s="76"/>
       <c r="K57" s="73"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="87" t="s">
         <v>217</v>
       </c>
@@ -8443,14 +8443,14 @@
       </c>
       <c r="G58" s="70"/>
       <c r="H58" s="71" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x06h-Testing-Platform-Interaction.md#testing-for-sensitive-functionality-exposure-through-ipc-mstg-platform-4"), "Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)")</f>
-        <v>Testing for Sensitive Functionality Exposure Through IPC (MSTG-PLATFORM-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE( BASE_URL, "0x06h-Testing-Platform-Interaction.md#testing-for-sensitive-functionality-exposure-through-ipc-mstg-platform-4"), "Проверка передачи конфиденциальных данных при обмене данными между потоками (IPC) (MSTG-PLATFORM-4)")</f>
+        <v>Проверка передачи конфиденциальных данных при обмене данными между потоками (IPC) (MSTG-PLATFORM-4)</v>
       </c>
       <c r="I58" s="76"/>
       <c r="J58" s="76"/>
       <c r="K58" s="73"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="87" t="s">
         <v>220</v>
       </c>
@@ -8468,14 +8468,14 @@
       </c>
       <c r="G59" s="70"/>
       <c r="H59" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-ios-webviews-mstg-platform-5"),"Testing iOS WebViews (MSTG-PLATFORM-5)")</f>
-        <v>Testing iOS WebViews (MSTG-PLATFORM-5)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-ios-webviews-mstg-platform-5"),"Тестирование iOS WebViews (MSTG-PLATFORM-5)")</f>
+        <v>Тестирование iOS WebViews (MSTG-PLATFORM-5)</v>
       </c>
       <c r="I59" s="76"/>
       <c r="J59" s="76"/>
       <c r="K59" s="73"/>
     </row>
-    <row r="60" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="87" t="s">
         <v>223</v>
       </c>
@@ -8493,14 +8493,14 @@
       </c>
       <c r="G60" s="70"/>
       <c r="H60" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-webview-protocol-handlers-mstg-platform-6"),"Testing WebView Protocol Handlers (MSTG-PLATFORM-6)")</f>
-        <v>Testing WebView Protocol Handlers (MSTG-PLATFORM-6)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-webview-protocol-handlers-mstg-platform-6"),"Тестирование обработчиков протокола WebView (MSTG-PLATFORM-6)")</f>
+        <v>Тестирование обработчиков протокола WebView (MSTG-PLATFORM-6)</v>
       </c>
       <c r="I60" s="76"/>
       <c r="J60" s="76"/>
       <c r="K60" s="73"/>
     </row>
-    <row r="61" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="87" t="s">
         <v>226</v>
       </c>
@@ -8518,14 +8518,14 @@
       </c>
       <c r="G61" s="70"/>
       <c r="H61" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#determining-whether-native-methods-are-exposed-through-webviews-mstg-platform-7"),"Determining Whether Native Methods Are Exposed Through WebViews (MSTG-PLATFORM-7)")</f>
-        <v>Determining Whether Native Methods Are Exposed Through WebViews (MSTG-PLATFORM-7)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#determining-whether-native-methods-are-exposed-through-webviews-mstg-platform-7"),"Определение раскрытия собственных методов в WebView (MSTG-PLATFORM-7)")</f>
+        <v>Определение раскрытия собственных методов в WebView (MSTG-PLATFORM-7)</v>
       </c>
       <c r="I61" s="76"/>
       <c r="J61" s="76"/>
       <c r="K61" s="73"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="87" t="s">
         <v>229</v>
       </c>
@@ -8543,8 +8543,8 @@
       </c>
       <c r="G62" s="70"/>
       <c r="H62" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-object-persistence-mstg-platform-8"),"Testing Object Persistence (MSTG-PLATFORM-8)")</f>
-        <v>Testing Object Persistence (MSTG-PLATFORM-8)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06h-Testing-Platform-Interaction.md#testing-object-persistence-mstg-platform-8"),"Стабильность объекта тестирования (MSTG-PLATFORM-8)")</f>
+        <v>Стабильность объекта тестирования (MSTG-PLATFORM-8)</v>
       </c>
       <c r="I62" s="76"/>
       <c r="J62" s="76"/>
@@ -9011,7 +9011,7 @@
   </sheetPr>
   <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -9558,7 +9558,7 @@
   </sheetPr>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
iOS Security Requiments V6
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -2762,7 +2762,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2942,11 +2942,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="26905769"/>
-        <c:axId val="92520310"/>
+        <c:axId val="97934166"/>
+        <c:axId val="19780430"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="26905769"/>
+        <c:axId val="97934166"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2986,7 +2986,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92520310"/>
+        <c:crossAx val="19780430"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2994,7 +2994,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92520310"/>
+        <c:axId val="19780430"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3037,7 +3037,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26905769"/>
+        <c:crossAx val="97934166"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3097,7 +3097,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3277,11 +3277,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="97759489"/>
-        <c:axId val="13697535"/>
+        <c:axId val="92657394"/>
+        <c:axId val="93328890"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="97759489"/>
+        <c:axId val="92657394"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3321,7 +3321,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13697535"/>
+        <c:crossAx val="93328890"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3329,7 +3329,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13697535"/>
+        <c:axId val="93328890"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3372,7 +3372,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97759489"/>
+        <c:crossAx val="92657394"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3546,7 +3546,7 @@
   </sheetPr>
   <dimension ref="B1:D50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -3949,7 +3949,7 @@
   </sheetPr>
   <dimension ref="B1:X50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -4561,7 +4561,7 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -6548,7 +6548,7 @@
   </sheetPr>
   <dimension ref="B1:H29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -7043,8 +7043,8 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H55" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H62" activeCellId="0" sqref="H62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H73" activeCellId="0" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8584,14 +8584,14 @@
       </c>
       <c r="G64" s="70"/>
       <c r="H64" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#making-sure-that-the-app-is-properly-signed-mstg-code-1"),"Making Sure that the App Is Properly Signed (MSTG-CODE-1)")</f>
-        <v>Making Sure that the App Is Properly Signed (MSTG-CODE-1)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#making-sure-that-the-app-is-properly-signed-mstg-code-1"),"Убедитесь, что приложение правильно подписано (MSTG-CODE-1)")</f>
+        <v>Убедитесь, что приложение правильно подписано (MSTG-CODE-1)</v>
       </c>
       <c r="I64" s="76"/>
       <c r="J64" s="76"/>
       <c r="K64" s="73"/>
     </row>
-    <row r="65" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="87" t="s">
         <v>237</v>
       </c>
@@ -8609,8 +8609,8 @@
       </c>
       <c r="G65" s="70"/>
       <c r="H65" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#determining-whether-the-app-is-debuggable-mstg-code-2"),"Determining Whether the App is Debuggable (MSTG-CODE-2)")</f>
-        <v>Determining Whether the App is Debuggable (MSTG-CODE-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#determining-whether-the-app-is-debuggable-mstg-code-2"),"Проверка включенного debug-режима (MSTG-CODE-2)")</f>
+        <v>Проверка включенного debug-режима (MSTG-CODE-2)</v>
       </c>
       <c r="I65" s="76"/>
       <c r="J65" s="76"/>
@@ -8634,14 +8634,14 @@
       </c>
       <c r="G66" s="70"/>
       <c r="H66" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-symbols-mstg-code-3"),"Finding Debugging Symbols (MSTG-CODE-3)")</f>
-        <v>Finding Debugging Symbols (MSTG-CODE-3)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-symbols-mstg-code-3"),"Проверка отладочных символов (MSTG-CODE-3)")</f>
+        <v>Проверка отладочных символов (MSTG-CODE-3)</v>
       </c>
       <c r="I66" s="76"/>
       <c r="J66" s="76"/>
       <c r="K66" s="73"/>
     </row>
-    <row r="67" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="87" t="s">
         <v>243</v>
       </c>
@@ -8659,8 +8659,8 @@
       </c>
       <c r="G67" s="70"/>
       <c r="H67" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-code-and-verbose-error-logging-mstg-code-4"),"Finding Debugging Code and Verbose Error Logging (MSTG-CODE-4)")</f>
-        <v>Finding Debugging Code and Verbose Error Logging (MSTG-CODE-4)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-code-and-verbose-error-logging-mstg-code-4"),"Проверка наличия отладочного кода и расширенного логгирования (MSTG-CODE-4)")</f>
+        <v>Проверка наличия отладочного кода и расширенного логгирования (MSTG-CODE-4)</v>
       </c>
       <c r="I67" s="76"/>
       <c r="J67" s="76"/>
@@ -8709,8 +8709,8 @@
       </c>
       <c r="G69" s="70"/>
       <c r="H69" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6"),"Testing Exception Handling (MSTG-CODE-6)")</f>
-        <v>Testing Exception Handling (MSTG-CODE-6)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6"),"Тестирование обработки исключений (MSTG-CODE-6)")</f>
+        <v>Тестирование обработки исключений (MSTG-CODE-6)</v>
       </c>
       <c r="I69" s="76"/>
       <c r="J69" s="76"/>
@@ -8734,8 +8734,8 @@
       </c>
       <c r="G70" s="70"/>
       <c r="H70" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6"),"Testing Exception Handling (MSTG-CODE-6)")</f>
-        <v>Testing Exception Handling (MSTG-CODE-6)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling-mstg-code-6"),"Тестирование обработки исключений (MSTG-CODE-6)")</f>
+        <v>Тестирование обработки исключений (MSTG-CODE-6)</v>
       </c>
       <c r="I70" s="76"/>
       <c r="J70" s="76"/>
@@ -8759,14 +8759,14 @@
       </c>
       <c r="G71" s="70"/>
       <c r="H71" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#memory-corruption-bugs-mstg-code-8"),"Memory Corruption Bugs (MSTG-CODE-8)")</f>
-        <v>Memory Corruption Bugs (MSTG-CODE-8)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#memory-corruption-bugs-mstg-code-8"),"Ошибки памяти (MSTG-CODE-8)")</f>
+        <v>Ошибки памяти (MSTG-CODE-8)</v>
       </c>
       <c r="I71" s="76"/>
       <c r="J71" s="76"/>
       <c r="K71" s="73"/>
     </row>
-    <row r="72" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="87" t="s">
         <v>258</v>
       </c>
@@ -8784,8 +8784,8 @@
       </c>
       <c r="G72" s="70"/>
       <c r="H72" s="90" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#make-sure-that-free-security-features-are-activated-mstg-code-9"),"Make Sure That Free Security Features Are Activated (MSTG-CODE-9)")</f>
-        <v>Make Sure That Free Security Features Are Activated (MSTG-CODE-9)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06i-Testing-Code-Quality-and-Build-Settings.md#make-sure-that-free-security-features-are-activated-mstg-code-9"),"Убедитесь, что активированы все стандартные функции безопасности (MSTG-CODE-9)")</f>
+        <v>Убедитесь, что активированы все стандартные функции безопасности (MSTG-CODE-9)</v>
       </c>
       <c r="I72" s="76"/>
       <c r="J72" s="76"/>
@@ -9011,7 +9011,7 @@
   </sheetPr>
   <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -9558,7 +9558,7 @@
   </sheetPr>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
iOS Reverse Engineering translated
</commit_message>
<xml_diff>
--- a/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
+++ b/Mobile_App_Security_Checklist-Russian_1.1.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Информация" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="369">
   <si>
     <r>
       <rPr>
@@ -1001,28 +1001,22 @@
     <t xml:space="preserve">Требования к устойчивости к атакам на стороне клиента — iOS</t>
   </si>
   <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testing Procedure(s)</t>
+    <t xml:space="preserve">XLS Version History</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MASVS version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
   </si>
   <si>
     <t xml:space="preserve">Comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XLS Version History</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MASVS version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
   </si>
   <si>
     <t xml:space="preserve">Alexander Antukh (Opera Software)</t>
@@ -2532,7 +2526,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2762,7 +2756,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2942,11 +2936,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="97934166"/>
-        <c:axId val="19780430"/>
+        <c:axId val="90722575"/>
+        <c:axId val="64324269"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="97934166"/>
+        <c:axId val="90722575"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2986,7 +2980,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19780430"/>
+        <c:crossAx val="64324269"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2994,7 +2988,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19780430"/>
+        <c:axId val="64324269"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3037,7 +3031,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97934166"/>
+        <c:crossAx val="90722575"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3097,7 +3091,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3277,11 +3271,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="92657394"/>
-        <c:axId val="93328890"/>
+        <c:axId val="61990994"/>
+        <c:axId val="84320114"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="92657394"/>
+        <c:axId val="61990994"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3321,7 +3315,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93328890"/>
+        <c:crossAx val="84320114"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3329,7 +3323,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93328890"/>
+        <c:axId val="84320114"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3372,7 +3366,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92657394"/>
+        <c:crossAx val="61990994"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7043,7 +7037,7 @@
   </sheetPr>
   <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H73" activeCellId="0" sqref="H73"/>
     </sheetView>
   </sheetViews>
@@ -9011,8 +9005,8 @@
   </sheetPr>
   <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9057,13 +9051,13 @@
         <v>271</v>
       </c>
       <c r="F3" s="56" t="s">
-        <v>315</v>
+        <v>56</v>
       </c>
       <c r="G3" s="121" t="s">
-        <v>316</v>
+        <v>57</v>
       </c>
       <c r="H3" s="58" t="s">
-        <v>317</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9094,8 +9088,8 @@
         <v>77</v>
       </c>
       <c r="G5" s="124" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#jailbreak-detection-mstg-resilience-1"),"Jailbreak Detection (MSTG-RESILIENCE-1)")</f>
-        <v>Jailbreak Detection (MSTG-RESILIENCE-1)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#jailbreak-detection-mstg-resilience-1"),"Определение jailbreak (MSTG-RESILIENCE-1)")</f>
+        <v>Определение jailbreak (MSTG-RESILIENCE-1)</v>
       </c>
       <c r="H5" s="125"/>
     </row>
@@ -9116,8 +9110,8 @@
         <v>77</v>
       </c>
       <c r="G6" s="124" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#anti-debugging-checks-mstg-resilience-2"),"Anti-Debugging Checks (MSTG-RESILIENCE-2)")</f>
-        <v>Anti-Debugging Checks (MSTG-RESILIENCE-2)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#anti-debugging-checks-mstg-resilience-2"),"Проверка определения отладчиков (MSTG-RESILIENCE-2)")</f>
+        <v>Проверка определения отладчиков (MSTG-RESILIENCE-2)</v>
       </c>
       <c r="H6" s="125"/>
     </row>
@@ -9138,8 +9132,8 @@
         <v>77</v>
       </c>
       <c r="G7" s="124" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks-mstg-resilience-3-and-mstg-resilience-11"),"File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)")</f>
-        <v>File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks-mstg-resilience-3-and-mstg-resilience-11"),"Проверка целостности файлов (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)")</f>
+        <v>Проверка целостности файлов (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)</v>
       </c>
       <c r="H7" s="125"/>
     </row>
@@ -9297,8 +9291,8 @@
         <v>77</v>
       </c>
       <c r="G15" s="124" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#device-binding-mstg-resilience-10"),"Device Binding (MSTG-RESILIENCE-10)")</f>
-        <v>Device Binding (MSTG-RESILIENCE-10)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#device-binding-mstg-resilience-10"),"Тестирование привязки к устройству (MSTG-RESILIENCE-10)")</f>
+        <v>Тестирование привязки к устройству (MSTG-RESILIENCE-10)</v>
       </c>
       <c r="H15" s="125"/>
     </row>
@@ -9313,7 +9307,7 @@
       <c r="G16" s="122"/>
       <c r="H16" s="86"/>
     </row>
-    <row r="17" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="45.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="65" t="s">
         <v>307</v>
       </c>
@@ -9330,12 +9324,12 @@
         <v>77</v>
       </c>
       <c r="G17" s="152" t="str">
-        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks-mstg-resilience-3-and-mstg-resilience-11"),"File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)")</f>
-        <v>File Integrity Checks (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)</v>
+        <f aca="false">HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks-mstg-resilience-3-and-mstg-resilience-11"),"Проверка целостности файлов (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)")</f>
+        <v>Проверка целостности файлов (MSTG-RESILIENCE-3 and MSTG-RESILIENCE-11)</v>
       </c>
       <c r="H17" s="125"/>
     </row>
-    <row r="18" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="67.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="65" t="s">
         <v>310</v>
       </c>
@@ -9571,7 +9565,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="153" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B1" s="153"/>
       <c r="C1" s="154"/>
@@ -9580,24 +9574,24 @@
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="155" t="s">
+        <v>316</v>
+      </c>
+      <c r="B2" s="155" t="s">
+        <v>317</v>
+      </c>
+      <c r="C2" s="155" t="s">
+        <v>318</v>
+      </c>
+      <c r="D2" s="155" t="s">
         <v>319</v>
       </c>
-      <c r="B2" s="155" t="s">
+      <c r="E2" s="155" t="s">
         <v>320</v>
-      </c>
-      <c r="C2" s="155" t="s">
-        <v>321</v>
-      </c>
-      <c r="D2" s="155" t="s">
-        <v>322</v>
-      </c>
-      <c r="E2" s="155" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="156" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B3" s="157" t="n">
         <v>0.1</v>
@@ -9607,12 +9601,12 @@
         <v>42765</v>
       </c>
       <c r="E3" s="159" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="159" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B4" s="157" t="n">
         <v>0.2</v>
@@ -9622,12 +9616,12 @@
         <v>42766</v>
       </c>
       <c r="E4" s="159" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="159" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B5" s="157" t="n">
         <v>0.3</v>
@@ -9637,102 +9631,102 @@
         <v>42778</v>
       </c>
       <c r="E5" s="159" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="159" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B6" s="157" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C6" s="157"/>
       <c r="D6" s="158" t="n">
         <v>42780</v>
       </c>
       <c r="E6" s="159" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="159" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B7" s="160" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C7" s="160"/>
       <c r="D7" s="158" t="n">
         <v>42781</v>
       </c>
       <c r="E7" s="159" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="159" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B8" s="160" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C8" s="160"/>
       <c r="D8" s="158" t="n">
         <v>42829</v>
       </c>
       <c r="E8" s="159" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="159" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B9" s="160" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C9" s="160"/>
       <c r="D9" s="158" t="n">
         <v>42919</v>
       </c>
       <c r="E9" s="159" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="159" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B10" s="160" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C10" s="160"/>
       <c r="D10" s="158" t="n">
         <v>42963</v>
       </c>
       <c r="E10" s="159" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="159" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B11" s="160" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C11" s="160"/>
       <c r="D11" s="158" t="n">
         <v>43113</v>
       </c>
       <c r="E11" s="159" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="159" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B12" s="160" t="n">
         <v>1.1</v>
@@ -9742,130 +9736,130 @@
         <v>43289</v>
       </c>
       <c r="E12" s="159" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="159" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B13" s="161" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C13" s="162"/>
       <c r="D13" s="158" t="n">
         <v>43464</v>
       </c>
       <c r="E13" s="163" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="159" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B14" s="161" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C14" s="162"/>
       <c r="D14" s="158" t="n">
         <v>43469</v>
       </c>
       <c r="E14" s="163" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="409.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="164" t="s">
+        <v>345</v>
+      </c>
+      <c r="B15" s="160" t="s">
+        <v>346</v>
+      </c>
+      <c r="C15" s="160" t="s">
         <v>347</v>
-      </c>
-      <c r="B15" s="160" t="s">
-        <v>348</v>
-      </c>
-      <c r="C15" s="160" t="s">
-        <v>349</v>
       </c>
       <c r="D15" s="158" t="n">
         <v>43471</v>
       </c>
       <c r="E15" s="165" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="159" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B16" s="161" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C16" s="160" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D16" s="166" t="n">
         <v>43475</v>
       </c>
       <c r="E16" s="163" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="78" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="164" t="s">
+        <v>345</v>
+      </c>
+      <c r="B17" s="161" t="s">
+        <v>351</v>
+      </c>
+      <c r="C17" s="160" t="s">
         <v>347</v>
-      </c>
-      <c r="B17" s="161" t="s">
-        <v>353</v>
-      </c>
-      <c r="C17" s="160" t="s">
-        <v>349</v>
       </c>
       <c r="D17" s="158" t="n">
         <v>43476</v>
       </c>
       <c r="E17" s="164" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="164" t="s">
+        <v>345</v>
+      </c>
+      <c r="B18" s="161" t="s">
+        <v>353</v>
+      </c>
+      <c r="C18" s="160" t="s">
         <v>347</v>
-      </c>
-      <c r="B18" s="161" t="s">
-        <v>355</v>
-      </c>
-      <c r="C18" s="160" t="s">
-        <v>349</v>
       </c>
       <c r="D18" s="158" t="n">
         <v>43478</v>
       </c>
       <c r="E18" s="164" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="164" t="s">
+        <v>345</v>
+      </c>
+      <c r="B19" s="161" t="s">
+        <v>355</v>
+      </c>
+      <c r="C19" s="160" t="s">
         <v>347</v>
-      </c>
-      <c r="B19" s="161" t="s">
-        <v>357</v>
-      </c>
-      <c r="C19" s="160" t="s">
-        <v>349</v>
       </c>
       <c r="D19" s="158" t="n">
         <v>43478</v>
       </c>
       <c r="E19" s="164" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="109.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="164" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B20" s="161" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C20" s="160" t="s">
         <v>3</v>
@@ -9874,15 +9868,15 @@
         <v>43641</v>
       </c>
       <c r="E20" s="165" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="164" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B21" s="161" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C21" s="160" t="s">
         <v>3</v>
@@ -9891,15 +9885,15 @@
         <v>43642</v>
       </c>
       <c r="E21" s="164" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="164" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B22" s="161" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C22" s="160" t="s">
         <v>3</v>
@@ -9908,15 +9902,15 @@
         <v>43649</v>
       </c>
       <c r="E22" s="164" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="164" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B23" s="161" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C23" s="160" t="s">
         <v>3</v>
@@ -9925,15 +9919,15 @@
         <v>43672</v>
       </c>
       <c r="E23" s="164" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="164" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B24" s="161" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C24" s="160" t="s">
         <v>3</v>
@@ -9942,15 +9936,15 @@
         <v>43674</v>
       </c>
       <c r="E24" s="164" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="164" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B25" s="161" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C25" s="160" t="s">
         <v>3</v>
@@ -9959,15 +9953,15 @@
         <v>43685</v>
       </c>
       <c r="E25" s="164" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="164" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B26" s="161" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C26" s="160" t="s">
         <v>3</v>
@@ -9976,7 +9970,7 @@
         <v>43719</v>
       </c>
       <c r="E26" s="164" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>